<commit_message>
Se modifica el resultado del partido IRN - ESP
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -13679,9 +13679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1490760</xdr:colOff>
+      <xdr:colOff>1490400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13695,7 +13695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1232280"/>
-          <a:ext cx="229680" cy="152280"/>
+          <a:ext cx="229320" cy="151920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13716,9 +13716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1490760</xdr:colOff>
+      <xdr:colOff>1490400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13732,7 +13732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4275360"/>
-          <a:ext cx="229680" cy="152280"/>
+          <a:ext cx="229320" cy="151920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13753,9 +13753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13769,7 +13769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7323480"/>
-          <a:ext cx="229680" cy="152280"/>
+          <a:ext cx="229320" cy="151920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13790,9 +13790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13806,7 +13806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="1232280"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13827,9 +13827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13843,7 +13843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4470840"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13864,9 +13864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13880,7 +13880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7518600"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13901,9 +13901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13917,7 +13917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1422720"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13938,9 +13938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>254160</xdr:colOff>
+      <xdr:colOff>253800</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13954,7 +13954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5460840" y="4280040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13975,9 +13975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13991,7 +13991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7518600"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14012,9 +14012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>185400</xdr:rowOff>
+      <xdr:rowOff>185040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14028,7 +14028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1431720"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14049,9 +14049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14065,7 +14065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4484520"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14086,9 +14086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>181080</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14102,7 +14102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7332840"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14123,9 +14123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14139,7 +14139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1613160"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14160,9 +14160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14176,7 +14176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4661280"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14197,9 +14197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14213,7 +14213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7709040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14234,9 +14234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14250,7 +14250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1613160"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14271,9 +14271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>181080</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14287,7 +14287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4856400"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14308,9 +14308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483200</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14324,7 +14324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="7899840"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14345,9 +14345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>181080</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14361,7 +14361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="7904520"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14382,9 +14382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14398,7 +14398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4661280"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14419,9 +14419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14435,7 +14435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1798920"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14456,9 +14456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14472,7 +14472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1803600"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14493,9 +14493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14509,7 +14509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4847040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14530,9 +14530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14546,7 +14546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7704360"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14567,9 +14567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14583,7 +14583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1994040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14604,9 +14604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14620,7 +14620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5042160"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14641,9 +14641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14657,7 +14657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="8090280"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14678,9 +14678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14694,7 +14694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1994040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14715,9 +14715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14731,7 +14731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5227920"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14752,9 +14752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483200</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14768,7 +14768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8276040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14789,9 +14789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14805,7 +14805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2184840"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14826,9 +14826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14842,7 +14842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="5042160"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14863,9 +14863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14879,7 +14879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="8276040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14900,9 +14900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14916,7 +14916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2180160"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14937,9 +14937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14953,7 +14953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5227920"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14974,9 +14974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483200</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14990,7 +14990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8085600"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15011,9 +15011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15027,7 +15027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2370600"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15048,9 +15048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15064,7 +15064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5423040"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15085,9 +15085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15101,7 +15101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="8466480"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15122,9 +15122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15138,7 +15138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="2375280"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15159,9 +15159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483200</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15175,7 +15175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8661600"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15196,9 +15196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15212,7 +15212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5613840"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15233,9 +15233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487880</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15249,7 +15249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2565720"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15270,9 +15270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15286,7 +15286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5450760" y="5417640"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15307,9 +15307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15323,7 +15323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455080" y="8656200"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15344,9 +15344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15360,7 +15360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5450760" y="2564640"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15381,9 +15381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1486440</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15397,7 +15397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3925440" y="5612760"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15418,9 +15418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15434,7 +15434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921120" y="8465760"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15455,9 +15455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15471,7 +15471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="2757240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15492,9 +15492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15508,7 +15508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="5800680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15529,9 +15529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15545,7 +15545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="8848440"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15566,9 +15566,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>201240</xdr:colOff>
+      <xdr:colOff>200880</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15582,7 +15582,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481000" y="2752560"/>
-          <a:ext cx="153720" cy="153720"/>
+          <a:ext cx="153360" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15603,9 +15603,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>196560</xdr:colOff>
+      <xdr:colOff>196200</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15619,7 +15619,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5476320" y="5991120"/>
-          <a:ext cx="153720" cy="153720"/>
+          <a:ext cx="153360" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15640,9 +15640,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1444320</xdr:colOff>
+      <xdr:colOff>1443960</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15656,7 +15656,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956040" y="9039240"/>
-          <a:ext cx="153720" cy="153720"/>
+          <a:ext cx="153360" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15677,9 +15677,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15693,7 +15693,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="2943000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15714,9 +15714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15730,7 +15730,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="5800680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15751,9 +15751,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15767,7 +15767,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9039240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15788,9 +15788,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15804,7 +15804,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="2943000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15825,9 +15825,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15841,7 +15841,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="5991120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15862,9 +15862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15878,7 +15878,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="8848440"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15899,9 +15899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15915,7 +15915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3133440"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15936,9 +15936,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15952,7 +15952,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="6181560"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15973,9 +15973,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15989,7 +15989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9229680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16010,9 +16010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16026,7 +16026,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3138120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16047,9 +16047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16063,7 +16063,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6372000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16084,9 +16084,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16100,7 +16100,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="9420120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16121,9 +16121,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16137,7 +16137,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3324240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16158,9 +16158,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16174,7 +16174,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6181560"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16195,9 +16195,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16211,7 +16211,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9420120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16232,9 +16232,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16248,7 +16248,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3324240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16269,9 +16269,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16285,7 +16285,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="6372000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16306,9 +16306,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16322,7 +16322,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9229680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16343,9 +16343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1467000</xdr:colOff>
+      <xdr:colOff>1466640</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16359,7 +16359,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3951360" y="3514680"/>
-          <a:ext cx="181080" cy="153720"/>
+          <a:ext cx="180720" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16380,9 +16380,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1467000</xdr:colOff>
+      <xdr:colOff>1466640</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16396,7 +16396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3951360" y="6562440"/>
-          <a:ext cx="181080" cy="153720"/>
+          <a:ext cx="180720" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16417,9 +16417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>219240</xdr:colOff>
+      <xdr:colOff>218880</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16433,7 +16433,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5471640" y="9610560"/>
-          <a:ext cx="181080" cy="153720"/>
+          <a:ext cx="180720" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16454,9 +16454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16470,7 +16470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3514680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16491,9 +16491,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>250200</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16507,7 +16507,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="6753240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16528,9 +16528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16544,7 +16544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9801000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16565,9 +16565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16581,7 +16581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3705120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16602,9 +16602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16618,7 +16618,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6562440"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16639,9 +16639,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16655,7 +16655,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9801000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16676,9 +16676,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16692,7 +16692,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3895560"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16713,9 +16713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16729,7 +16729,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="6943680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16750,9 +16750,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16766,7 +16766,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9991440"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16787,9 +16787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>250200</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16803,7 +16803,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="3900240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16824,9 +16824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>250200</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16840,7 +16840,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="7134120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16861,9 +16861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16877,7 +16877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="10182240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16898,9 +16898,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16914,7 +16914,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="4090680"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16935,9 +16935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>250200</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16951,7 +16951,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="6948360"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16972,9 +16972,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16988,7 +16988,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="10182240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17009,9 +17009,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17025,7 +17025,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="4086000"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17046,9 +17046,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17062,7 +17062,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="7134120"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17083,9 +17083,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17099,7 +17099,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="9991440"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17120,9 +17120,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>250200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17136,7 +17136,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="3709800"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17157,9 +17157,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488960</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17173,7 +17173,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="6753240"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17194,9 +17194,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17210,7 +17210,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9610560"/>
-          <a:ext cx="226800" cy="153720"/>
+          <a:ext cx="226440" cy="153360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31389,8 +31389,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32014,15 +32014,15 @@
       </c>
       <c r="U9" s="42" t="n">
         <f aca="false">IF(S9="",0,IF(VLOOKUP(E9,$AB$8:$AK$53,7,0)=VLOOKUP(H9,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="40" t="n">
         <f aca="false">U9*F9</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W9" s="40" t="n">
         <f aca="false">U9*G9</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X9" s="40" t="n">
         <f aca="false">IF(OR(E9=my_team,H9=my_team),1,0)</f>
@@ -32943,7 +32943,7 @@
       </c>
       <c r="AL14" s="40" t="n">
         <f aca="false">AP14/AP18*1000+AQ14/AQ18*100+AT14/AT18*10+AR14/AR18</f>
-        <v>0</v>
+        <v>50.75</v>
       </c>
       <c r="AM14" s="40" t="n">
         <f aca="false">VLOOKUP(AB14,db_fifarank,2,0)/2000000</f>
@@ -32951,7 +32951,7 @@
       </c>
       <c r="AN14" s="42" t="n">
         <f aca="false">1000*AK14/AK18+100*AJ14+10*AF14/AF18+1*AL14/AL18+AM14</f>
-        <v>883.000679</v>
+        <v>883.981355328502</v>
       </c>
       <c r="AO14" s="43" t="str">
         <f aca="false">IF(SUM(AC14:AE17)=12,J15,INDEX(T,72,lang))</f>
@@ -32963,15 +32963,15 @@
       </c>
       <c r="AQ14" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB14&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB14&amp;"_draw")*($U$7:$U$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR14" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB14)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB14)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS14" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB14)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB14)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT14" s="44" t="n">
         <f aca="false">AR14-AS14</f>
@@ -33097,7 +33097,7 @@
       </c>
       <c r="AA15" s="40" t="n">
         <f aca="false">COUNTIF(AN14:AN17,CONCATENATE("&gt;=",AN15))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB15" s="42" t="str">
         <f aca="false">VLOOKUP("Spain",T,lang,0)</f>
@@ -33105,11 +33105,11 @@
       </c>
       <c r="AC15" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB15 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB15 &amp; "_draw")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE15" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB15 &amp; "_lose")</f>
@@ -33117,7 +33117,7 @@
       </c>
       <c r="AF15" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB15,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB15,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG15" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB15,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB15,$F$7:$F$54)</f>
@@ -33125,23 +33125,23 @@
       </c>
       <c r="AH15" s="40" t="n">
         <f aca="false">(AF15-AG15)*100+AK15*10000+AF15</f>
-        <v>20003</v>
+        <v>40104</v>
       </c>
       <c r="AI15" s="40" t="n">
         <f aca="false">AF15-AG15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="40" t="n">
         <f aca="false">(AI15-AI19)/AI18</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AK15" s="40" t="n">
         <f aca="false">AC15*3+AD15</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL15" s="40" t="n">
         <f aca="false">AP15/AP18*1000+AQ15/AQ18*100+AT15/AT18*10+AR15/AR18</f>
-        <v>0</v>
+        <v>50.75</v>
       </c>
       <c r="AM15" s="40" t="n">
         <f aca="false">VLOOKUP(AB15,db_fifarank,2,0)/2000000</f>
@@ -33149,7 +33149,7 @@
       </c>
       <c r="AN15" s="42" t="n">
         <f aca="false">1000*AK15/AK18+100*AJ15+10*AF15/AF18+1*AL15/AL18+AM15</f>
-        <v>456.0006155</v>
+        <v>883.981291828503</v>
       </c>
       <c r="AO15" s="43" t="str">
         <f aca="false">IF(SUM(AC14:AE17)=12,J16,INDEX(T,73,lang))</f>
@@ -33161,15 +33161,15 @@
       </c>
       <c r="AQ15" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB15&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB15&amp;"_draw")*($U$7:$U$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR15" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB15)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB15)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS15" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB15)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB15)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT15" s="44" t="n">
         <f aca="false">AR15-AS15</f>
@@ -33236,7 +33236,7 @@
       </c>
       <c r="J16" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA14:AK17,2,0)</f>
-        <v>Irán</v>
+        <v>España</v>
       </c>
       <c r="K16" s="76" t="n">
         <f aca="false">L16+M16+N16</f>
@@ -33256,7 +33256,7 @@
       </c>
       <c r="O16" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA14:AK17,6,0) &amp; " - " &amp; VLOOKUP(2,AA14:AK17,7,0)</f>
-        <v>1 - 0</v>
+        <v>4 - 3</v>
       </c>
       <c r="P16" s="77" t="n">
         <f aca="false">L16*3+M16</f>
@@ -33430,7 +33430,7 @@
       </c>
       <c r="J17" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA14:AK17,2,0)</f>
-        <v>España</v>
+        <v>Irán</v>
       </c>
       <c r="K17" s="76" t="n">
         <f aca="false">L17+M17+N17</f>
@@ -33438,23 +33438,23 @@
       </c>
       <c r="L17" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA14:AK17,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA14:AK17,4,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA14:AK17,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA14:AK17,6,0) &amp; " - " &amp; VLOOKUP(3,AA14:AK17,7,0)</f>
-        <v>3 - 3</v>
+        <v>1 - 1</v>
       </c>
       <c r="P17" s="77" t="n">
         <f aca="false">L17*3+M17</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R17" s="40" t="n">
         <f aca="false">DATE(2018,6,17)+TIME(4,0,0)+gmt_delta</f>
@@ -33490,7 +33490,7 @@
       </c>
       <c r="AA17" s="40" t="n">
         <f aca="false">COUNTIF(AN14:AN17,CONCATENATE("&gt;=",AN17))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB17" s="42" t="str">
         <f aca="false">VLOOKUP("Iran",T,lang,0)</f>
@@ -33502,11 +33502,11 @@
       </c>
       <c r="AD17" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB17 &amp; "_draw")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB17 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF17" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB17,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB17,$G$7:$G$54)</f>
@@ -33514,23 +33514,23 @@
       </c>
       <c r="AG17" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB17,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB17,$F$7:$F$54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH17" s="40" t="n">
         <f aca="false">(AF17-AG17)*100+AK17*10000+AF17</f>
-        <v>40101</v>
+        <v>30001</v>
       </c>
       <c r="AI17" s="40" t="n">
         <f aca="false">AF17-AG17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="40" t="n">
         <f aca="false">(AI17-AI19)/AI18</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AK17" s="40" t="n">
         <f aca="false">AC17*3+AD17</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL17" s="40" t="n">
         <f aca="false">AP17/AP18*1000+AQ17/AQ18*100+AT17/AT18*10+AR17/AR18</f>
@@ -33542,7 +33542,7 @@
       </c>
       <c r="AN17" s="42" t="n">
         <f aca="false">1000*AK17/AK18+100*AJ17+10*AF17/AF18+1*AL17/AL18+AM17</f>
-        <v>877.000399</v>
+        <v>652.000399</v>
       </c>
       <c r="AP17" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB17&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB17&amp;"_win")*($U$7:$U$54))</f>
@@ -33689,7 +33689,7 @@
       </c>
       <c r="AD18" s="40" t="n">
         <f aca="false">MAX(AD14:AD17)-MIN(AD14:AD17)+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE18" s="40" t="n">
         <f aca="false">MAX(AE14:AE17)-MIN(AE14:AE17)+1</f>
@@ -33701,7 +33701,7 @@
       </c>
       <c r="AG18" s="40" t="n">
         <f aca="false">MAX(AG14:AG17)-MIN(AG14:AG17)+1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH18" s="40" t="n">
         <f aca="false">MAX(AH14:AH17)-AH19+1</f>
@@ -33717,7 +33717,7 @@
       </c>
       <c r="AL18" s="40" t="n">
         <f aca="false">MAX(AL14:AL17)-MIN(AL14:AL17)+1</f>
-        <v>1</v>
+        <v>51.75</v>
       </c>
       <c r="AP18" s="40" t="n">
         <f aca="false">MAX(AP14:AP17)-MIN(AP14:AP17)+1</f>
@@ -33725,15 +33725,15 @@
       </c>
       <c r="AQ18" s="40" t="n">
         <f aca="false">MAX(AQ14:AQ17)-MIN(AQ14:AQ17)+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR18" s="40" t="n">
         <f aca="false">MAX(AR14:AR17)-MIN(AR14:AR17)+1</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AS18" s="40" t="n">
         <f aca="false">MAX(AS14:AS17)-MIN(AS14:AS17)+1</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AT18" s="40" t="n">
         <f aca="false">MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
@@ -34962,7 +34962,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="66" t="str">
         <f aca="false">AB15</f>
@@ -35002,11 +35002,11 @@
       </c>
       <c r="S26" s="41" t="str">
         <f aca="false">IF(OR(F26="",G26=""),"",IF(F26&gt;G26,E26&amp;"_win",IF(F26&lt;G26,E26&amp;"_lose",E26&amp;"_draw")))</f>
-        <v>Irán_draw</v>
+        <v>Irán_lose</v>
       </c>
       <c r="T26" s="41" t="str">
         <f aca="false">IF(S26="","",IF(F26&lt;G26,H26&amp;"_win",IF(F26&gt;G26,H26&amp;"_lose",H26&amp;"_draw")))</f>
-        <v>España_draw</v>
+        <v>España_win</v>
       </c>
       <c r="U26" s="42" t="n">
         <f aca="false">IF(S26="",0,IF(VLOOKUP(E26,$AB$8:$AK$53,7,0)=VLOOKUP(H26,$AB$8:$AK$53,7,0),1,0))</f>
@@ -35026,7 +35026,7 @@
       </c>
       <c r="Y26" s="40" t="n">
         <f aca="false">IF(OR(F26="",G26=""),"",IF(F26&gt;G26,1,IF(F26&lt;G26,-1,0)))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA26" s="40" t="n">
         <f aca="false">COUNTIF(AN26:AN29,CONCATENATE("&gt;=",AN26))</f>
@@ -40158,7 +40158,7 @@
       <formula>IF($AZ26=$T60,1,0)</formula>
     </cfRule>
     <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>IF($AZ27=$T60,1,0)</formula>
+      <formula>IF($AZ27=$T60,а,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ27">

</xml_diff>

<commit_message>
Se actualizan resultados hasta el dia 22 de junio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -11535,7 +11535,7 @@
     <numFmt numFmtId="165" formatCode=";;;"/>
     <numFmt numFmtId="166" formatCode="H:MM;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -11658,6 +11658,13 @@
     </font>
     <font>
       <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -12469,7 +12476,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -12866,19 +12873,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="true"/>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -13679,9 +13690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1490400</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13695,7 +13706,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1232280"/>
-          <a:ext cx="229320" cy="151920"/>
+          <a:ext cx="227520" cy="150120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13716,9 +13727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1490400</xdr:colOff>
+      <xdr:colOff>1488600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13732,7 +13743,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4275360"/>
-          <a:ext cx="229320" cy="151920"/>
+          <a:ext cx="227520" cy="150120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13753,9 +13764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>252000</xdr:colOff>
+      <xdr:colOff>250200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13769,7 +13780,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7323480"/>
-          <a:ext cx="229320" cy="151920"/>
+          <a:ext cx="227520" cy="150120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13790,9 +13801,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13806,7 +13817,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="1232280"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13827,9 +13838,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13843,7 +13854,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4470840"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13864,9 +13875,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13880,7 +13891,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7518600"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13901,9 +13912,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13917,7 +13928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1422720"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13938,9 +13949,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>253800</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13954,7 +13965,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5460840" y="4280040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13975,9 +13986,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13991,7 +14002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7518600"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14012,9 +14023,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>185040</xdr:rowOff>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14028,7 +14039,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1431720"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14049,9 +14060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14065,7 +14076,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4484520"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14086,9 +14097,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14102,7 +14113,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7332840"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14123,9 +14134,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14139,7 +14150,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1613160"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14160,9 +14171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14176,7 +14187,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4661280"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14197,9 +14208,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14213,7 +14224,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7709040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14234,9 +14245,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14250,7 +14261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1613160"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14271,9 +14282,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14287,7 +14298,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4856400"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14308,9 +14319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14324,7 +14335,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="7899840"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14345,9 +14356,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14361,7 +14372,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="7904520"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14382,9 +14393,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14398,7 +14409,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4661280"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14419,9 +14430,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14435,7 +14446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1798920"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14456,9 +14467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14472,7 +14483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1803600"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14493,9 +14504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14509,7 +14520,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4847040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14530,9 +14541,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14546,7 +14557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7704360"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14567,9 +14578,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14583,7 +14594,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1994040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14604,9 +14615,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14620,7 +14631,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5042160"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14641,9 +14652,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14657,7 +14668,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="8090280"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14678,9 +14689,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14694,7 +14705,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1994040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14715,9 +14726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14731,7 +14742,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5227920"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14752,9 +14763,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14768,7 +14779,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8276040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14789,9 +14800,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14805,7 +14816,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2184840"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14826,9 +14837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14842,7 +14853,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="5042160"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14863,9 +14874,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14879,7 +14890,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="8276040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14900,9 +14911,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14916,7 +14927,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2180160"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14937,9 +14948,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14953,7 +14964,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5227920"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14974,9 +14985,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14990,7 +15001,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8085600"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15011,9 +15022,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15027,7 +15038,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2370600"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15048,9 +15059,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15064,7 +15075,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5423040"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15085,9 +15096,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15101,7 +15112,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="8466480"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15122,9 +15133,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15138,7 +15149,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="2375280"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15159,9 +15170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15175,7 +15186,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8661600"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15196,9 +15207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15212,7 +15223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5613840"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15233,9 +15244,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487520</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15249,7 +15260,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2565720"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15270,9 +15281,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15286,7 +15297,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5450760" y="5417640"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15307,9 +15318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15323,7 +15334,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455080" y="8656200"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15344,9 +15355,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15360,7 +15371,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5450760" y="2564640"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15381,9 +15392,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486440</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15397,7 +15408,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3925440" y="5612760"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15418,9 +15429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15434,7 +15445,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921120" y="8465760"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15455,9 +15466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15471,7 +15482,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="2757240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15492,9 +15503,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15508,7 +15519,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="5800680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15529,9 +15540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15545,7 +15556,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="8848440"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15566,9 +15577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>200880</xdr:colOff>
+      <xdr:colOff>199080</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15582,7 +15593,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481000" y="2752560"/>
-          <a:ext cx="153360" cy="153360"/>
+          <a:ext cx="151560" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15603,9 +15614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>196200</xdr:colOff>
+      <xdr:colOff>194400</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15619,7 +15630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5476320" y="5991120"/>
-          <a:ext cx="153360" cy="153360"/>
+          <a:ext cx="151560" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15640,9 +15651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1443960</xdr:colOff>
+      <xdr:colOff>1442160</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15656,7 +15667,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956040" y="9039240"/>
-          <a:ext cx="153360" cy="153360"/>
+          <a:ext cx="151560" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15677,9 +15688,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15693,7 +15704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="2943000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15714,9 +15725,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15730,7 +15741,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="5800680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15751,9 +15762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15767,7 +15778,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9039240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15788,9 +15799,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15804,7 +15815,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="2943000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15825,9 +15836,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15841,7 +15852,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="5991120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15862,9 +15873,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15878,7 +15889,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="8848440"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15899,9 +15910,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15915,7 +15926,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3133440"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15936,9 +15947,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15952,7 +15963,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="6181560"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15973,9 +15984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15989,7 +16000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9229680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16010,9 +16021,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16026,7 +16037,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3138120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16047,9 +16058,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16063,7 +16074,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6372000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16084,9 +16095,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16100,7 +16111,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="9420120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16121,9 +16132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16137,7 +16148,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3324240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16158,9 +16169,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16174,7 +16185,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6181560"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16195,9 +16206,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16211,7 +16222,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9420120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16232,9 +16243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16248,7 +16259,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3324240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16269,9 +16280,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16285,7 +16296,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="6372000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16306,9 +16317,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16322,7 +16333,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9229680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16343,9 +16354,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1466640</xdr:colOff>
+      <xdr:colOff>1464840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16359,7 +16370,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3951360" y="3514680"/>
-          <a:ext cx="180720" cy="153360"/>
+          <a:ext cx="178920" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16380,9 +16391,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1466640</xdr:colOff>
+      <xdr:colOff>1464840</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16396,7 +16407,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3951360" y="6562440"/>
-          <a:ext cx="180720" cy="153360"/>
+          <a:ext cx="178920" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16417,9 +16428,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>218880</xdr:colOff>
+      <xdr:colOff>217080</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16433,7 +16444,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5471640" y="9610560"/>
-          <a:ext cx="180720" cy="153360"/>
+          <a:ext cx="178920" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16454,9 +16465,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16470,7 +16481,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3514680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16491,9 +16502,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250200</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16507,7 +16518,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="6753240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16528,9 +16539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16544,7 +16555,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9801000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16565,9 +16576,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16581,7 +16592,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3705120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16602,9 +16613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16618,7 +16629,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6562440"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16639,9 +16650,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16655,7 +16666,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9801000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16676,9 +16687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16692,7 +16703,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3895560"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16713,9 +16724,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16729,7 +16740,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="6943680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16750,9 +16761,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16766,7 +16777,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9991440"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16787,9 +16798,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250200</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16803,7 +16814,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="3900240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16824,9 +16835,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250200</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16840,7 +16851,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="7134120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16861,9 +16872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16877,7 +16888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="10182240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16898,9 +16909,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16914,7 +16925,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="4090680"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16935,9 +16946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250200</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16951,7 +16962,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="6948360"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16972,9 +16983,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16988,7 +16999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="10182240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17009,9 +17020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17025,7 +17036,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="4086000"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17046,9 +17057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17062,7 +17073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="7134120"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17083,9 +17094,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17099,7 +17110,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="9991440"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17120,9 +17131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250200</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17136,7 +17147,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="3709800"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17157,9 +17168,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1486800</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17173,7 +17184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="6753240"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17194,9 +17205,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1482120</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17210,7 +17221,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9610560"/>
-          <a:ext cx="226440" cy="153360"/>
+          <a:ext cx="224640" cy="151560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31389,8 +31400,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32752,15 +32763,15 @@
       </c>
       <c r="U13" s="42" t="n">
         <f aca="false">IF(S13="",0,IF(VLOOKUP(E13,$AB$8:$AK$53,7,0)=VLOOKUP(H13,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="40" t="n">
         <f aca="false">U13*F13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13" s="40" t="n">
         <f aca="false">U13*G13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13" s="40" t="n">
         <f aca="false">IF(OR(E13=my_team,H13=my_team),1,0)</f>
@@ -33077,15 +33088,15 @@
       </c>
       <c r="U15" s="42" t="n">
         <f aca="false">IF(S15="",0,IF(VLOOKUP(E15,$AB$8:$AK$53,7,0)=VLOOKUP(H15,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="40" t="n">
         <f aca="false">U15*F15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15" s="40" t="n">
         <f aca="false">U15*G15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15" s="40" t="n">
         <f aca="false">IF(OR(E15=my_team,H15=my_team),1,0)</f>
@@ -33973,7 +33984,7 @@
       </c>
       <c r="AC20" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB20 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD20" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB20 &amp; "_draw")</f>
@@ -33985,7 +33996,7 @@
       </c>
       <c r="AF20" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB20,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB20,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG20" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB20,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB20,$F$7:$F$54)</f>
@@ -33993,19 +34004,19 @@
       </c>
       <c r="AH20" s="40" t="n">
         <f aca="false">(AF20-AG20)*100+AK20*10000+AF20</f>
-        <v>30102</v>
+        <v>60203</v>
       </c>
       <c r="AI20" s="40" t="n">
         <f aca="false">AF20-AG20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ20" s="40" t="n">
         <f aca="false">(AI20-AI25)/AI24</f>
-        <v>0.666666666666667</v>
+        <v>0.8</v>
       </c>
       <c r="AK20" s="40" t="n">
         <f aca="false">AC20*3+AD20</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL20" s="40" t="n">
         <f aca="false">AP20/AP24*1000+AQ20/AQ24*100+AT20/AT24*10+AR20/AR24</f>
@@ -34017,7 +34028,7 @@
       </c>
       <c r="AN20" s="42" t="n">
         <f aca="false">1000*AK20/AK24+100*AJ20+10*AF20/AF24+1*AL20/AL24+AM20</f>
-        <v>823.333924833333</v>
+        <v>944.643448642857</v>
       </c>
       <c r="AO20" s="43" t="str">
         <f aca="false">IF(SUM(AC20:AE23)=12,J21,INDEX(T,74,lang))</f>
@@ -34107,11 +34118,11 @@
       </c>
       <c r="K21" s="72" t="n">
         <f aca="false">L21+M21+N21</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA20:AK23,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA20:AK23,4,0)</f>
@@ -34123,11 +34134,11 @@
       </c>
       <c r="O21" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA20:AK23,6,0) &amp; " - " &amp; VLOOKUP(1,AA20:AK23,7,0)</f>
-        <v>2 - 1</v>
+        <v>3 - 1</v>
       </c>
       <c r="P21" s="73" t="n">
         <f aca="false">L21*3+M21</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R21" s="40" t="n">
         <f aca="false">DATE(2018,6,19)+TIME(4,0,0)+gmt_delta</f>
@@ -34175,7 +34186,7 @@
       </c>
       <c r="AD21" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB21 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB21 &amp; "_lose")</f>
@@ -34183,15 +34194,15 @@
       </c>
       <c r="AF21" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB21,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB21,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG21" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB21,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB21,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH21" s="40" t="n">
         <f aca="false">(AF21-AG21)*100+AK21*10000+AF21</f>
-        <v>-99</v>
+        <v>9902</v>
       </c>
       <c r="AI21" s="40" t="n">
         <f aca="false">AF21-AG21</f>
@@ -34199,11 +34210,11 @@
       </c>
       <c r="AJ21" s="40" t="n">
         <f aca="false">(AI21-AI25)/AI24</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AK21" s="40" t="n">
         <f aca="false">AC21*3+AD21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL21" s="40" t="n">
         <f aca="false">AP21/AP24*1000+AQ21/AQ24*100+AT21/AT24*10+AR21/AR24</f>
@@ -34215,7 +34226,7 @@
       </c>
       <c r="AN21" s="42" t="n">
         <f aca="false">1000*AK21/AK24+100*AJ21+10*AF21/AF24+1*AL21/AL24+AM21</f>
-        <v>3.33370683333333</v>
+        <v>167.857516357143</v>
       </c>
       <c r="AO21" s="43" t="str">
         <f aca="false">IF(SUM(AC20:AE23)=12,J22,INDEX(T,75,lang))</f>
@@ -34306,7 +34317,7 @@
       </c>
       <c r="K22" s="76" t="n">
         <f aca="false">L22+M22+N22</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA20:AK23,3,0)</f>
@@ -34314,7 +34325,7 @@
       </c>
       <c r="M22" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA20:AK23,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA20:AK23,5,0)</f>
@@ -34322,11 +34333,11 @@
       </c>
       <c r="O22" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA20:AK23,6,0) &amp; " - " &amp; VLOOKUP(2,AA20:AK23,7,0)</f>
-        <v>1 - 0</v>
+        <v>2 - 1</v>
       </c>
       <c r="P22" s="77" t="n">
         <f aca="false">L22*3+M22</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R22" s="40" t="n">
         <f aca="false">DATE(2018,6,19)+TIME(1,0,0)+gmt_delta</f>
@@ -34378,7 +34389,7 @@
       </c>
       <c r="AE22" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB22 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF22" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB22,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB22,$G$7:$G$54)</f>
@@ -34386,15 +34397,15 @@
       </c>
       <c r="AG22" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB22,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB22,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH22" s="40" t="n">
         <f aca="false">(AF22-AG22)*100+AK22*10000+AF22</f>
-        <v>-100</v>
+        <v>-200</v>
       </c>
       <c r="AI22" s="40" t="n">
         <f aca="false">AF22-AG22</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AJ22" s="40" t="n">
         <f aca="false">(AI22-AI25)/AI24</f>
@@ -34503,7 +34514,7 @@
       </c>
       <c r="K23" s="76" t="n">
         <f aca="false">L23+M23+N23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA20:AK23,3,0)</f>
@@ -34511,7 +34522,7 @@
       </c>
       <c r="M23" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA20:AK23,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA20:AK23,5,0)</f>
@@ -34519,11 +34530,11 @@
       </c>
       <c r="O23" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA20:AK23,6,0) &amp; " - " &amp; VLOOKUP(3,AA20:AK23,7,0)</f>
-        <v>1 - 2</v>
+        <v>2 - 3</v>
       </c>
       <c r="P23" s="77" t="n">
         <f aca="false">L23*3+M23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="40" t="n">
         <f aca="false">DATE(2018,6,19)+TIME(7,0,0)+gmt_delta</f>
@@ -34571,7 +34582,7 @@
       </c>
       <c r="AD23" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB23 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB23 &amp; "_lose")</f>
@@ -34579,15 +34590,15 @@
       </c>
       <c r="AF23" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB23,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB23,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG23" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB23,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB23,$F$7:$F$54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH23" s="40" t="n">
         <f aca="false">(AF23-AG23)*100+AK23*10000+AF23</f>
-        <v>30101</v>
+        <v>40102</v>
       </c>
       <c r="AI23" s="40" t="n">
         <f aca="false">AF23-AG23</f>
@@ -34595,11 +34606,11 @@
       </c>
       <c r="AJ23" s="40" t="n">
         <f aca="false">(AI23-AI25)/AI24</f>
-        <v>0.666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AK23" s="40" t="n">
         <f aca="false">AC23*3+AD23</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL23" s="40" t="n">
         <f aca="false">AP23/AP24*1000+AQ23/AQ24*100+AT23/AT24*10+AR23/AR24</f>
@@ -34611,7 +34622,7 @@
       </c>
       <c r="AN23" s="42" t="n">
         <f aca="false">1000*AK23/AK24+100*AJ23+10*AF23/AF24+1*AL23/AL24+AM23</f>
-        <v>820.0005495</v>
+        <v>636.429120928572</v>
       </c>
       <c r="AP23" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB23&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB23&amp;"_win")*($U$7:$U$54))</f>
@@ -34700,7 +34711,7 @@
       </c>
       <c r="K24" s="88" t="n">
         <f aca="false">L24+M24+N24</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA20:AK23,3,0)</f>
@@ -34712,11 +34723,11 @@
       </c>
       <c r="N24" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA20:AK23,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O24" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA20:AK23,6,0) &amp; " - " &amp; VLOOKUP(4,AA20:AK23,7,0)</f>
-        <v>0 - 1</v>
+        <v>0 - 2</v>
       </c>
       <c r="P24" s="89" t="n">
         <f aca="false">L24*3+M24</f>
@@ -34756,19 +34767,19 @@
       </c>
       <c r="AC24" s="40" t="n">
         <f aca="false">MAX(AC20:AC23)-MIN(AC20:AC23)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD24" s="40" t="n">
         <f aca="false">MAX(AD20:AD23)-MIN(AD20:AD23)+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE24" s="40" t="n">
         <f aca="false">MAX(AE20:AE23)-MIN(AE20:AE23)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF24" s="40" t="n">
         <f aca="false">MAX(AF20:AF23)-MIN(AF20:AF23)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG24" s="40" t="n">
         <f aca="false">MAX(AG20:AG23)-MIN(AG20:AG23)+1</f>
@@ -34776,15 +34787,15 @@
       </c>
       <c r="AH24" s="40" t="n">
         <f aca="false">MAX(AH20:AH23)-AH25+1</f>
-        <v>30203</v>
+        <v>60404</v>
       </c>
       <c r="AI24" s="40" t="n">
         <f aca="false">MAX(AI20:AI23)-AI25+1</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AK24" s="40" t="n">
         <f aca="false">MAX(AK20:AK23)-MIN(AK20:AK23)+1</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AL24" s="40" t="n">
         <f aca="false">MAX(AL20:AL23)-MIN(AL20:AL23)+1</f>
@@ -34906,11 +34917,11 @@
       </c>
       <c r="AH25" s="40" t="n">
         <f aca="false">MIN(AH20:AH23)</f>
-        <v>-100</v>
+        <v>-200</v>
       </c>
       <c r="AI25" s="40" t="n">
         <f aca="false">MIN(AI20:AI23)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AY25" s="70" t="str">
         <f aca="false">INDEX(T,24+MONTH(R60),lang) &amp; " " &amp; DAY(R60) &amp; ", " &amp; YEAR(R60) &amp; "   " &amp; TEXT(TIME(HOUR(R60),MINUTE(R60),0),"hh:mm")</f>
@@ -35030,7 +35041,7 @@
       </c>
       <c r="AA26" s="40" t="n">
         <f aca="false">COUNTIF(AN26:AN29,CONCATENATE("&gt;=",AN26))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB26" s="42" t="str">
         <f aca="false">VLOOKUP("Argentina",T,lang,0)</f>
@@ -35046,7 +35057,7 @@
       </c>
       <c r="AE26" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB26 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF26" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB26,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB26,$G$7:$G$54)</f>
@@ -35054,19 +35065,19 @@
       </c>
       <c r="AG26" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB26,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB26,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH26" s="40" t="n">
         <f aca="false">(AF26-AG26)*100+AK26*10000+AF26</f>
-        <v>10001</v>
+        <v>9701</v>
       </c>
       <c r="AI26" s="40" t="n">
         <f aca="false">AF26-AG26</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AJ26" s="40" t="n">
         <f aca="false">(AI26-AI31)/AI30</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AK26" s="40" t="n">
         <f aca="false">AC26*3+AD26</f>
@@ -35074,7 +35085,7 @@
       </c>
       <c r="AL26" s="40" t="n">
         <f aca="false">AP26/AP30*1000+AQ26/AQ30*100+AT26/AT30*10+AR26/AR30</f>
-        <v>50.5</v>
+        <v>0</v>
       </c>
       <c r="AM26" s="40" t="n">
         <f aca="false">VLOOKUP(AB26,db_fifarank,2,0)/2000000</f>
@@ -35082,7 +35093,7 @@
       </c>
       <c r="AN26" s="42" t="n">
         <f aca="false">1000*AK26/AK30+100*AJ26+10*AF26/AF30+1*AL26/AL30+AM26</f>
-        <v>294.314589857605</v>
+        <v>168.667340666667</v>
       </c>
       <c r="AO26" s="43" t="str">
         <f aca="false">IF(SUM(AC26:AE29)=12,J27,INDEX(T,76,lang))</f>
@@ -35094,15 +35105,15 @@
       </c>
       <c r="AQ26" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB26&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB26&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR26" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB26)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB26)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS26" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB26)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB26)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT26" s="44" t="n">
         <f aca="false">AR26-AS26</f>
@@ -35156,8 +35167,12 @@
         <f aca="false">AB20</f>
         <v>Francia</v>
       </c>
-      <c r="F27" s="64"/>
-      <c r="G27" s="65"/>
+      <c r="F27" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="65" t="n">
+        <v>0</v>
+      </c>
       <c r="H27" s="66" t="str">
         <f aca="false">AB22</f>
         <v>Perú</v>
@@ -35168,11 +35183,11 @@
       </c>
       <c r="K27" s="72" t="n">
         <f aca="false">L27+M27+N27</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L27" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA26:AK29,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M27" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA26:AK29,4,0)</f>
@@ -35184,11 +35199,11 @@
       </c>
       <c r="O27" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA26:AK29,6,0) &amp; " - " &amp; VLOOKUP(1,AA26:AK29,7,0)</f>
-        <v>2 - 0</v>
+        <v>5 - 0</v>
       </c>
       <c r="P27" s="73" t="n">
         <f aca="false">L27*3+M27</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R27" s="40" t="n">
         <f aca="false">DATE(2018,6,21)+TIME(4,0,0)+gmt_delta</f>
@@ -35196,11 +35211,11 @@
       </c>
       <c r="S27" s="41" t="str">
         <f aca="false">IF(OR(F27="",G27=""),"",IF(F27&gt;G27,E27&amp;"_win",IF(F27&lt;G27,E27&amp;"_lose",E27&amp;"_draw")))</f>
-        <v/>
+        <v>Francia_win</v>
       </c>
       <c r="T27" s="41" t="str">
         <f aca="false">IF(S27="","",IF(F27&lt;G27,H27&amp;"_win",IF(F27&gt;G27,H27&amp;"_lose",H27&amp;"_draw")))</f>
-        <v/>
+        <v>Perú_lose</v>
       </c>
       <c r="U27" s="42" t="n">
         <f aca="false">IF(S27="",0,IF(VLOOKUP(E27,$AB$8:$AK$53,7,0)=VLOOKUP(H27,$AB$8:$AK$53,7,0),1,0))</f>
@@ -35218,9 +35233,9 @@
         <f aca="false">IF(OR(E27=my_team,H27=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="40" t="str">
+      <c r="Y27" s="40" t="n">
         <f aca="false">IF(OR(F27="",G27=""),"",IF(F27&gt;G27,1,IF(F27&lt;G27,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA27" s="40" t="n">
         <f aca="false">COUNTIF(AN26:AN29,CONCATENATE("&gt;=",AN27))</f>
@@ -35240,7 +35255,7 @@
       </c>
       <c r="AE27" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB27 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF27" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB27,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB27,$G$7:$G$54)</f>
@@ -35248,19 +35263,19 @@
       </c>
       <c r="AG27" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB27,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB27,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH27" s="40" t="n">
         <f aca="false">(AF27-AG27)*100+AK27*10000+AF27</f>
-        <v>10001</v>
+        <v>9801</v>
       </c>
       <c r="AI27" s="40" t="n">
         <f aca="false">AF27-AG27</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AJ27" s="40" t="n">
         <f aca="false">(AI27-AI31)/AI30</f>
-        <v>0.4</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="AK27" s="40" t="n">
         <f aca="false">AC27*3+AD27</f>
@@ -35268,7 +35283,7 @@
       </c>
       <c r="AL27" s="40" t="n">
         <f aca="false">AP27/AP30*1000+AQ27/AQ30*100+AT27/AT30*10+AR27/AR30</f>
-        <v>50.5</v>
+        <v>0</v>
       </c>
       <c r="AM27" s="40" t="n">
         <f aca="false">VLOOKUP(AB27,db_fifarank,2,0)/2000000</f>
@@ -35276,7 +35291,7 @@
       </c>
       <c r="AN27" s="42" t="n">
         <f aca="false">1000*AK27/AK30+100*AJ27+10*AF27/AF30+1*AL27/AL30+AM27</f>
-        <v>294.314370857605</v>
+        <v>179.778232777778</v>
       </c>
       <c r="AO27" s="43" t="str">
         <f aca="false">IF(SUM(AC26:AE29)=12,J28,INDEX(T,77,lang))</f>
@@ -35288,15 +35303,15 @@
       </c>
       <c r="AQ27" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB27&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB27&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR27" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB27)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB27)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS27" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB27)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB27)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT27" s="44" t="n">
         <f aca="false">AR27-AS27</f>
@@ -35351,39 +35366,43 @@
         <f aca="false">AB23</f>
         <v>Dinamarca</v>
       </c>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65"/>
+      <c r="F28" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="65" t="n">
+        <v>1</v>
+      </c>
       <c r="H28" s="66" t="str">
         <f aca="false">AB21</f>
         <v>Australia</v>
       </c>
       <c r="J28" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA26:AK29,2,0)</f>
-        <v>Argentina</v>
+        <v>Nigeria</v>
       </c>
       <c r="K28" s="76" t="n">
         <f aca="false">L28+M28+N28</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L28" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA26:AK29,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA26:AK29,4,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA26:AK29,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA26:AK29,6,0) &amp; " - " &amp; VLOOKUP(2,AA26:AK29,7,0)</f>
-        <v>1 - 1</v>
+        <v>2 - 2</v>
       </c>
       <c r="P28" s="77" t="n">
         <f aca="false">L28*3+M28</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R28" s="40" t="n">
         <f aca="false">DATE(2018,6,21)+TIME(1,0,0)+gmt_delta</f>
@@ -35391,11 +35410,11 @@
       </c>
       <c r="S28" s="41" t="str">
         <f aca="false">IF(OR(F28="",G28=""),"",IF(F28&gt;G28,E28&amp;"_win",IF(F28&lt;G28,E28&amp;"_lose",E28&amp;"_draw")))</f>
-        <v/>
+        <v>Dinamarca_draw</v>
       </c>
       <c r="T28" s="41" t="str">
         <f aca="false">IF(S28="","",IF(F28&lt;G28,H28&amp;"_win",IF(F28&gt;G28,H28&amp;"_lose",H28&amp;"_draw")))</f>
-        <v/>
+        <v>Australia_draw</v>
       </c>
       <c r="U28" s="42" t="n">
         <f aca="false">IF(S28="",0,IF(VLOOKUP(E28,$AB$8:$AK$53,7,0)=VLOOKUP(H28,$AB$8:$AK$53,7,0),1,0))</f>
@@ -35413,9 +35432,9 @@
         <f aca="false">IF(OR(E28=my_team,H28=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y28" s="40" t="str">
+      <c r="Y28" s="40" t="n">
         <f aca="false">IF(OR(F28="",G28=""),"",IF(F28&gt;G28,1,IF(F28&lt;G28,-1,0)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AA28" s="40" t="n">
         <f aca="false">COUNTIF(AN26:AN29,CONCATENATE("&gt;=",AN28))</f>
@@ -35427,7 +35446,7 @@
       </c>
       <c r="AC28" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB28 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD28" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB28 &amp; "_draw")</f>
@@ -35439,7 +35458,7 @@
       </c>
       <c r="AF28" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB28,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB28,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AG28" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB28,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB28,$F$7:$F$54)</f>
@@ -35447,19 +35466,19 @@
       </c>
       <c r="AH28" s="40" t="n">
         <f aca="false">(AF28-AG28)*100+AK28*10000+AF28</f>
-        <v>30202</v>
+        <v>60505</v>
       </c>
       <c r="AI28" s="40" t="n">
         <f aca="false">AF28-AG28</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AJ28" s="40" t="n">
         <f aca="false">(AI28-AI31)/AI30</f>
-        <v>0.8</v>
+        <v>0.888888888888889</v>
       </c>
       <c r="AK28" s="40" t="n">
         <f aca="false">AC28*3+AD28</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL28" s="40" t="n">
         <f aca="false">AP28/AP30*1000+AQ28/AQ30*100+AT28/AT30*10+AR28/AR30</f>
@@ -35471,7 +35490,7 @@
       </c>
       <c r="AN28" s="42" t="n">
         <f aca="false">1000*AK28/AK30+100*AJ28+10*AF28/AF30+1*AL28/AL30+AM28</f>
-        <v>836.667175666667</v>
+        <v>1098.88939788889</v>
       </c>
       <c r="AP28" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB28&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB28&amp;"_win")*($U$7:$U$54))</f>
@@ -35541,8 +35560,12 @@
         <f aca="false">AB26</f>
         <v>Argentina</v>
       </c>
-      <c r="F29" s="64"/>
-      <c r="G29" s="65"/>
+      <c r="F29" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="65" t="n">
+        <v>3</v>
+      </c>
       <c r="H29" s="66" t="str">
         <f aca="false">AB28</f>
         <v>Croacia</v>
@@ -35553,7 +35576,7 @@
       </c>
       <c r="K29" s="76" t="n">
         <f aca="false">L29+M29+N29</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L29" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA26:AK29,3,0)</f>
@@ -35565,11 +35588,11 @@
       </c>
       <c r="N29" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA26:AK29,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA26:AK29,6,0) &amp; " - " &amp; VLOOKUP(3,AA26:AK29,7,0)</f>
-        <v>1 - 1</v>
+        <v>1 - 3</v>
       </c>
       <c r="P29" s="77" t="n">
         <f aca="false">L29*3+M29</f>
@@ -35581,11 +35604,11 @@
       </c>
       <c r="S29" s="41" t="str">
         <f aca="false">IF(OR(F29="",G29=""),"",IF(F29&gt;G29,E29&amp;"_win",IF(F29&lt;G29,E29&amp;"_lose",E29&amp;"_draw")))</f>
-        <v/>
+        <v>Argentina_lose</v>
       </c>
       <c r="T29" s="41" t="str">
         <f aca="false">IF(S29="","",IF(F29&lt;G29,H29&amp;"_win",IF(F29&gt;G29,H29&amp;"_lose",H29&amp;"_draw")))</f>
-        <v/>
+        <v>Croacia_win</v>
       </c>
       <c r="U29" s="42" t="n">
         <f aca="false">IF(S29="",0,IF(VLOOKUP(E29,$AB$8:$AK$53,7,0)=VLOOKUP(H29,$AB$8:$AK$53,7,0),1,0))</f>
@@ -35603,13 +35626,13 @@
         <f aca="false">IF(OR(E29=my_team,H29=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y29" s="40" t="str">
+      <c r="Y29" s="40" t="n">
         <f aca="false">IF(OR(F29="",G29=""),"",IF(F29&gt;G29,1,IF(F29&lt;G29,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA29" s="40" t="n">
         <f aca="false">COUNTIF(AN26:AN29,CONCATENATE("&gt;=",AN29))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB29" s="42" t="str">
         <f aca="false">VLOOKUP("Nigeria",T,lang,0)</f>
@@ -35617,7 +35640,7 @@
       </c>
       <c r="AC29" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB29 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD29" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB29 &amp; "_draw")</f>
@@ -35629,7 +35652,7 @@
       </c>
       <c r="AF29" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB29,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB29,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG29" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB29,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB29,$F$7:$F$54)</f>
@@ -35637,19 +35660,19 @@
       </c>
       <c r="AH29" s="40" t="n">
         <f aca="false">(AF29-AG29)*100+AK29*10000+AF29</f>
-        <v>-200</v>
+        <v>30002</v>
       </c>
       <c r="AI29" s="40" t="n">
         <f aca="false">AF29-AG29</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AJ29" s="40" t="n">
         <f aca="false">(AI29-AI31)/AI30</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="AK29" s="40" t="n">
         <f aca="false">AC29*3+AD29</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL29" s="40" t="n">
         <f aca="false">AP29/AP30*1000+AQ29/AQ30*100+AT29/AT30*10+AR29/AR30</f>
@@ -35661,7 +35684,7 @@
       </c>
       <c r="AN29" s="42" t="n">
         <f aca="false">1000*AK29/AK30+100*AJ29+10*AF29/AF30+1*AL29/AL30+AM29</f>
-        <v>0.00032</v>
+        <v>537.333653333333</v>
       </c>
       <c r="AP29" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB29&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB29&amp;"_win")*($U$7:$U$54))</f>
@@ -35732,19 +35755,23 @@
         <f aca="false">AB29</f>
         <v>Nigeria</v>
       </c>
-      <c r="F30" s="64"/>
-      <c r="G30" s="65"/>
+      <c r="F30" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="65" t="n">
+        <v>0</v>
+      </c>
       <c r="H30" s="66" t="str">
         <f aca="false">AB27</f>
         <v>Islandia</v>
       </c>
       <c r="J30" s="87" t="str">
         <f aca="false">VLOOKUP(4,AA26:AK29,2,0)</f>
-        <v>Nigeria</v>
+        <v>Argentina</v>
       </c>
       <c r="K30" s="88" t="n">
         <f aca="false">L30+M30+N30</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L30" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA26:AK29,3,0)</f>
@@ -35752,7 +35779,7 @@
       </c>
       <c r="M30" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA26:AK29,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA26:AK29,5,0)</f>
@@ -35760,11 +35787,11 @@
       </c>
       <c r="O30" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA26:AK29,6,0) &amp; " - " &amp; VLOOKUP(4,AA26:AK29,7,0)</f>
-        <v>0 - 2</v>
+        <v>1 - 4</v>
       </c>
       <c r="P30" s="89" t="n">
         <f aca="false">L30*3+M30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" s="40" t="n">
         <f aca="false">DATE(2018,6,22)+TIME(4,0,0)+gmt_delta</f>
@@ -35772,11 +35799,11 @@
       </c>
       <c r="S30" s="41" t="str">
         <f aca="false">IF(OR(F30="",G30=""),"",IF(F30&gt;G30,E30&amp;"_win",IF(F30&lt;G30,E30&amp;"_lose",E30&amp;"_draw")))</f>
-        <v/>
+        <v>Nigeria_win</v>
       </c>
       <c r="T30" s="41" t="str">
         <f aca="false">IF(S30="","",IF(F30&lt;G30,H30&amp;"_win",IF(F30&gt;G30,H30&amp;"_lose",H30&amp;"_draw")))</f>
-        <v/>
+        <v>Islandia_lose</v>
       </c>
       <c r="U30" s="42" t="n">
         <f aca="false">IF(S30="",0,IF(VLOOKUP(E30,$AB$8:$AK$53,7,0)=VLOOKUP(H30,$AB$8:$AK$53,7,0),1,0))</f>
@@ -35794,13 +35821,13 @@
         <f aca="false">IF(OR(E30=my_team,H30=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y30" s="40" t="str">
+      <c r="Y30" s="40" t="n">
         <f aca="false">IF(OR(F30="",G30=""),"",IF(F30&gt;G30,1,IF(F30&lt;G30,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AC30" s="40" t="n">
         <f aca="false">MAX(AC26:AC29)-MIN(AC26:AC29)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD30" s="40" t="n">
         <f aca="false">MAX(AD26:AD29)-MIN(AD26:AD29)+1</f>
@@ -35812,27 +35839,27 @@
       </c>
       <c r="AF30" s="40" t="n">
         <f aca="false">MAX(AF26:AF29)-MIN(AF26:AF29)+1</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG30" s="40" t="n">
         <f aca="false">MAX(AG26:AG29)-MIN(AG26:AG29)+1</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH30" s="40" t="n">
         <f aca="false">MAX(AH26:AH29)-AH31+1</f>
-        <v>30403</v>
+        <v>50805</v>
       </c>
       <c r="AI30" s="40" t="n">
         <f aca="false">MAX(AI26:AI29)-AI31+1</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AK30" s="40" t="n">
         <f aca="false">MAX(AK26:AK29)-MIN(AK26:AK29)+1</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AL30" s="40" t="n">
         <f aca="false">MAX(AL26:AL29)-MIN(AL26:AL29)+1</f>
-        <v>51.5</v>
+        <v>1</v>
       </c>
       <c r="AP30" s="40" t="n">
         <f aca="false">MAX(AP26:AP29)-MIN(AP26:AP29)+1</f>
@@ -35840,15 +35867,15 @@
       </c>
       <c r="AQ30" s="40" t="n">
         <f aca="false">MAX(AQ26:AQ29)-MIN(AQ26:AQ29)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR30" s="40" t="n">
         <f aca="false">MAX(AR26:AR29)-MIN(AR26:AR29)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS30" s="40" t="n">
         <f aca="false">MAX(AS26:AS29)-MIN(AS26:AS29)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT30" s="40" t="n">
         <f aca="false">MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
@@ -35902,8 +35929,12 @@
         <f aca="false">AB32</f>
         <v>Brasil</v>
       </c>
-      <c r="F31" s="64"/>
-      <c r="G31" s="65"/>
+      <c r="F31" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="65" t="n">
+        <v>0</v>
+      </c>
       <c r="H31" s="66" t="str">
         <f aca="false">AB34</f>
         <v>Costa Rica</v>
@@ -35914,11 +35945,11 @@
       </c>
       <c r="S31" s="41" t="str">
         <f aca="false">IF(OR(F31="",G31=""),"",IF(F31&gt;G31,E31&amp;"_win",IF(F31&lt;G31,E31&amp;"_lose",E31&amp;"_draw")))</f>
-        <v/>
+        <v>Brasil_win</v>
       </c>
       <c r="T31" s="41" t="str">
         <f aca="false">IF(S31="","",IF(F31&lt;G31,H31&amp;"_win",IF(F31&gt;G31,H31&amp;"_lose",H31&amp;"_draw")))</f>
-        <v/>
+        <v>Costa Rica_lose</v>
       </c>
       <c r="U31" s="42" t="n">
         <f aca="false">IF(S31="",0,IF(VLOOKUP(E31,$AB$8:$AK$53,7,0)=VLOOKUP(H31,$AB$8:$AK$53,7,0),1,0))</f>
@@ -35936,17 +35967,17 @@
         <f aca="false">IF(OR(E31=my_team,H31=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y31" s="40" t="str">
+      <c r="Y31" s="40" t="n">
         <f aca="false">IF(OR(F31="",G31=""),"",IF(F31&gt;G31,1,IF(F31&lt;G31,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AH31" s="40" t="n">
         <f aca="false">MIN(AH26:AH29)</f>
-        <v>-200</v>
+        <v>9701</v>
       </c>
       <c r="AI31" s="40" t="n">
         <f aca="false">MIN(AI26:AI29)</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AY31" s="78"/>
       <c r="AZ31" s="82" t="str">
@@ -36000,8 +36031,12 @@
         <f aca="false">AB35</f>
         <v>Serbia</v>
       </c>
-      <c r="F32" s="64"/>
-      <c r="G32" s="65"/>
+      <c r="F32" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="99" t="n">
+        <v>2</v>
+      </c>
       <c r="H32" s="66" t="str">
         <f aca="false">AB33</f>
         <v>Suiza</v>
@@ -36040,11 +36075,11 @@
       </c>
       <c r="S32" s="41" t="str">
         <f aca="false">IF(OR(F32="",G32=""),"",IF(F32&gt;G32,E32&amp;"_win",IF(F32&lt;G32,E32&amp;"_lose",E32&amp;"_draw")))</f>
-        <v/>
+        <v>Serbia_lose</v>
       </c>
       <c r="T32" s="41" t="str">
         <f aca="false">IF(S32="","",IF(F32&lt;G32,H32&amp;"_win",IF(F32&gt;G32,H32&amp;"_lose",H32&amp;"_draw")))</f>
-        <v/>
+        <v>Suiza_win</v>
       </c>
       <c r="U32" s="42" t="n">
         <f aca="false">IF(S32="",0,IF(VLOOKUP(E32,$AB$8:$AK$53,7,0)=VLOOKUP(H32,$AB$8:$AK$53,7,0),1,0))</f>
@@ -36062,13 +36097,13 @@
         <f aca="false">IF(OR(E32=my_team,H32=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y32" s="40" t="str">
+      <c r="Y32" s="40" t="n">
         <f aca="false">IF(OR(F32="",G32=""),"",IF(F32&gt;G32,1,IF(F32&lt;G32,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA32" s="40" t="n">
         <f aca="false">COUNTIF(AN32:AN35,CONCATENATE("&gt;=",AN32))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB32" s="42" t="str">
         <f aca="false">VLOOKUP("Brazil",T,lang,0)</f>
@@ -36076,7 +36111,7 @@
       </c>
       <c r="AC32" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB32 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB32 &amp; "_draw")</f>
@@ -36088,7 +36123,7 @@
       </c>
       <c r="AF32" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB32,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB32,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG32" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB32,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB32,$F$7:$F$54)</f>
@@ -36096,23 +36131,23 @@
       </c>
       <c r="AH32" s="40" t="n">
         <f aca="false">(AF32-AG32)*100+AK32*10000+AF32</f>
-        <v>10001</v>
+        <v>40203</v>
       </c>
       <c r="AI32" s="40" t="n">
         <f aca="false">AF32-AG32</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ32" s="40" t="n">
         <f aca="false">(AI32-AI37)/AI36</f>
-        <v>0.333333333333333</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="AK32" s="40" t="n">
         <f aca="false">AC32*3+AD32</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AL32" s="40" t="n">
         <f aca="false">AP32/AP36*1000+AQ32/AQ36*100+AT32/AT36*10+AR32/AR36</f>
-        <v>50.5</v>
+        <v>0</v>
       </c>
       <c r="AM32" s="40" t="n">
         <f aca="false">VLOOKUP(AB32,db_fifarank,2,0)/2000000</f>
@@ -36120,7 +36155,7 @@
       </c>
       <c r="AN32" s="42" t="n">
         <f aca="false">1000*AK32/AK36+100*AJ32+10*AF32/AF36+1*AL32/AL36+AM32</f>
-        <v>289.314657357605</v>
+        <v>890.834074833333</v>
       </c>
       <c r="AO32" s="43" t="str">
         <f aca="false">IF(SUM(AC32:AE35)=12,J33,INDEX(T,78,lang))</f>
@@ -36132,15 +36167,15 @@
       </c>
       <c r="AQ32" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB32&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB32&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR32" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB32)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB32)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS32" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB32)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB32)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT32" s="44" t="n">
         <f aca="false">AR32-AS32</f>
@@ -36202,11 +36237,11 @@
       </c>
       <c r="J33" s="71" t="str">
         <f aca="false">VLOOKUP(1,AA32:AK35,2,0)</f>
-        <v>Serbia</v>
+        <v>Brasil</v>
       </c>
       <c r="K33" s="72" t="n">
         <f aca="false">L33+M33+N33</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L33" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA32:AK35,3,0)</f>
@@ -36214,7 +36249,7 @@
       </c>
       <c r="M33" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA32:AK35,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA32:AK35,5,0)</f>
@@ -36222,11 +36257,11 @@
       </c>
       <c r="O33" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(1,AA32:AK35,7,0)</f>
-        <v>1 - 0</v>
+        <v>3 - 1</v>
       </c>
       <c r="P33" s="73" t="n">
         <f aca="false">L33*3+M33</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R33" s="40" t="n">
         <f aca="false">DATE(2018,6,23)+TIME(7,0,0)+gmt_delta</f>
@@ -36262,7 +36297,7 @@
       </c>
       <c r="AA33" s="40" t="n">
         <f aca="false">COUNTIF(AN32:AN35,CONCATENATE("&gt;=",AN33))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB33" s="42" t="str">
         <f aca="false">VLOOKUP("Switzerland",T,lang,0)</f>
@@ -36270,7 +36305,7 @@
       </c>
       <c r="AC33" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB33 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD33" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB33 &amp; "_draw")</f>
@@ -36282,31 +36317,31 @@
       </c>
       <c r="AF33" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB33,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB33,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG33" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB33,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB33,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH33" s="40" t="n">
         <f aca="false">(AF33-AG33)*100+AK33*10000+AF33</f>
-        <v>10001</v>
+        <v>40103</v>
       </c>
       <c r="AI33" s="40" t="n">
         <f aca="false">AF33-AG33</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ33" s="40" t="n">
         <f aca="false">(AI33-AI37)/AI36</f>
-        <v>0.333333333333333</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="AK33" s="40" t="n">
         <f aca="false">AC33*3+AD33</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AL33" s="40" t="n">
         <f aca="false">AP33/AP36*1000+AQ33/AQ36*100+AT33/AT36*10+AR33/AR36</f>
-        <v>50.5</v>
+        <v>0</v>
       </c>
       <c r="AM33" s="40" t="n">
         <f aca="false">VLOOKUP(AB33,db_fifarank,2,0)/2000000</f>
@@ -36314,7 +36349,7 @@
       </c>
       <c r="AN33" s="42" t="n">
         <f aca="false">1000*AK33/AK36+100*AJ33+10*AF33/AF36+1*AL33/AL36+AM33</f>
-        <v>289.314510857605</v>
+        <v>874.167261666667</v>
       </c>
       <c r="AO33" s="43" t="str">
         <f aca="false">IF(SUM(AC32:AE35)=12,J34,INDEX(T,79,lang))</f>
@@ -36326,15 +36361,15 @@
       </c>
       <c r="AQ33" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB33&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB33&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR33" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB33)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB33)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS33" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB33)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB33)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT33" s="44" t="n">
         <f aca="false">AR33-AS33</f>
@@ -36397,15 +36432,15 @@
       </c>
       <c r="J34" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA32:AK35,2,0)</f>
-        <v>Brasil</v>
+        <v>Suiza</v>
       </c>
       <c r="K34" s="76" t="n">
         <f aca="false">L34+M34+N34</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L34" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA32:AK35,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA32:AK35,4,0)</f>
@@ -36417,11 +36452,11 @@
       </c>
       <c r="O34" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(2,AA32:AK35,7,0)</f>
-        <v>1 - 1</v>
+        <v>3 - 2</v>
       </c>
       <c r="P34" s="77" t="n">
         <f aca="false">L34*3+M34</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R34" s="40" t="n">
         <f aca="false">DATE(2018,6,23)+TIME(4,0,0)+gmt_delta</f>
@@ -36473,7 +36508,7 @@
       </c>
       <c r="AE34" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB34 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF34" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB34,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB34,$G$7:$G$54)</f>
@@ -36481,15 +36516,15 @@
       </c>
       <c r="AG34" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB34,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB34,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH34" s="40" t="n">
         <f aca="false">(AF34-AG34)*100+AK34*10000+AF34</f>
-        <v>-100</v>
+        <v>-300</v>
       </c>
       <c r="AI34" s="40" t="n">
         <f aca="false">AF34-AG34</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AJ34" s="40" t="n">
         <f aca="false">(AI34-AI37)/AI36</f>
@@ -36590,31 +36625,31 @@
       </c>
       <c r="J35" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA32:AK35,2,0)</f>
-        <v>Suiza</v>
+        <v>Serbia</v>
       </c>
       <c r="K35" s="76" t="n">
         <f aca="false">L35+M35+N35</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L35" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA32:AK35,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA32:AK35,4,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA32:AK35,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(3,AA32:AK35,7,0)</f>
-        <v>1 - 1</v>
+        <v>2 - 2</v>
       </c>
       <c r="P35" s="77" t="n">
         <f aca="false">L35*3+M35</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R35" s="40" t="n">
         <f aca="false">DATE(2018,6,23)+TIME(1,0,0)+gmt_delta</f>
@@ -36650,7 +36685,7 @@
       </c>
       <c r="AA35" s="40" t="n">
         <f aca="false">COUNTIF(AN32:AN35,CONCATENATE("&gt;=",AN35))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB35" s="42" t="str">
         <f aca="false">VLOOKUP("Serbia",T,lang,0)</f>
@@ -36666,27 +36701,27 @@
       </c>
       <c r="AE35" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB35 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF35" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB35,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB35,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG35" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB35,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB35,$F$7:$F$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH35" s="40" t="n">
         <f aca="false">(AF35-AG35)*100+AK35*10000+AF35</f>
-        <v>30101</v>
+        <v>30002</v>
       </c>
       <c r="AI35" s="40" t="n">
         <f aca="false">AF35-AG35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ35" s="40" t="n">
         <f aca="false">(AI35-AI37)/AI36</f>
-        <v>0.666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AK35" s="40" t="n">
         <f aca="false">AC35*3+AD35</f>
@@ -36702,7 +36737,7 @@
       </c>
       <c r="AN35" s="42" t="n">
         <f aca="false">1000*AK35/AK36+100*AJ35+10*AF35/AF36+1*AL35/AL36+AM35</f>
-        <v>821.667044666667</v>
+        <v>655.000378</v>
       </c>
       <c r="AP35" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB35&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB35&amp;"_win")*($U$7:$U$54))</f>
@@ -36790,7 +36825,7 @@
       </c>
       <c r="K36" s="88" t="n">
         <f aca="false">L36+M36+N36</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L36" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA32:AK35,3,0)</f>
@@ -36802,11 +36837,11 @@
       </c>
       <c r="N36" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA32:AK35,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O36" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(4,AA32:AK35,7,0)</f>
-        <v>0 - 1</v>
+        <v>0 - 3</v>
       </c>
       <c r="P36" s="89" t="n">
         <f aca="false">L36*3+M36</f>
@@ -36854,31 +36889,31 @@
       </c>
       <c r="AE36" s="40" t="n">
         <f aca="false">MAX(AE32:AE35)-MIN(AE32:AE35)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF36" s="40" t="n">
         <f aca="false">MAX(AF32:AF35)-MIN(AF32:AF35)+1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG36" s="40" t="n">
         <f aca="false">MAX(AG32:AG35)-MIN(AG32:AG35)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH36" s="40" t="n">
         <f aca="false">MAX(AH32:AH35)-AH37+1</f>
-        <v>30202</v>
+        <v>40504</v>
       </c>
       <c r="AI36" s="40" t="n">
         <f aca="false">MAX(AI32:AI35)-AI37+1</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AK36" s="40" t="n">
         <f aca="false">MAX(AK32:AK35)-MIN(AK32:AK35)+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL36" s="40" t="n">
         <f aca="false">MAX(AL32:AL35)-MIN(AL32:AL35)+1</f>
-        <v>51.5</v>
+        <v>1</v>
       </c>
       <c r="AP36" s="40" t="n">
         <f aca="false">MAX(AP32:AP35)-MIN(AP32:AP35)+1</f>
@@ -36886,15 +36921,15 @@
       </c>
       <c r="AQ36" s="40" t="n">
         <f aca="false">MAX(AQ32:AQ35)-MIN(AQ32:AQ35)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR36" s="40" t="n">
         <f aca="false">MAX(AR32:AR35)-MIN(AR32:AR35)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS36" s="40" t="n">
         <f aca="false">MAX(AS32:AS35)-MIN(AS32:AS35)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT36" s="40" t="n">
         <f aca="false">MAX(AT32:AT35)-MIN(AT32:AT35)+1</f>
@@ -36991,11 +37026,11 @@
       </c>
       <c r="AH37" s="40" t="n">
         <f aca="false">MIN(AH32:AH35)</f>
-        <v>-100</v>
+        <v>-300</v>
       </c>
       <c r="AI37" s="40" t="n">
         <f aca="false">MIN(AI32:AI35)</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AY37" s="70" t="str">
         <f aca="false">INDEX(T,24+MONTH(R65),lang) &amp; " " &amp; DAY(R65) &amp; ", " &amp; YEAR(R65) &amp; "   " &amp; TEXT(TIME(HOUR(R65),MINUTE(R65),0),"hh:mm")</f>
@@ -37727,23 +37762,23 @@
         <f aca="false">AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="99" t="str">
+      <c r="BJ41" s="100" t="str">
         <f aca="false">INDEX(T,102,lang)</f>
         <v>Campeón 2018</v>
       </c>
-      <c r="BK41" s="99"/>
-      <c r="BL41" s="99"/>
-      <c r="BM41" s="99"/>
-      <c r="BN41" s="99"/>
-      <c r="BO41" s="100" t="str">
+      <c r="BK41" s="100"/>
+      <c r="BL41" s="100"/>
+      <c r="BM41" s="100"/>
+      <c r="BN41" s="100"/>
+      <c r="BO41" s="101" t="str">
         <f aca="false">S85</f>
         <v/>
       </c>
-      <c r="BP41" s="100"/>
-      <c r="BQ41" s="100"/>
-      <c r="BR41" s="100"/>
-      <c r="BS41" s="100"/>
-      <c r="BT41" s="100"/>
+      <c r="BP41" s="101"/>
+      <c r="BQ41" s="101"/>
+      <c r="BR41" s="101"/>
+      <c r="BS41" s="101"/>
+      <c r="BT41" s="101"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="59" t="n">
@@ -37887,17 +37922,17 @@
         <f aca="false">MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>1</v>
       </c>
-      <c r="BJ42" s="99"/>
-      <c r="BK42" s="99"/>
-      <c r="BL42" s="99"/>
-      <c r="BM42" s="99"/>
-      <c r="BN42" s="99"/>
-      <c r="BO42" s="100"/>
-      <c r="BP42" s="100"/>
-      <c r="BQ42" s="100"/>
-      <c r="BR42" s="100"/>
-      <c r="BS42" s="100"/>
-      <c r="BT42" s="100"/>
+      <c r="BJ42" s="100"/>
+      <c r="BK42" s="100"/>
+      <c r="BL42" s="100"/>
+      <c r="BM42" s="100"/>
+      <c r="BN42" s="100"/>
+      <c r="BO42" s="101"/>
+      <c r="BP42" s="101"/>
+      <c r="BQ42" s="101"/>
+      <c r="BR42" s="101"/>
+      <c r="BS42" s="101"/>
+      <c r="BT42" s="101"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="59" t="n">
@@ -37965,7 +38000,7 @@
         <f aca="false">MIN(AI38:AI41)</f>
         <v>-1</v>
       </c>
-      <c r="AY43" s="101"/>
+      <c r="AY43" s="102"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="59" t="n">
@@ -38463,12 +38498,12 @@
         <f aca="false">AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="102" t="s">
+      <c r="AY46" s="103" t="s">
         <v>2559</v>
       </c>
-      <c r="AZ46" s="102"/>
-      <c r="BA46" s="102"/>
-      <c r="BB46" s="102"/>
+      <c r="AZ46" s="103"/>
+      <c r="BA46" s="103"/>
+      <c r="BB46" s="103"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="59" t="n">
@@ -38632,10 +38667,10 @@
         <f aca="false">AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="102"/>
-      <c r="AZ47" s="102"/>
-      <c r="BA47" s="102"/>
-      <c r="BB47" s="102"/>
+      <c r="AY47" s="103"/>
+      <c r="AZ47" s="103"/>
+      <c r="BA47" s="103"/>
+      <c r="BB47" s="103"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="59" t="n">
@@ -38779,10 +38814,10 @@
         <f aca="false">MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="102"/>
-      <c r="AZ48" s="102"/>
-      <c r="BA48" s="102"/>
-      <c r="BB48" s="102"/>
+      <c r="AY48" s="103"/>
+      <c r="AZ48" s="103"/>
+      <c r="BA48" s="103"/>
+      <c r="BB48" s="103"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="59" t="n">
@@ -38850,10 +38885,10 @@
         <f aca="false">MIN(AI44:AI47)</f>
         <v>-3</v>
       </c>
-      <c r="AY49" s="102"/>
-      <c r="AZ49" s="102"/>
-      <c r="BA49" s="102"/>
-      <c r="BB49" s="102"/>
+      <c r="AY49" s="103"/>
+      <c r="AZ49" s="103"/>
+      <c r="BA49" s="103"/>
+      <c r="BB49" s="103"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="59" t="n">
@@ -39021,10 +39056,10 @@
         <f aca="false">AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="102"/>
-      <c r="AZ50" s="102"/>
-      <c r="BA50" s="102"/>
-      <c r="BB50" s="102"/>
+      <c r="AY50" s="103"/>
+      <c r="AZ50" s="103"/>
+      <c r="BA50" s="103"/>
+      <c r="BB50" s="103"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="59" t="n">
@@ -39192,10 +39227,10 @@
         <f aca="false">AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="102"/>
-      <c r="AZ51" s="102"/>
-      <c r="BA51" s="102"/>
-      <c r="BB51" s="102"/>
+      <c r="AY51" s="103"/>
+      <c r="AZ51" s="103"/>
+      <c r="BA51" s="103"/>
+      <c r="BB51" s="103"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="59" t="n">
@@ -39359,10 +39394,10 @@
         <f aca="false">AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="102"/>
-      <c r="AZ52" s="102"/>
-      <c r="BA52" s="102"/>
-      <c r="BB52" s="102"/>
+      <c r="AY52" s="103"/>
+      <c r="AZ52" s="103"/>
+      <c r="BA52" s="103"/>
+      <c r="BB52" s="103"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="59" t="n">
@@ -39528,28 +39563,28 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="103" t="n">
+      <c r="A54" s="104" t="n">
         <v>48</v>
       </c>
-      <c r="B54" s="104" t="str">
+      <c r="B54" s="105" t="str">
         <f aca="false">INDEX(T,18+INT(MOD(R54-1,7)),lang)</f>
         <v>Thu</v>
       </c>
-      <c r="C54" s="105" t="str">
+      <c r="C54" s="106" t="str">
         <f aca="false">INDEX(T,24+MONTH(R54),lang) &amp; " " &amp; DAY(R54) &amp; ", " &amp; YEAR(R54)</f>
         <v>Jun 28, 2018</v>
       </c>
-      <c r="D54" s="106" t="n">
+      <c r="D54" s="107" t="n">
         <f aca="false">TIME(HOUR(R54),MINUTE(R54),0)</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="E54" s="107" t="str">
+      <c r="E54" s="108" t="str">
         <f aca="false">AB51</f>
         <v>Senegal</v>
       </c>
       <c r="F54" s="83"/>
       <c r="G54" s="84"/>
-      <c r="H54" s="108" t="str">
+      <c r="H54" s="109" t="str">
         <f aca="false">AB52</f>
         <v>Colombia</v>
       </c>
@@ -39672,13 +39707,13 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="92"/>
-      <c r="B55" s="109"/>
+      <c r="B55" s="110"/>
       <c r="C55" s="92"/>
-      <c r="D55" s="110"/>
-      <c r="E55" s="111"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="113"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="112"/>
+      <c r="F55" s="113"/>
+      <c r="G55" s="113"/>
+      <c r="H55" s="114"/>
       <c r="J55" s="91"/>
       <c r="K55" s="92"/>
       <c r="L55" s="92"/>

</xml_diff>

<commit_message>
Se actualizan resultados hasta el dia 24 de junio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -13690,9 +13690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>171720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13706,7 +13706,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1232280"/>
-          <a:ext cx="227520" cy="150120"/>
+          <a:ext cx="226440" cy="149040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13727,9 +13727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1488600</xdr:colOff>
+      <xdr:colOff>1487520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13743,7 +13743,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4275360"/>
-          <a:ext cx="227520" cy="150120"/>
+          <a:ext cx="226440" cy="149040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13764,9 +13764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250200</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13780,7 +13780,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7323480"/>
-          <a:ext cx="227520" cy="150120"/>
+          <a:ext cx="226440" cy="149040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13801,9 +13801,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13817,7 +13817,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="1232280"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13838,9 +13838,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13854,7 +13854,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4470840"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13875,9 +13875,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13891,7 +13891,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7518600"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13912,9 +13912,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13928,7 +13928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1422720"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13949,9 +13949,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>252000</xdr:colOff>
+      <xdr:colOff>250920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13965,7 +13965,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5460840" y="4280040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13986,9 +13986,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14002,7 +14002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7518600"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14023,9 +14023,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:rowOff>182160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14039,7 +14039,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1431720"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14060,9 +14060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14076,7 +14076,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4484520"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14097,9 +14097,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14113,7 +14113,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7332840"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14134,9 +14134,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14150,7 +14150,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1613160"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14171,9 +14171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14187,7 +14187,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4661280"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14208,9 +14208,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14224,7 +14224,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="7709040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14245,9 +14245,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14261,7 +14261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1613160"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14282,9 +14282,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14298,7 +14298,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4856400"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14319,9 +14319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481040</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14335,7 +14335,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="7899840"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14356,9 +14356,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14372,7 +14372,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="7904520"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14393,9 +14393,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14409,7 +14409,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="4661280"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14430,9 +14430,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14446,7 +14446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1798920"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14467,9 +14467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14483,7 +14483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1803600"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14504,9 +14504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14520,7 +14520,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="4847040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14541,9 +14541,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14557,7 +14557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="7704360"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14578,9 +14578,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14594,7 +14594,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="1994040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14615,9 +14615,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14631,7 +14631,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5042160"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14652,9 +14652,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14668,7 +14668,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="8090280"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14689,9 +14689,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14705,7 +14705,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="1994040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14726,9 +14726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14742,7 +14742,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5227920"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14763,9 +14763,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481040</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14779,7 +14779,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8276040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14800,9 +14800,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14816,7 +14816,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2184840"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14837,9 +14837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14853,7 +14853,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="5042160"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14874,9 +14874,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14890,7 +14890,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="8276040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14911,9 +14911,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14927,7 +14927,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2180160"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14948,9 +14948,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14964,7 +14964,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5227920"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14985,9 +14985,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481040</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15001,7 +15001,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8085600"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15022,9 +15022,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15038,7 +15038,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2370600"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15059,9 +15059,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15075,7 +15075,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="5423040"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15096,9 +15096,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15112,7 +15112,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="8466480"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15133,9 +15133,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15149,7 +15149,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456160" y="2375280"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15170,9 +15170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481040</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15186,7 +15186,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8661600"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15207,9 +15207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15223,7 +15223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5613840"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15244,9 +15244,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15260,7 +15260,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926520" y="2565720"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15281,9 +15281,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241920</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15297,7 +15297,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5450760" y="5417640"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15318,9 +15318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15334,7 +15334,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455080" y="8656200"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15355,9 +15355,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241920</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15371,7 +15371,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5450760" y="2564640"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15392,9 +15392,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15408,7 +15408,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3925440" y="5612760"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15429,9 +15429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480320</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15445,7 +15445,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921120" y="8465760"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15466,9 +15466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15482,7 +15482,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="2757240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15503,9 +15503,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15519,7 +15519,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="5800680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15540,9 +15540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15556,7 +15556,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="8848440"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15577,9 +15577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>199080</xdr:colOff>
+      <xdr:colOff>198000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15593,7 +15593,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481000" y="2752560"/>
-          <a:ext cx="151560" cy="151560"/>
+          <a:ext cx="150480" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15614,9 +15614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>193320</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15630,7 +15630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5476320" y="5991120"/>
-          <a:ext cx="151560" cy="151560"/>
+          <a:ext cx="150480" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15651,9 +15651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1442160</xdr:colOff>
+      <xdr:colOff>1441080</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15667,7 +15667,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956040" y="9039240"/>
-          <a:ext cx="151560" cy="151560"/>
+          <a:ext cx="150480" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15688,9 +15688,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15704,7 +15704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="2943000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15725,9 +15725,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15741,7 +15741,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="5800680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15762,9 +15762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15778,7 +15778,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9039240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15799,9 +15799,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15815,7 +15815,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="2943000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15836,9 +15836,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15852,7 +15852,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="5991120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15873,9 +15873,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15889,7 +15889,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="8848440"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15910,9 +15910,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15926,7 +15926,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3133440"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15947,9 +15947,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15963,7 +15963,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="6181560"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15984,9 +15984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16000,7 +16000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9229680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16021,9 +16021,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16037,7 +16037,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3138120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16058,9 +16058,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16074,7 +16074,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6372000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16095,9 +16095,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16111,7 +16111,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="9420120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16132,9 +16132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16148,7 +16148,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3324240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16169,9 +16169,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16185,7 +16185,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6181560"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16206,9 +16206,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16222,7 +16222,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9420120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16243,9 +16243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16259,7 +16259,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3324240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16280,9 +16280,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16296,7 +16296,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="6372000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16317,9 +16317,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16333,7 +16333,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9229680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16354,9 +16354,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1464840</xdr:colOff>
+      <xdr:colOff>1463760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16370,7 +16370,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3951360" y="3514680"/>
-          <a:ext cx="178920" cy="151560"/>
+          <a:ext cx="177840" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16391,9 +16391,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1464840</xdr:colOff>
+      <xdr:colOff>1463760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16407,7 +16407,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3951360" y="6562440"/>
-          <a:ext cx="178920" cy="151560"/>
+          <a:ext cx="177840" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16428,9 +16428,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>217080</xdr:colOff>
+      <xdr:colOff>216000</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16444,7 +16444,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5471640" y="9610560"/>
-          <a:ext cx="178920" cy="151560"/>
+          <a:ext cx="177840" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16465,9 +16465,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16481,7 +16481,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="3514680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16502,9 +16502,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16518,7 +16518,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="6753240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16539,9 +16539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16555,7 +16555,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9801000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16576,9 +16576,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16592,7 +16592,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3705120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16613,9 +16613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16629,7 +16629,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="6562440"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16650,9 +16650,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16666,7 +16666,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9801000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16687,9 +16687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16703,7 +16703,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="3895560"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16724,9 +16724,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16740,7 +16740,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="6943680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16761,9 +16761,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16777,7 +16777,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="9991440"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16798,9 +16798,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16814,7 +16814,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="3900240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16835,9 +16835,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16851,7 +16851,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="7134120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16872,9 +16872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16888,7 +16888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="10182240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16909,9 +16909,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16925,7 +16925,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="4090680"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16946,9 +16946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16962,7 +16962,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="6948360"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16983,9 +16983,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16999,7 +16999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="10182240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17020,9 +17020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17036,7 +17036,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452560" y="4086000"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17057,9 +17057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17073,7 +17073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="7134120"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17094,9 +17094,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17110,7 +17110,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="9991440"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17131,9 +17131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17147,7 +17147,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457240" y="3709800"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17168,9 +17168,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486800</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17184,7 +17184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927600" y="6753240"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17205,9 +17205,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482120</xdr:colOff>
+      <xdr:colOff>1481040</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17221,7 +17221,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922920" y="9610560"/>
-          <a:ext cx="224640" cy="151560"/>
+          <a:ext cx="223560" cy="150480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31400,8 +31400,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J54" activeCellId="0" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36229,8 +36229,12 @@
         <f aca="false">AB38</f>
         <v>Alemania</v>
       </c>
-      <c r="F33" s="64"/>
-      <c r="G33" s="65"/>
+      <c r="F33" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="65" t="n">
+        <v>1</v>
+      </c>
       <c r="H33" s="66" t="str">
         <f aca="false">AB40</f>
         <v>Suecia</v>
@@ -36269,31 +36273,31 @@
       </c>
       <c r="S33" s="41" t="str">
         <f aca="false">IF(OR(F33="",G33=""),"",IF(F33&gt;G33,E33&amp;"_win",IF(F33&lt;G33,E33&amp;"_lose",E33&amp;"_draw")))</f>
-        <v/>
+        <v>Alemania_win</v>
       </c>
       <c r="T33" s="41" t="str">
         <f aca="false">IF(S33="","",IF(F33&lt;G33,H33&amp;"_win",IF(F33&gt;G33,H33&amp;"_lose",H33&amp;"_draw")))</f>
-        <v/>
+        <v>Suecia_lose</v>
       </c>
       <c r="U33" s="42" t="n">
         <f aca="false">IF(S33="",0,IF(VLOOKUP(E33,$AB$8:$AK$53,7,0)=VLOOKUP(H33,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33" s="40" t="n">
         <f aca="false">U33*F33</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W33" s="40" t="n">
         <f aca="false">U33*G33</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X33" s="40" t="n">
         <f aca="false">IF(OR(E33=my_team,H33=my_team),1,0)</f>
         <v>1</v>
       </c>
-      <c r="Y33" s="40" t="str">
+      <c r="Y33" s="40" t="n">
         <f aca="false">IF(OR(F33="",G33=""),"",IF(F33&gt;G33,1,IF(F33&lt;G33,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA33" s="40" t="n">
         <f aca="false">COUNTIF(AN32:AN35,CONCATENATE("&gt;=",AN33))</f>
@@ -36424,8 +36428,12 @@
         <f aca="false">AB41</f>
         <v>República de Corea</v>
       </c>
-      <c r="F34" s="64"/>
-      <c r="G34" s="65"/>
+      <c r="F34" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="65" t="n">
+        <v>2</v>
+      </c>
       <c r="H34" s="66" t="str">
         <f aca="false">AB39</f>
         <v>México</v>
@@ -36464,11 +36472,11 @@
       </c>
       <c r="S34" s="41" t="str">
         <f aca="false">IF(OR(F34="",G34=""),"",IF(F34&gt;G34,E34&amp;"_win",IF(F34&lt;G34,E34&amp;"_lose",E34&amp;"_draw")))</f>
-        <v/>
+        <v>República de Corea_lose</v>
       </c>
       <c r="T34" s="41" t="str">
         <f aca="false">IF(S34="","",IF(F34&lt;G34,H34&amp;"_win",IF(F34&gt;G34,H34&amp;"_lose",H34&amp;"_draw")))</f>
-        <v/>
+        <v>México_win</v>
       </c>
       <c r="U34" s="42" t="n">
         <f aca="false">IF(S34="",0,IF(VLOOKUP(E34,$AB$8:$AK$53,7,0)=VLOOKUP(H34,$AB$8:$AK$53,7,0),1,0))</f>
@@ -36486,9 +36494,9 @@
         <f aca="false">IF(OR(E34=my_team,H34=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y34" s="40" t="str">
+      <c r="Y34" s="40" t="n">
         <f aca="false">IF(OR(F34="",G34=""),"",IF(F34&gt;G34,1,IF(F34&lt;G34,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA34" s="40" t="n">
         <f aca="false">COUNTIF(AN32:AN35,CONCATENATE("&gt;=",AN34))</f>
@@ -36617,8 +36625,12 @@
         <f aca="false">AB44</f>
         <v>Bélgica</v>
       </c>
-      <c r="F35" s="64"/>
-      <c r="G35" s="65"/>
+      <c r="F35" s="64" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="65" t="n">
+        <v>2</v>
+      </c>
       <c r="H35" s="66" t="str">
         <f aca="false">AB46</f>
         <v>Túnez</v>
@@ -36657,11 +36669,11 @@
       </c>
       <c r="S35" s="41" t="str">
         <f aca="false">IF(OR(F35="",G35=""),"",IF(F35&gt;G35,E35&amp;"_win",IF(F35&lt;G35,E35&amp;"_lose",E35&amp;"_draw")))</f>
-        <v/>
+        <v>Bélgica_win</v>
       </c>
       <c r="T35" s="41" t="str">
         <f aca="false">IF(S35="","",IF(F35&lt;G35,H35&amp;"_win",IF(F35&gt;G35,H35&amp;"_lose",H35&amp;"_draw")))</f>
-        <v/>
+        <v>Túnez_lose</v>
       </c>
       <c r="U35" s="42" t="n">
         <f aca="false">IF(S35="",0,IF(VLOOKUP(E35,$AB$8:$AK$53,7,0)=VLOOKUP(H35,$AB$8:$AK$53,7,0),1,0))</f>
@@ -36679,9 +36691,9 @@
         <f aca="false">IF(OR(E35=my_team,H35=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y35" s="40" t="str">
+      <c r="Y35" s="40" t="n">
         <f aca="false">IF(OR(F35="",G35=""),"",IF(F35&gt;G35,1,IF(F35&lt;G35,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA35" s="40" t="n">
         <f aca="false">COUNTIF(AN32:AN35,CONCATENATE("&gt;=",AN35))</f>
@@ -36813,8 +36825,12 @@
         <f aca="false">AB47</f>
         <v>Inglaterra</v>
       </c>
-      <c r="F36" s="64"/>
-      <c r="G36" s="65"/>
+      <c r="F36" s="64" t="n">
+        <v>6</v>
+      </c>
+      <c r="G36" s="65" t="n">
+        <v>1</v>
+      </c>
       <c r="H36" s="66" t="str">
         <f aca="false">AB45</f>
         <v>Panamá</v>
@@ -36853,11 +36869,11 @@
       </c>
       <c r="S36" s="41" t="str">
         <f aca="false">IF(OR(F36="",G36=""),"",IF(F36&gt;G36,E36&amp;"_win",IF(F36&lt;G36,E36&amp;"_lose",E36&amp;"_draw")))</f>
-        <v/>
+        <v>Inglaterra_win</v>
       </c>
       <c r="T36" s="41" t="str">
         <f aca="false">IF(S36="","",IF(F36&lt;G36,H36&amp;"_win",IF(F36&gt;G36,H36&amp;"_lose",H36&amp;"_draw")))</f>
-        <v/>
+        <v>Panamá_lose</v>
       </c>
       <c r="U36" s="42" t="n">
         <f aca="false">IF(S36="",0,IF(VLOOKUP(E36,$AB$8:$AK$53,7,0)=VLOOKUP(H36,$AB$8:$AK$53,7,0),1,0))</f>
@@ -36875,9 +36891,9 @@
         <f aca="false">IF(OR(E36=my_team,H36=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y36" s="40" t="str">
+      <c r="Y36" s="40" t="n">
         <f aca="false">IF(OR(F36="",G36=""),"",IF(F36&gt;G36,1,IF(F36&lt;G36,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AC36" s="40" t="n">
         <f aca="false">MAX(AC32:AC35)-MIN(AC32:AC35)+1</f>
@@ -36986,8 +37002,12 @@
         <f aca="false">AB50</f>
         <v>Polonia</v>
       </c>
-      <c r="F37" s="64"/>
-      <c r="G37" s="65"/>
+      <c r="F37" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="65" t="n">
+        <v>3</v>
+      </c>
       <c r="H37" s="66" t="str">
         <f aca="false">AB52</f>
         <v>Colombia</v>
@@ -36998,11 +37018,11 @@
       </c>
       <c r="S37" s="41" t="str">
         <f aca="false">IF(OR(F37="",G37=""),"",IF(F37&gt;G37,E37&amp;"_win",IF(F37&lt;G37,E37&amp;"_lose",E37&amp;"_draw")))</f>
-        <v/>
+        <v>Polonia_lose</v>
       </c>
       <c r="T37" s="41" t="str">
         <f aca="false">IF(S37="","",IF(F37&lt;G37,H37&amp;"_win",IF(F37&gt;G37,H37&amp;"_lose",H37&amp;"_draw")))</f>
-        <v/>
+        <v>Colombia_win</v>
       </c>
       <c r="U37" s="42" t="n">
         <f aca="false">IF(S37="",0,IF(VLOOKUP(E37,$AB$8:$AK$53,7,0)=VLOOKUP(H37,$AB$8:$AK$53,7,0),1,0))</f>
@@ -37020,9 +37040,9 @@
         <f aca="false">IF(OR(E37=my_team,H37=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y37" s="40" t="str">
+      <c r="Y37" s="40" t="n">
         <f aca="false">IF(OR(F37="",G37=""),"",IF(F37&gt;G37,1,IF(F37&lt;G37,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AH37" s="40" t="n">
         <f aca="false">MIN(AH32:AH35)</f>
@@ -37081,8 +37101,12 @@
         <f aca="false">AB53</f>
         <v>Japón</v>
       </c>
-      <c r="F38" s="64"/>
-      <c r="G38" s="65"/>
+      <c r="F38" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" s="65" t="n">
+        <v>2</v>
+      </c>
       <c r="H38" s="66" t="str">
         <f aca="false">AB51</f>
         <v>Senegal</v>
@@ -37121,35 +37145,35 @@
       </c>
       <c r="S38" s="41" t="str">
         <f aca="false">IF(OR(F38="",G38=""),"",IF(F38&gt;G38,E38&amp;"_win",IF(F38&lt;G38,E38&amp;"_lose",E38&amp;"_draw")))</f>
-        <v/>
+        <v>Japón_draw</v>
       </c>
       <c r="T38" s="41" t="str">
         <f aca="false">IF(S38="","",IF(F38&lt;G38,H38&amp;"_win",IF(F38&gt;G38,H38&amp;"_lose",H38&amp;"_draw")))</f>
-        <v/>
+        <v>Senegal_draw</v>
       </c>
       <c r="U38" s="42" t="n">
         <f aca="false">IF(S38="",0,IF(VLOOKUP(E38,$AB$8:$AK$53,7,0)=VLOOKUP(H38,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V38" s="40" t="n">
         <f aca="false">U38*F38</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W38" s="40" t="n">
         <f aca="false">U38*G38</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X38" s="40" t="n">
         <f aca="false">IF(OR(E38=my_team,H38=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y38" s="40" t="str">
+      <c r="Y38" s="40" t="n">
         <f aca="false">IF(OR(F38="",G38=""),"",IF(F38&gt;G38,1,IF(F38&lt;G38,-1,0)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AA38" s="40" t="n">
         <f aca="false">COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN38))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB38" s="42" t="str">
         <f aca="false">VLOOKUP("Germany",T,lang,0)</f>
@@ -37157,7 +37181,7 @@
       </c>
       <c r="AC38" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB38 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD38" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB38 &amp; "_draw")</f>
@@ -37169,31 +37193,31 @@
       </c>
       <c r="AF38" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB38,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB38,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG38" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB38,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB38,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH38" s="40" t="n">
         <f aca="false">(AF38-AG38)*100+AK38*10000+AF38</f>
-        <v>-100</v>
+        <v>30002</v>
       </c>
       <c r="AI38" s="40" t="n">
         <f aca="false">AF38-AG38</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ38" s="40" t="n">
         <f aca="false">(AI38-AI43)/AI42</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AK38" s="40" t="n">
         <f aca="false">AC38*3+AD38</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL38" s="40" t="n">
         <f aca="false">AP38/AP42*1000+AQ38/AQ42*100+AT38/AT42*10+AR38/AR42</f>
-        <v>0</v>
+        <v>504</v>
       </c>
       <c r="AM38" s="40" t="n">
         <f aca="false">VLOOKUP(AB38,db_fifarank,2,0)/2000000</f>
@@ -37201,7 +37225,7 @@
       </c>
       <c r="AN38" s="42" t="n">
         <f aca="false">1000*AK38/AK42+100*AJ38+10*AF38/AF42+1*AL38/AL42+AM38</f>
-        <v>0.000801</v>
+        <v>476.231022222347</v>
       </c>
       <c r="AO38" s="43" t="str">
         <f aca="false">IF(SUM(AC38:AE41)=12,J39,INDEX(T,80,lang))</f>
@@ -37209,7 +37233,7 @@
       </c>
       <c r="AP38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB38&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB38&amp;"_win")*($U$7:$U$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB38&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB38&amp;"_draw")*($U$7:$U$54))</f>
@@ -37217,15 +37241,15 @@
       </c>
       <c r="AR38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB38)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB38)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB38)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB38)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT38" s="44" t="n">
         <f aca="false">AR38-AS38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY38" s="78" t="n">
         <v>56</v>
@@ -37283,11 +37307,11 @@
       </c>
       <c r="K39" s="72" t="n">
         <f aca="false">L39+M39+N39</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L39" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA38:AK41,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M39" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA38:AK41,4,0)</f>
@@ -37299,11 +37323,11 @@
       </c>
       <c r="O39" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(1,AA38:AK41,7,0)</f>
-        <v>1 - 0</v>
+        <v>3 - 1</v>
       </c>
       <c r="P39" s="73" t="n">
         <f aca="false">L39*3+M39</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R39" s="40" t="n">
         <f aca="false">DATE(2018,6,25)+TIME(3,0,0)+gmt_delta</f>
@@ -37347,7 +37371,7 @@
       </c>
       <c r="AC39" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB39 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD39" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB39 &amp; "_draw")</f>
@@ -37359,27 +37383,27 @@
       </c>
       <c r="AF39" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB39,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB39,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG39" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB39,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB39,$F$7:$F$54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH39" s="40" t="n">
         <f aca="false">(AF39-AG39)*100+AK39*10000+AF39</f>
-        <v>30101</v>
+        <v>60203</v>
       </c>
       <c r="AI39" s="40" t="n">
         <f aca="false">AF39-AG39</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ39" s="40" t="n">
         <f aca="false">(AI39-AI43)/AI42</f>
-        <v>0.666666666666667</v>
+        <v>0.8</v>
       </c>
       <c r="AK39" s="40" t="n">
         <f aca="false">AC39*3+AD39</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL39" s="40" t="n">
         <f aca="false">AP39/AP42*1000+AQ39/AQ42*100+AT39/AT42*10+AR39/AR42</f>
@@ -37391,7 +37415,7 @@
       </c>
       <c r="AN39" s="42" t="n">
         <f aca="false">1000*AK39/AK42+100*AJ39+10*AF39/AF42+1*AL39/AL42+AM39</f>
-        <v>821.667182666667</v>
+        <v>947.143373142857</v>
       </c>
       <c r="AO39" s="43" t="str">
         <f aca="false">IF(SUM(AC38:AE41)=12,J40,INDEX(T,81,lang))</f>
@@ -37465,11 +37489,11 @@
       </c>
       <c r="J40" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA38:AK41,2,0)</f>
-        <v>Suecia</v>
+        <v>Alemania</v>
       </c>
       <c r="K40" s="76" t="n">
         <f aca="false">L40+M40+N40</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L40" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA38:AK41,3,0)</f>
@@ -37481,11 +37505,11 @@
       </c>
       <c r="N40" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA38:AK41,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O40" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(2,AA38:AK41,7,0)</f>
-        <v>1 - 0</v>
+        <v>2 - 2</v>
       </c>
       <c r="P40" s="77" t="n">
         <f aca="false">L40*3+M40</f>
@@ -37525,7 +37549,7 @@
       </c>
       <c r="AA40" s="40" t="n">
         <f aca="false">COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN40))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB40" s="42" t="str">
         <f aca="false">VLOOKUP("Sweden",T,lang,0)</f>
@@ -37541,27 +37565,27 @@
       </c>
       <c r="AE40" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB40 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF40" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB40,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB40,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG40" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB40,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB40,$F$7:$F$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH40" s="40" t="n">
         <f aca="false">(AF40-AG40)*100+AK40*10000+AF40</f>
-        <v>30101</v>
+        <v>30002</v>
       </c>
       <c r="AI40" s="40" t="n">
         <f aca="false">AF40-AG40</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ40" s="40" t="n">
         <f aca="false">(AI40-AI43)/AI42</f>
-        <v>0.666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="AK40" s="40" t="n">
         <f aca="false">AC40*3+AD40</f>
@@ -37569,7 +37593,7 @@
       </c>
       <c r="AL40" s="40" t="n">
         <f aca="false">AP40/AP42*1000+AQ40/AQ42*100+AT40/AT42*10+AR40/AR42</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AM40" s="40" t="n">
         <f aca="false">VLOOKUP(AB40,db_fifarank,2,0)/2000000</f>
@@ -37577,7 +37601,7 @@
       </c>
       <c r="AN40" s="42" t="n">
         <f aca="false">1000*AK40/AK42+100*AJ40+10*AF40/AF42+1*AL40/AL42+AM40</f>
-        <v>821.667165666667</v>
+        <v>475.232688726284</v>
       </c>
       <c r="AP40" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB40&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB40&amp;"_win")*($U$7:$U$54))</f>
@@ -37589,15 +37613,15 @@
       </c>
       <c r="AR40" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB40)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB40)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS40" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB40)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB40)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT40" s="44" t="n">
         <f aca="false">AR40-AS40</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37628,15 +37652,15 @@
       </c>
       <c r="J41" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA38:AK41,2,0)</f>
-        <v>Alemania</v>
+        <v>Suecia</v>
       </c>
       <c r="K41" s="76" t="n">
         <f aca="false">L41+M41+N41</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L41" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA38:AK41,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA38:AK41,4,0)</f>
@@ -37648,11 +37672,11 @@
       </c>
       <c r="O41" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(3,AA38:AK41,7,0)</f>
-        <v>0 - 1</v>
+        <v>2 - 2</v>
       </c>
       <c r="P41" s="77" t="n">
         <f aca="false">L41*3+M41</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R41" s="40" t="n">
         <f aca="false">DATE(2018,6,25)+TIME(7,0,0)+gmt_delta</f>
@@ -37704,23 +37728,23 @@
       </c>
       <c r="AE41" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB41 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF41" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB41,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB41,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG41" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB41,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB41,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH41" s="40" t="n">
         <f aca="false">(AF41-AG41)*100+AK41*10000+AF41</f>
-        <v>-100</v>
+        <v>-199</v>
       </c>
       <c r="AI41" s="40" t="n">
         <f aca="false">AF41-AG41</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AJ41" s="40" t="n">
         <f aca="false">(AI41-AI43)/AI42</f>
@@ -37740,7 +37764,7 @@
       </c>
       <c r="AN41" s="42" t="n">
         <f aca="false">1000*AK41/AK42+100*AJ41+10*AF41/AF42+1*AL41/AL42+AM41</f>
-        <v>0.000285</v>
+        <v>3.33361833333333</v>
       </c>
       <c r="AP41" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB41&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB41&amp;"_win")*($U$7:$U$54))</f>
@@ -37812,7 +37836,7 @@
       </c>
       <c r="K42" s="88" t="n">
         <f aca="false">L42+M42+N42</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L42" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA38:AK41,3,0)</f>
@@ -37824,11 +37848,11 @@
       </c>
       <c r="N42" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA38:AK41,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O42" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(4,AA38:AK41,7,0)</f>
-        <v>0 - 1</v>
+        <v>1 - 3</v>
       </c>
       <c r="P42" s="89" t="n">
         <f aca="false">L42*3+M42</f>
@@ -37868,7 +37892,7 @@
       </c>
       <c r="AC42" s="40" t="n">
         <f aca="false">MAX(AC38:AC41)-MIN(AC38:AC41)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD42" s="40" t="n">
         <f aca="false">MAX(AD38:AD41)-MIN(AD38:AD41)+1</f>
@@ -37876,35 +37900,35 @@
       </c>
       <c r="AE42" s="40" t="n">
         <f aca="false">MAX(AE38:AE41)-MIN(AE38:AE41)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF42" s="40" t="n">
         <f aca="false">MAX(AF38:AF41)-MIN(AF38:AF41)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG42" s="40" t="n">
         <f aca="false">MAX(AG38:AG41)-MIN(AG38:AG41)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH42" s="40" t="n">
         <f aca="false">MAX(AH38:AH41)-AH43+1</f>
-        <v>30202</v>
+        <v>60403</v>
       </c>
       <c r="AI42" s="40" t="n">
         <f aca="false">MAX(AI38:AI41)-AI43+1</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AK42" s="40" t="n">
         <f aca="false">MAX(AK38:AK41)-MIN(AK38:AK41)+1</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AL42" s="40" t="n">
         <f aca="false">MAX(AL38:AL41)-MIN(AL38:AL41)+1</f>
-        <v>1</v>
+        <v>508</v>
       </c>
       <c r="AP42" s="40" t="n">
         <f aca="false">MAX(AP38:AP41)-MIN(AP38:AP41)+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ42" s="40" t="n">
         <f aca="false">MAX(AQ38:AQ41)-MIN(AQ38:AQ41)+1</f>
@@ -37912,15 +37936,15 @@
       </c>
       <c r="AR42" s="40" t="n">
         <f aca="false">MAX(AR38:AR41)-MIN(AR38:AR41)+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS42" s="40" t="n">
         <f aca="false">MAX(AS38:AS41)-MIN(AS38:AS41)+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT42" s="40" t="n">
         <f aca="false">MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BJ42" s="100"/>
       <c r="BK42" s="100"/>
@@ -37994,11 +38018,11 @@
       </c>
       <c r="AH43" s="40" t="n">
         <f aca="false">MIN(AH38:AH41)</f>
-        <v>-100</v>
+        <v>-199</v>
       </c>
       <c r="AI43" s="40" t="n">
         <f aca="false">MIN(AI38:AI41)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AY43" s="102"/>
     </row>
@@ -38098,7 +38122,7 @@
       </c>
       <c r="AC44" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD44" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_draw")</f>
@@ -38110,27 +38134,27 @@
       </c>
       <c r="AF44" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB44,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB44,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AG44" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB44,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB44,$F$7:$F$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH44" s="40" t="n">
         <f aca="false">(AF44-AG44)*100+AK44*10000+AF44</f>
-        <v>30303</v>
+        <v>60608</v>
       </c>
       <c r="AI44" s="40" t="n">
         <f aca="false">AF44-AG44</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ44" s="40" t="n">
         <f aca="false">(AI44-AI49)/AI48</f>
-        <v>0.857142857142857</v>
+        <v>0.933333333333333</v>
       </c>
       <c r="AK44" s="40" t="n">
         <f aca="false">AC44*3+AD44</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL44" s="40" t="n">
         <f aca="false">AP44/AP48*1000+AQ44/AQ48*100+AT44/AT48*10+AR44/AR48</f>
@@ -38142,7 +38166,7 @@
       </c>
       <c r="AN44" s="42" t="n">
         <f aca="false">1000*AK44/AK48+100*AJ44+10*AF44/AF48+1*AL44/AL48+AM44</f>
-        <v>843.214948214286</v>
+        <v>960.476852976191</v>
       </c>
       <c r="AO44" s="43" t="str">
         <f aca="false">IF(SUM(AC44:AE47)=12,J45,INDEX(T,82,lang))</f>
@@ -38201,11 +38225,11 @@
       </c>
       <c r="K45" s="72" t="n">
         <f aca="false">L45+M45+N45</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L45" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA44:AK47,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M45" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA44:AK47,4,0)</f>
@@ -38217,11 +38241,11 @@
       </c>
       <c r="O45" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(1,AA44:AK47,7,0)</f>
-        <v>3 - 0</v>
+        <v>8 - 2</v>
       </c>
       <c r="P45" s="73" t="n">
         <f aca="false">L45*3+M45</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R45" s="40" t="n">
         <f aca="false">DATE(2018,6,26)+TIME(7,0,0)+gmt_delta</f>
@@ -38273,23 +38297,23 @@
       </c>
       <c r="AE45" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB45 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF45" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB45,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB45,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG45" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB45,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB45,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="AH45" s="40" t="n">
         <f aca="false">(AF45-AG45)*100+AK45*10000+AF45</f>
-        <v>-300</v>
+        <v>-799</v>
       </c>
       <c r="AI45" s="40" t="n">
         <f aca="false">AF45-AG45</f>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AJ45" s="40" t="n">
         <f aca="false">(AI45-AI49)/AI48</f>
@@ -38309,7 +38333,7 @@
       </c>
       <c r="AN45" s="42" t="n">
         <f aca="false">1000*AK45/AK48+100*AJ45+10*AF45/AF48+1*AL45/AL48+AM45</f>
-        <v>0.0003105</v>
+        <v>1.2503105</v>
       </c>
       <c r="AO45" s="43" t="str">
         <f aca="false">IF(SUM(AC44:AE47)=12,J46,INDEX(T,83,lang))</f>
@@ -38368,11 +38392,11 @@
       </c>
       <c r="K46" s="76" t="n">
         <f aca="false">L46+M46+N46</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L46" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA44:AK47,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M46" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA44:AK47,4,0)</f>
@@ -38384,11 +38408,11 @@
       </c>
       <c r="O46" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(2,AA44:AK47,7,0)</f>
-        <v>2 - 1</v>
+        <v>8 - 2</v>
       </c>
       <c r="P46" s="77" t="n">
         <f aca="false">L46*3+M46</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R46" s="40" t="n">
         <f aca="false">DATE(2018,6,26)+TIME(7,0,0)+gmt_delta</f>
@@ -38440,27 +38464,27 @@
       </c>
       <c r="AE46" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF46" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB46,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB46,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG46" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB46,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB46,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AH46" s="40" t="n">
         <f aca="false">(AF46-AG46)*100+AK46*10000+AF46</f>
-        <v>-99</v>
+        <v>-397</v>
       </c>
       <c r="AI46" s="40" t="n">
         <f aca="false">AF46-AG46</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="AJ46" s="40" t="n">
         <f aca="false">(AI46-AI49)/AI48</f>
-        <v>0.285714285714286</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="AK46" s="40" t="n">
         <f aca="false">AC46*3+AD46</f>
@@ -38476,7 +38500,7 @@
       </c>
       <c r="AN46" s="42" t="n">
         <f aca="false">1000*AK46/AK48+100*AJ46+10*AF46/AF48+1*AL46/AL48+AM46</f>
-        <v>31.0718475714286</v>
+        <v>30.4170856666667</v>
       </c>
       <c r="AP46" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB46&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB46&amp;"_win")*($U$7:$U$54))</f>
@@ -38537,7 +38561,7 @@
       </c>
       <c r="K47" s="76" t="n">
         <f aca="false">L47+M47+N47</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L47" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA44:AK47,3,0)</f>
@@ -38549,11 +38573,11 @@
       </c>
       <c r="N47" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA44:AK47,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O47" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(3,AA44:AK47,7,0)</f>
-        <v>1 - 2</v>
+        <v>3 - 7</v>
       </c>
       <c r="P47" s="77" t="n">
         <f aca="false">L47*3+M47</f>
@@ -38601,7 +38625,7 @@
       </c>
       <c r="AC47" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB47 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD47" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB47 &amp; "_draw")</f>
@@ -38613,27 +38637,27 @@
       </c>
       <c r="AF47" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB47,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB47,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AG47" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB47,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB47,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH47" s="40" t="n">
         <f aca="false">(AF47-AG47)*100+AK47*10000+AF47</f>
-        <v>30102</v>
+        <v>60608</v>
       </c>
       <c r="AI47" s="40" t="n">
         <f aca="false">AF47-AG47</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AJ47" s="40" t="n">
         <f aca="false">(AI47-AI49)/AI48</f>
-        <v>0.571428571428571</v>
+        <v>0.933333333333333</v>
       </c>
       <c r="AK47" s="40" t="n">
         <f aca="false">AC47*3+AD47</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL47" s="40" t="n">
         <f aca="false">AP47/AP48*1000+AQ47/AQ48*100+AT47/AT48*10+AR47/AR48</f>
@@ -38645,7 +38669,7 @@
       </c>
       <c r="AN47" s="42" t="n">
         <f aca="false">1000*AK47/AK48+100*AJ47+10*AF47/AF48+1*AL47/AL48+AM47</f>
-        <v>812.143380642857</v>
+        <v>960.47671397619</v>
       </c>
       <c r="AP47" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB47&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB47&amp;"_win")*($U$7:$U$54))</f>
@@ -38704,7 +38728,7 @@
       </c>
       <c r="K48" s="88" t="n">
         <f aca="false">L48+M48+N48</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L48" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA44:AK47,3,0)</f>
@@ -38716,11 +38740,11 @@
       </c>
       <c r="N48" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA44:AK47,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O48" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(4,AA44:AK47,7,0)</f>
-        <v>0 - 3</v>
+        <v>1 - 9</v>
       </c>
       <c r="P48" s="89" t="n">
         <f aca="false">L48*3+M48</f>
@@ -38760,7 +38784,7 @@
       </c>
       <c r="AC48" s="40" t="n">
         <f aca="false">MAX(AC44:AC47)-MIN(AC44:AC47)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD48" s="40" t="n">
         <f aca="false">MAX(AD44:AD47)-MIN(AD44:AD47)+1</f>
@@ -38768,27 +38792,27 @@
       </c>
       <c r="AE48" s="40" t="n">
         <f aca="false">MAX(AE44:AE47)-MIN(AE44:AE47)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF48" s="40" t="n">
         <f aca="false">MAX(AF44:AF47)-MIN(AF44:AF47)+1</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AG48" s="40" t="n">
         <f aca="false">MAX(AG44:AG47)-MIN(AG44:AG47)+1</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AH48" s="40" t="n">
         <f aca="false">MAX(AH44:AH47)-AH49+1</f>
-        <v>30604</v>
+        <v>61408</v>
       </c>
       <c r="AI48" s="40" t="n">
         <f aca="false">MAX(AI44:AI47)-AI49+1</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="AK48" s="40" t="n">
         <f aca="false">MAX(AK44:AK47)-MIN(AK44:AK47)+1</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AL48" s="40" t="n">
         <f aca="false">MAX(AL44:AL47)-MIN(AL44:AL47)+1</f>
@@ -38879,11 +38903,11 @@
       </c>
       <c r="AH49" s="40" t="n">
         <f aca="false">MIN(AH44:AH47)</f>
-        <v>-300</v>
+        <v>-799</v>
       </c>
       <c r="AI49" s="40" t="n">
         <f aca="false">MIN(AI44:AI47)</f>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AY49" s="103"/>
       <c r="AZ49" s="103"/>
@@ -38978,7 +39002,7 @@
       </c>
       <c r="AA50" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN50))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB50" s="42" t="str">
         <f aca="false">VLOOKUP("Poland",T,lang,0)</f>
@@ -38994,7 +39018,7 @@
       </c>
       <c r="AE50" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF50" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB50,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB50,$G$7:$G$54)</f>
@@ -39002,15 +39026,15 @@
       </c>
       <c r="AG50" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB50,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB50,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AH50" s="40" t="n">
         <f aca="false">(AF50-AG50)*100+AK50*10000+AF50</f>
-        <v>-99</v>
+        <v>-399</v>
       </c>
       <c r="AI50" s="40" t="n">
         <f aca="false">AF50-AG50</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="AJ50" s="40" t="n">
         <f aca="false">(AI50-AI55)/AI54</f>
@@ -39030,7 +39054,7 @@
       </c>
       <c r="AN50" s="42" t="n">
         <f aca="false">1000*AK50/AK54+100*AJ50+10*AF50/AF54+1*AL50/AL54+AM50</f>
-        <v>5.0006045</v>
+        <v>2.5006045</v>
       </c>
       <c r="AO50" s="43" t="str">
         <f aca="false">IF(SUM(AC50:AE53)=12,J51,INDEX(T,84,lang))</f>
@@ -39093,7 +39117,7 @@
       </c>
       <c r="K51" s="72" t="n">
         <f aca="false">L51+M51+N51</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L51" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA50:AK53,3,0)</f>
@@ -39101,7 +39125,7 @@
       </c>
       <c r="M51" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA50:AK53,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA50:AK53,5,0)</f>
@@ -39109,11 +39133,11 @@
       </c>
       <c r="O51" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(1,AA50:AK53,7,0)</f>
-        <v>2 - 1</v>
+        <v>4 - 3</v>
       </c>
       <c r="P51" s="73" t="n">
         <f aca="false">L51*3+M51</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R51" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(7,0,0)+gmt_delta</f>
@@ -39161,7 +39185,7 @@
       </c>
       <c r="AD51" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB51 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE51" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB51 &amp; "_lose")</f>
@@ -39169,15 +39193,15 @@
       </c>
       <c r="AF51" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB51,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB51,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG51" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB51,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB51,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH51" s="40" t="n">
         <f aca="false">(AF51-AG51)*100+AK51*10000+AF51</f>
-        <v>30102</v>
+        <v>40104</v>
       </c>
       <c r="AI51" s="40" t="n">
         <f aca="false">AF51-AG51</f>
@@ -39185,15 +39209,15 @@
       </c>
       <c r="AJ51" s="40" t="n">
         <f aca="false">(AI51-AI55)/AI54</f>
-        <v>0.666666666666667</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="AK51" s="40" t="n">
         <f aca="false">AC51*3+AD51</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL51" s="40" t="n">
         <f aca="false">AP51/AP54*1000+AQ51/AQ54*100+AT51/AT54*10+AR51/AR54</f>
-        <v>0</v>
+        <v>50.6666666666667</v>
       </c>
       <c r="AM51" s="40" t="n">
         <f aca="false">VLOOKUP(AB51,db_fifarank,2,0)/2000000</f>
@@ -39201,7 +39225,7 @@
       </c>
       <c r="AN51" s="42" t="n">
         <f aca="false">1000*AK51/AK54+100*AJ51+10*AF51/AF54+1*AL51/AL54+AM51</f>
-        <v>826.667108666667</v>
+        <v>882.409658589862</v>
       </c>
       <c r="AO51" s="43" t="str">
         <f aca="false">IF(SUM(AC50:AE53)=12,J52,INDEX(T,85,lang))</f>
@@ -39213,15 +39237,15 @@
       </c>
       <c r="AQ51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB51&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB51&amp;"_draw")*($U$7:$U$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB51)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB51)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB51)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB51)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT51" s="44" t="n">
         <f aca="false">AR51-AS51</f>
@@ -39264,7 +39288,7 @@
       </c>
       <c r="K52" s="76" t="n">
         <f aca="false">L52+M52+N52</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,3,0)</f>
@@ -39272,7 +39296,7 @@
       </c>
       <c r="M52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,5,0)</f>
@@ -39280,11 +39304,11 @@
       </c>
       <c r="O52" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(2,AA50:AK53,7,0)</f>
-        <v>2 - 1</v>
+        <v>4 - 3</v>
       </c>
       <c r="P52" s="77" t="n">
         <f aca="false">L52*3+M52</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R52" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(7,0,0)+gmt_delta</f>
@@ -39320,7 +39344,7 @@
       </c>
       <c r="AA52" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN52))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB52" s="42" t="str">
         <f aca="false">VLOOKUP("Colombia",T,lang,0)</f>
@@ -39328,7 +39352,7 @@
       </c>
       <c r="AC52" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD52" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_draw")</f>
@@ -39340,7 +39364,7 @@
       </c>
       <c r="AF52" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB52,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB52,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG52" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB52,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB52,$F$7:$F$54)</f>
@@ -39348,19 +39372,19 @@
       </c>
       <c r="AH52" s="40" t="n">
         <f aca="false">(AF52-AG52)*100+AK52*10000+AF52</f>
-        <v>-99</v>
+        <v>30204</v>
       </c>
       <c r="AI52" s="40" t="n">
         <f aca="false">AF52-AG52</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AJ52" s="40" t="n">
         <f aca="false">(AI52-AI55)/AI54</f>
-        <v>0</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="AK52" s="40" t="n">
         <f aca="false">AC52*3+AD52</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL52" s="40" t="n">
         <f aca="false">AP52/AP54*1000+AQ52/AQ54*100+AT52/AT54*10+AR52/AR54</f>
@@ -39372,7 +39396,7 @@
       </c>
       <c r="AN52" s="42" t="n">
         <f aca="false">1000*AK52/AK54+100*AJ52+10*AF52/AF54+1*AL52/AL54+AM52</f>
-        <v>5.000539</v>
+        <v>695.714824714286</v>
       </c>
       <c r="AP52" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB52&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB52&amp;"_win")*($U$7:$U$54))</f>
@@ -39427,15 +39451,15 @@
       </c>
       <c r="J53" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA50:AK53,2,0)</f>
-        <v>Polonia</v>
+        <v>Colombia</v>
       </c>
       <c r="K53" s="76" t="n">
         <f aca="false">L53+M53+N53</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L53" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA50:AK53,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA50:AK53,4,0)</f>
@@ -39447,11 +39471,11 @@
       </c>
       <c r="O53" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(3,AA50:AK53,7,0)</f>
-        <v>1 - 2</v>
+        <v>4 - 2</v>
       </c>
       <c r="P53" s="77" t="n">
         <f aca="false">L53*3+M53</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R53" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -39499,7 +39523,7 @@
       </c>
       <c r="AD53" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB53 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE53" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB53 &amp; "_lose")</f>
@@ -39507,15 +39531,15 @@
       </c>
       <c r="AF53" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB53,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB53,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG53" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB53,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB53,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH53" s="40" t="n">
         <f aca="false">(AF53-AG53)*100+AK53*10000+AF53</f>
-        <v>30102</v>
+        <v>40104</v>
       </c>
       <c r="AI53" s="40" t="n">
         <f aca="false">AF53-AG53</f>
@@ -39523,15 +39547,15 @@
       </c>
       <c r="AJ53" s="40" t="n">
         <f aca="false">(AI53-AI55)/AI54</f>
-        <v>0.666666666666667</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="AK53" s="40" t="n">
         <f aca="false">AC53*3+AD53</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL53" s="40" t="n">
         <f aca="false">AP53/AP54*1000+AQ53/AQ54*100+AT53/AT54*10+AR53/AR54</f>
-        <v>0</v>
+        <v>50.6666666666667</v>
       </c>
       <c r="AM53" s="40" t="n">
         <f aca="false">VLOOKUP(AB53,db_fifarank,2,0)/2000000</f>
@@ -39539,7 +39563,7 @@
       </c>
       <c r="AN53" s="42" t="n">
         <f aca="false">1000*AK53/AK54+100*AJ53+10*AF53/AF54+1*AL53/AL54+AM53</f>
-        <v>826.666966666667</v>
+        <v>882.409516589862</v>
       </c>
       <c r="AP53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB53&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_win")*($U$7:$U$54))</f>
@@ -39547,15 +39571,15 @@
       </c>
       <c r="AQ53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB53&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_draw")*($U$7:$U$54))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB53)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB53)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB53)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB53)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT53" s="44" t="n">
         <f aca="false">AR53-AS53</f>
@@ -39590,11 +39614,11 @@
       </c>
       <c r="J54" s="87" t="str">
         <f aca="false">VLOOKUP(4,AA50:AK53,2,0)</f>
-        <v>Colombia</v>
+        <v>Polonia</v>
       </c>
       <c r="K54" s="88" t="n">
         <f aca="false">L54+M54+N54</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,3,0)</f>
@@ -39606,11 +39630,11 @@
       </c>
       <c r="N54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O54" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(4,AA50:AK53,7,0)</f>
-        <v>1 - 2</v>
+        <v>1 - 5</v>
       </c>
       <c r="P54" s="89" t="n">
         <f aca="false">L54*3+M54</f>
@@ -39654,35 +39678,35 @@
       </c>
       <c r="AD54" s="40" t="n">
         <f aca="false">MAX(AD50:AD53)-MIN(AD50:AD53)+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE54" s="40" t="n">
         <f aca="false">MAX(AE50:AE53)-MIN(AE50:AE53)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF54" s="40" t="n">
         <f aca="false">MAX(AF50:AF53)-MIN(AF50:AF53)+1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG54" s="40" t="n">
         <f aca="false">MAX(AG50:AG53)-MIN(AG50:AG53)+1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH54" s="40" t="n">
         <f aca="false">MAX(AH50:AH53)-AH55+1</f>
-        <v>30202</v>
+        <v>40504</v>
       </c>
       <c r="AI54" s="40" t="n">
         <f aca="false">MAX(AI50:AI53)-AI55+1</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AK54" s="40" t="n">
         <f aca="false">MAX(AK50:AK53)-MIN(AK50:AK53)+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL54" s="40" t="n">
         <f aca="false">MAX(AL50:AL53)-MIN(AL50:AL53)+1</f>
-        <v>1</v>
+        <v>51.6666666666667</v>
       </c>
       <c r="AP54" s="40" t="n">
         <f aca="false">MAX(AP50:AP53)-MIN(AP50:AP53)+1</f>
@@ -39690,15 +39714,15 @@
       </c>
       <c r="AQ54" s="40" t="n">
         <f aca="false">MAX(AQ50:AQ53)-MIN(AQ50:AQ53)+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR54" s="40" t="n">
         <f aca="false">MAX(AR50:AR53)-MIN(AR50:AR53)+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS54" s="40" t="n">
         <f aca="false">MAX(AS50:AS53)-MIN(AS50:AS53)+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT54" s="40" t="n">
         <f aca="false">MAX(AT50:AT53)-MIN(AT50:AT53)+1</f>
@@ -39723,11 +39747,11 @@
       <c r="P55" s="92"/>
       <c r="AH55" s="40" t="n">
         <f aca="false">MIN(AH50:AH53)</f>
-        <v>-99</v>
+        <v>-399</v>
       </c>
       <c r="AI55" s="40" t="n">
         <f aca="false">MIN(AI50:AI53)</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Resumen de partidos hasta el dia 27 de junio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -14014,9 +14014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487160</xdr:colOff>
+      <xdr:colOff>1486440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14030,7 +14030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1232280"/>
-          <a:ext cx="225360" cy="147960"/>
+          <a:ext cx="224640" cy="147240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14051,9 +14051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1487160</xdr:colOff>
+      <xdr:colOff>1486440</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14067,7 +14067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4276080"/>
-          <a:ext cx="225360" cy="147960"/>
+          <a:ext cx="224640" cy="147240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14088,9 +14088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14104,7 +14104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7324200"/>
-          <a:ext cx="225360" cy="147960"/>
+          <a:ext cx="224640" cy="147240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14125,9 +14125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14141,7 +14141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="1232280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14162,9 +14162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14178,7 +14178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4470840"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14199,9 +14199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14215,7 +14215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7519320"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14236,9 +14236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14252,7 +14252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1422720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14273,9 +14273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>249840</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14289,7 +14289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5461560" y="4280760"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14310,9 +14310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14326,7 +14326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7519320"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14347,9 +14347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>181080</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14363,7 +14363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1431720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14384,9 +14384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>185760</xdr:rowOff>
+      <xdr:rowOff>185040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14400,7 +14400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4484520"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14421,9 +14421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>176760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14437,7 +14437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7333560"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14458,9 +14458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14474,7 +14474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1613880"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14495,9 +14495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14511,7 +14511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4661280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14532,9 +14532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14548,7 +14548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7709760"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14569,9 +14569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14585,7 +14585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1613880"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14606,9 +14606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>176760</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14622,7 +14622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4856400"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14643,9 +14643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479600</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14659,7 +14659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="7899840"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14680,9 +14680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>176760</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14696,7 +14696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="7904520"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14717,9 +14717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14733,7 +14733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4661280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14754,9 +14754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14770,7 +14770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1799640"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,9 +14791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14807,7 +14807,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1804320"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14844,7 +14844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4847040"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14865,9 +14865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14881,7 +14881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7705080"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14902,9 +14902,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14918,7 +14918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1994760"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14939,9 +14939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14955,7 +14955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5042880"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14976,9 +14976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14992,7 +14992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8090280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15013,9 +15013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15029,7 +15029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1994760"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15050,9 +15050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15066,7 +15066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5228640"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15087,9 +15087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479600</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15103,7 +15103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8276040"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15124,9 +15124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15140,7 +15140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2184840"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15161,9 +15161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15177,7 +15177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="5042880"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15198,9 +15198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15214,7 +15214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8276040"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15235,9 +15235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15251,7 +15251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="2180160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15272,9 +15272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15288,7 +15288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5228640"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,9 +15309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479600</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15325,7 +15325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8085600"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15346,9 +15346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15362,7 +15362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2370600"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15383,9 +15383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15399,7 +15399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5423760"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15420,9 +15420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15436,7 +15436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="8467200"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15457,9 +15457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15473,7 +15473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="2375280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15494,9 +15494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479600</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15510,7 +15510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8662320"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15531,9 +15531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15547,7 +15547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5613840"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15568,9 +15568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15584,7 +15584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2565720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15605,9 +15605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15621,7 +15621,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5418360"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15642,9 +15642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15658,7 +15658,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455800" y="8656920"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15679,9 +15679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15695,7 +15695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2564640"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483200</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15732,7 +15732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926160" y="5612760"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15753,9 +15753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15769,7 +15769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8466480"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15806,7 +15806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2757960"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15827,9 +15827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15843,7 +15843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5800680"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15864,9 +15864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15880,7 +15880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="8849160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15901,9 +15901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>197640</xdr:colOff>
+      <xdr:colOff>196920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15917,7 +15917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481720" y="2753280"/>
-          <a:ext cx="149400" cy="149400"/>
+          <a:ext cx="148680" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15938,9 +15938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>192960</xdr:colOff>
+      <xdr:colOff>192240</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15954,7 +15954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5477040" y="5991120"/>
-          <a:ext cx="149400" cy="149400"/>
+          <a:ext cx="148680" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15975,9 +15975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1440720</xdr:colOff>
+      <xdr:colOff>1440000</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15991,7 +15991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956760" y="9039240"/>
-          <a:ext cx="149400" cy="149400"/>
+          <a:ext cx="148680" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16012,9 +16012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16028,7 +16028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2943720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16049,9 +16049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16065,7 +16065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="5800680"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16086,9 +16086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16102,7 +16102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9039240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,9 +16123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16139,7 +16139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="2943720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16160,9 +16160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16176,7 +16176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5991120"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16197,9 +16197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16213,7 +16213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="8849160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16234,9 +16234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16250,7 +16250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3134160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16271,9 +16271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16287,7 +16287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6182280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16308,9 +16308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16324,7 +16324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9229680"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16345,9 +16345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16361,7 +16361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3138840"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16382,9 +16382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16398,7 +16398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6372720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16419,9 +16419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16435,7 +16435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9420120"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16456,9 +16456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16472,7 +16472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3324240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16493,9 +16493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16509,7 +16509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6182280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16530,9 +16530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16546,7 +16546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9420120"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16567,9 +16567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16583,7 +16583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3324240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16604,9 +16604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16620,7 +16620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6372720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16641,9 +16641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16657,7 +16657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9229680"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16678,9 +16678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1463400</xdr:colOff>
+      <xdr:colOff>1462680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16694,7 +16694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="3514680"/>
-          <a:ext cx="176760" cy="149400"/>
+          <a:ext cx="176040" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16715,9 +16715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1463400</xdr:colOff>
+      <xdr:colOff>1462680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16731,7 +16731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="6563160"/>
-          <a:ext cx="176760" cy="149400"/>
+          <a:ext cx="176040" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16752,9 +16752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>215640</xdr:colOff>
+      <xdr:colOff>214920</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16768,7 +16768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5472360" y="9611280"/>
-          <a:ext cx="176760" cy="149400"/>
+          <a:ext cx="176040" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16789,9 +16789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16805,7 +16805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3514680"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16826,9 +16826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246960</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16842,7 +16842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6753240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16863,9 +16863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16879,7 +16879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9801720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16900,9 +16900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16916,7 +16916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3705120"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16937,9 +16937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16953,7 +16953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6563160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16974,9 +16974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16990,7 +16990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9801720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17011,9 +17011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17027,7 +17027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3896280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17048,9 +17048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17064,7 +17064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6943680"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17085,9 +17085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17101,7 +17101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9992160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17122,9 +17122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246960</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17138,7 +17138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3900960"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17159,9 +17159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246960</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17175,7 +17175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="7134120"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17196,9 +17196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17212,7 +17212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="10182240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17233,9 +17233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17249,7 +17249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="4091400"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17270,9 +17270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246960</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17286,7 +17286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6948360"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17307,9 +17307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17323,7 +17323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="10182240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17344,9 +17344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17360,7 +17360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="4086720"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17381,9 +17381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17397,7 +17397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="7134120"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17418,9 +17418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17434,7 +17434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9992160"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17455,9 +17455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246960</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17471,7 +17471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3709800"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17492,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17508,7 +17508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6753240"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17529,9 +17529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1479960</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17545,7 +17545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9611280"/>
-          <a:ext cx="222480" cy="149400"/>
+          <a:ext cx="221760" cy="148680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31724,8 +31724,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G49" activeCellId="0" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34079,7 +34079,7 @@
       </c>
       <c r="AZ18" s="79" t="str">
         <f aca="false">AO32</f>
-        <v>1E</v>
+        <v>Brasil</v>
       </c>
       <c r="BA18" s="80"/>
       <c r="BB18" s="81"/>
@@ -34182,7 +34182,7 @@
       <c r="AY19" s="78"/>
       <c r="AZ19" s="82" t="str">
         <f aca="false">AO39</f>
-        <v>2F</v>
+        <v>México</v>
       </c>
       <c r="BA19" s="83"/>
       <c r="BB19" s="84"/>
@@ -36435,7 +36435,7 @@
       </c>
       <c r="AC32" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB32 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD32" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB32 &amp; "_draw")</f>
@@ -36447,7 +36447,7 @@
       </c>
       <c r="AF32" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB32,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB32,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG32" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB32,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB32,$F$7:$F$54)</f>
@@ -36455,19 +36455,19 @@
       </c>
       <c r="AH32" s="40" t="n">
         <f aca="false">(AF32-AG32)*100+AK32*10000+AF32</f>
-        <v>40203</v>
+        <v>70405</v>
       </c>
       <c r="AI32" s="40" t="n">
         <f aca="false">AF32-AG32</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AJ32" s="40" t="n">
         <f aca="false">(AI32-AI37)/AI36</f>
-        <v>0.833333333333333</v>
+        <v>0.875</v>
       </c>
       <c r="AK32" s="40" t="n">
         <f aca="false">AC32*3+AD32</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AL32" s="40" t="n">
         <f aca="false">AP32/AP36*1000+AQ32/AQ36*100+AT32/AT36*10+AR32/AR36</f>
@@ -36479,11 +36479,11 @@
       </c>
       <c r="AN32" s="42" t="n">
         <f aca="false">1000*AK32/AK36+100*AJ32+10*AF32/AF36+1*AL32/AL36+AM32</f>
-        <v>890.834074833333</v>
+        <v>1097.5007415</v>
       </c>
       <c r="AO32" s="43" t="str">
         <f aca="false">IF(SUM(AC32:AE35)=12,J33,INDEX(T,78,lang))</f>
-        <v>1E</v>
+        <v>Brasil</v>
       </c>
       <c r="AP32" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB32&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB32&amp;"_win")*($U$7:$U$54))</f>
@@ -36569,11 +36569,11 @@
       </c>
       <c r="K33" s="72" t="n">
         <f aca="false">L33+M33+N33</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L33" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA32:AK35,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M33" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA32:AK35,4,0)</f>
@@ -36585,11 +36585,11 @@
       </c>
       <c r="O33" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(1,AA32:AK35,7,0)</f>
-        <v>3 - 1</v>
+        <v>5 - 1</v>
       </c>
       <c r="P33" s="73" t="n">
         <f aca="false">L33*3+M33</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R33" s="40" t="n">
         <f aca="false">DATE(2018,6,23)+TIME(7,0,0)+gmt_delta</f>
@@ -36605,15 +36605,15 @@
       </c>
       <c r="U33" s="42" t="n">
         <f aca="false">IF(S33="",0,IF(VLOOKUP(E33,$AB$8:$AK$53,7,0)=VLOOKUP(H33,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V33" s="40" t="n">
         <f aca="false">U33*F33</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W33" s="40" t="n">
         <f aca="false">U33*G33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X33" s="40" t="n">
         <f aca="false">IF(OR(E33=my_team,H33=my_team),1,0)</f>
@@ -36637,7 +36637,7 @@
       </c>
       <c r="AD33" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB33 &amp; "_draw")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE33" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB33 &amp; "_lose")</f>
@@ -36645,15 +36645,15 @@
       </c>
       <c r="AF33" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB33,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB33,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG33" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB33,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB33,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH33" s="40" t="n">
         <f aca="false">(AF33-AG33)*100+AK33*10000+AF33</f>
-        <v>40103</v>
+        <v>50104</v>
       </c>
       <c r="AI33" s="40" t="n">
         <f aca="false">AF33-AG33</f>
@@ -36661,11 +36661,11 @@
       </c>
       <c r="AJ33" s="40" t="n">
         <f aca="false">(AI33-AI37)/AI36</f>
-        <v>0.666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AK33" s="40" t="n">
         <f aca="false">AC33*3+AD33</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL33" s="40" t="n">
         <f aca="false">AP33/AP36*1000+AQ33/AQ36*100+AT33/AT36*10+AR33/AR36</f>
@@ -36677,11 +36677,11 @@
       </c>
       <c r="AN33" s="42" t="n">
         <f aca="false">1000*AK33/AK36+100*AJ33+10*AF33/AF36+1*AL33/AL36+AM33</f>
-        <v>874.167261666667</v>
+        <v>772.286309285714</v>
       </c>
       <c r="AO33" s="43" t="str">
         <f aca="false">IF(SUM(AC32:AE35)=12,J34,INDEX(T,79,lang))</f>
-        <v>2E</v>
+        <v>Suiza</v>
       </c>
       <c r="AP33" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB33&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB33&amp;"_win")*($U$7:$U$54))</f>
@@ -36768,7 +36768,7 @@
       </c>
       <c r="K34" s="76" t="n">
         <f aca="false">L34+M34+N34</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L34" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA32:AK35,3,0)</f>
@@ -36776,7 +36776,7 @@
       </c>
       <c r="M34" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA32:AK35,4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N34" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA32:AK35,5,0)</f>
@@ -36784,11 +36784,11 @@
       </c>
       <c r="O34" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(2,AA32:AK35,7,0)</f>
-        <v>3 - 2</v>
+        <v>4 - 3</v>
       </c>
       <c r="P34" s="77" t="n">
         <f aca="false">L34*3+M34</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R34" s="40" t="n">
         <f aca="false">DATE(2018,6,23)+TIME(4,0,0)+gmt_delta</f>
@@ -36836,7 +36836,7 @@
       </c>
       <c r="AD34" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB34 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB34 &amp; "_lose")</f>
@@ -36844,15 +36844,15 @@
       </c>
       <c r="AF34" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB34,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB34,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG34" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB34,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB34,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH34" s="40" t="n">
         <f aca="false">(AF34-AG34)*100+AK34*10000+AF34</f>
-        <v>-300</v>
+        <v>9701</v>
       </c>
       <c r="AI34" s="40" t="n">
         <f aca="false">AF34-AG34</f>
@@ -36864,7 +36864,7 @@
       </c>
       <c r="AK34" s="40" t="n">
         <f aca="false">AC34*3+AD34</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL34" s="40" t="n">
         <f aca="false">AP34/AP36*1000+AQ34/AQ36*100+AT34/AT36*10+AR34/AR36</f>
@@ -36876,7 +36876,7 @@
       </c>
       <c r="AN34" s="42" t="n">
         <f aca="false">1000*AK34/AK36+100*AJ34+10*AF34/AF36+1*AL34/AL36+AM34</f>
-        <v>0.000425</v>
+        <v>144.857567857143</v>
       </c>
       <c r="AP34" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB34&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB34&amp;"_win")*($U$7:$U$54))</f>
@@ -36903,7 +36903,7 @@
       </c>
       <c r="AZ34" s="79" t="str">
         <f aca="false">AO38</f>
-        <v>1F</v>
+        <v>Suecia</v>
       </c>
       <c r="BA34" s="80"/>
       <c r="BB34" s="81"/>
@@ -36965,7 +36965,7 @@
       </c>
       <c r="K35" s="76" t="n">
         <f aca="false">L35+M35+N35</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L35" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA32:AK35,3,0)</f>
@@ -36977,11 +36977,11 @@
       </c>
       <c r="N35" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA32:AK35,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O35" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(3,AA32:AK35,7,0)</f>
-        <v>2 - 2</v>
+        <v>2 - 4</v>
       </c>
       <c r="P35" s="77" t="n">
         <f aca="false">L35*3+M35</f>
@@ -37037,7 +37037,7 @@
       </c>
       <c r="AE35" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB35 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF35" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB35,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB35,$G$7:$G$54)</f>
@@ -37045,19 +37045,19 @@
       </c>
       <c r="AG35" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB35,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB35,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH35" s="40" t="n">
         <f aca="false">(AF35-AG35)*100+AK35*10000+AF35</f>
-        <v>30002</v>
+        <v>29802</v>
       </c>
       <c r="AI35" s="40" t="n">
         <f aca="false">AF35-AG35</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AJ35" s="40" t="n">
         <f aca="false">(AI35-AI37)/AI36</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="AK35" s="40" t="n">
         <f aca="false">AC35*3+AD35</f>
@@ -37073,7 +37073,7 @@
       </c>
       <c r="AN35" s="42" t="n">
         <f aca="false">1000*AK35/AK36+100*AJ35+10*AF35/AF36+1*AL35/AL36+AM35</f>
-        <v>655.000378</v>
+        <v>445.071806571429</v>
       </c>
       <c r="AP35" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB35&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB35&amp;"_win")*($U$7:$U$54))</f>
@@ -37098,7 +37098,7 @@
       <c r="AY35" s="78"/>
       <c r="AZ35" s="82" t="str">
         <f aca="false">AO33</f>
-        <v>2E</v>
+        <v>Suiza</v>
       </c>
       <c r="BA35" s="83"/>
       <c r="BB35" s="84"/>
@@ -37165,7 +37165,7 @@
       </c>
       <c r="K36" s="88" t="n">
         <f aca="false">L36+M36+N36</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L36" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA32:AK35,3,0)</f>
@@ -37173,7 +37173,7 @@
       </c>
       <c r="M36" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA32:AK35,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA32:AK35,5,0)</f>
@@ -37181,11 +37181,11 @@
       </c>
       <c r="O36" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA32:AK35,6,0) &amp; " - " &amp; VLOOKUP(4,AA32:AK35,7,0)</f>
-        <v>0 - 3</v>
+        <v>1 - 4</v>
       </c>
       <c r="P36" s="89" t="n">
         <f aca="false">L36*3+M36</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="40" t="n">
         <f aca="false">DATE(2018,6,24)+TIME(1,0,0)+gmt_delta</f>
@@ -37221,11 +37221,11 @@
       </c>
       <c r="AC36" s="40" t="n">
         <f aca="false">MAX(AC32:AC35)-MIN(AC32:AC35)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD36" s="40" t="n">
         <f aca="false">MAX(AD32:AD35)-MIN(AD32:AD35)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE36" s="40" t="n">
         <f aca="false">MAX(AE32:AE35)-MIN(AE32:AE35)+1</f>
@@ -37233,23 +37233,23 @@
       </c>
       <c r="AF36" s="40" t="n">
         <f aca="false">MAX(AF32:AF35)-MIN(AF32:AF35)+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG36" s="40" t="n">
         <f aca="false">MAX(AG32:AG35)-MIN(AG32:AG35)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH36" s="40" t="n">
         <f aca="false">MAX(AH32:AH35)-AH37+1</f>
-        <v>40504</v>
+        <v>60705</v>
       </c>
       <c r="AI36" s="40" t="n">
         <f aca="false">MAX(AI32:AI35)-AI37+1</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AK36" s="40" t="n">
         <f aca="false">MAX(AK32:AK35)-MIN(AK32:AK35)+1</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AL36" s="40" t="n">
         <f aca="false">MAX(AL32:AL35)-MIN(AL32:AL35)+1</f>
@@ -37370,7 +37370,7 @@
       </c>
       <c r="AH37" s="40" t="n">
         <f aca="false">MIN(AH32:AH35)</f>
-        <v>-300</v>
+        <v>9701</v>
       </c>
       <c r="AI37" s="40" t="n">
         <f aca="false">MIN(AI32:AI35)</f>
@@ -37497,7 +37497,7 @@
       </c>
       <c r="AA38" s="40" t="n">
         <f aca="false">COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN38))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB38" s="42" t="str">
         <f aca="false">VLOOKUP("Germany",T,lang,0)</f>
@@ -37513,7 +37513,7 @@
       </c>
       <c r="AE38" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB38 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF38" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB38,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB38,$G$7:$G$54)</f>
@@ -37521,19 +37521,19 @@
       </c>
       <c r="AG38" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB38,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB38,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH38" s="40" t="n">
         <f aca="false">(AF38-AG38)*100+AK38*10000+AF38</f>
-        <v>30002</v>
+        <v>29802</v>
       </c>
       <c r="AI38" s="40" t="n">
         <f aca="false">AF38-AG38</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AJ38" s="40" t="n">
         <f aca="false">(AI38-AI43)/AI42</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AK38" s="40" t="n">
         <f aca="false">AC38*3+AD38</f>
@@ -37541,7 +37541,7 @@
       </c>
       <c r="AL38" s="40" t="n">
         <f aca="false">AP38/AP42*1000+AQ38/AQ42*100+AT38/AT42*10+AR38/AR42</f>
-        <v>504</v>
+        <v>0</v>
       </c>
       <c r="AM38" s="40" t="n">
         <f aca="false">VLOOKUP(AB38,db_fifarank,2,0)/2000000</f>
@@ -37549,15 +37549,15 @@
       </c>
       <c r="AN38" s="42" t="n">
         <f aca="false">1000*AK38/AK42+100*AJ38+10*AF38/AF42+1*AL38/AL42+AM38</f>
-        <v>476.231022222347</v>
+        <v>755.000801</v>
       </c>
       <c r="AO38" s="43" t="str">
         <f aca="false">IF(SUM(AC38:AE41)=12,J39,INDEX(T,80,lang))</f>
-        <v>1F</v>
+        <v>Suecia</v>
       </c>
       <c r="AP38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB38&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB38&amp;"_win")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB38&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB38&amp;"_draw")*($U$7:$U$54))</f>
@@ -37565,15 +37565,15 @@
       </c>
       <c r="AR38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB38)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB38)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS38" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB38)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB38)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT38" s="44" t="n">
         <f aca="false">AR38-AS38</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY38" s="78" t="n">
         <v>56</v>
@@ -37631,11 +37631,11 @@
       </c>
       <c r="J39" s="71" t="str">
         <f aca="false">VLOOKUP(1,AA38:AK41,2,0)</f>
-        <v>México</v>
+        <v>Suecia</v>
       </c>
       <c r="K39" s="72" t="n">
         <f aca="false">L39+M39+N39</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L39" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA38:AK41,3,0)</f>
@@ -37647,11 +37647,11 @@
       </c>
       <c r="N39" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA38:AK41,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O39" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(1,AA38:AK41,7,0)</f>
-        <v>3 - 1</v>
+        <v>5 - 2</v>
       </c>
       <c r="P39" s="73" t="n">
         <f aca="false">L39*3+M39</f>
@@ -37691,7 +37691,7 @@
       </c>
       <c r="AA39" s="40" t="n">
         <f aca="false">COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN39))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB39" s="42" t="str">
         <f aca="false">VLOOKUP("Mexico",T,lang,0)</f>
@@ -37707,7 +37707,7 @@
       </c>
       <c r="AE39" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB39 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF39" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB39,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB39,$G$7:$G$54)</f>
@@ -37715,19 +37715,19 @@
       </c>
       <c r="AG39" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB39,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB39,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH39" s="40" t="n">
         <f aca="false">(AF39-AG39)*100+AK39*10000+AF39</f>
-        <v>60203</v>
+        <v>59903</v>
       </c>
       <c r="AI39" s="40" t="n">
         <f aca="false">AF39-AG39</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AJ39" s="40" t="n">
         <f aca="false">(AI39-AI43)/AI42</f>
-        <v>0.8</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="AK39" s="40" t="n">
         <f aca="false">AC39*3+AD39</f>
@@ -37743,11 +37743,11 @@
       </c>
       <c r="AN39" s="42" t="n">
         <f aca="false">1000*AK39/AK42+100*AJ39+10*AF39/AF42+1*AL39/AL42+AM39</f>
-        <v>947.143373142857</v>
+        <v>1524.16718266667</v>
       </c>
       <c r="AO39" s="43" t="str">
         <f aca="false">IF(SUM(AC38:AE41)=12,J40,INDEX(T,81,lang))</f>
-        <v>2F</v>
+        <v>México</v>
       </c>
       <c r="AP39" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB39&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB39&amp;"_win")*($U$7:$U$54))</f>
@@ -37821,15 +37821,15 @@
       </c>
       <c r="J40" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA38:AK41,2,0)</f>
-        <v>Alemania</v>
+        <v>México</v>
       </c>
       <c r="K40" s="76" t="n">
         <f aca="false">L40+M40+N40</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L40" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA38:AK41,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M40" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA38:AK41,4,0)</f>
@@ -37841,11 +37841,11 @@
       </c>
       <c r="O40" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(2,AA38:AK41,7,0)</f>
-        <v>2 - 2</v>
+        <v>3 - 4</v>
       </c>
       <c r="P40" s="77" t="n">
         <f aca="false">L40*3+M40</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R40" s="40" t="n">
         <f aca="false">DATE(2018,6,25)+TIME(3,0,0)+gmt_delta</f>
@@ -37881,7 +37881,7 @@
       </c>
       <c r="AA40" s="40" t="n">
         <f aca="false">COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN40))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB40" s="42" t="str">
         <f aca="false">VLOOKUP("Sweden",T,lang,0)</f>
@@ -37889,7 +37889,7 @@
       </c>
       <c r="AC40" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB40 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD40" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB40 &amp; "_draw")</f>
@@ -37901,7 +37901,7 @@
       </c>
       <c r="AF40" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB40,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB40,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AG40" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB40,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB40,$F$7:$F$54)</f>
@@ -37909,23 +37909,23 @@
       </c>
       <c r="AH40" s="40" t="n">
         <f aca="false">(AF40-AG40)*100+AK40*10000+AF40</f>
-        <v>30002</v>
+        <v>60305</v>
       </c>
       <c r="AI40" s="40" t="n">
         <f aca="false">AF40-AG40</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ40" s="40" t="n">
         <f aca="false">(AI40-AI43)/AI42</f>
-        <v>0.4</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="AK40" s="40" t="n">
         <f aca="false">AC40*3+AD40</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL40" s="40" t="n">
         <f aca="false">AP40/AP42*1000+AQ40/AQ42*100+AT40/AT42*10+AR40/AR42</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="AM40" s="40" t="n">
         <f aca="false">VLOOKUP(AB40,db_fifarank,2,0)/2000000</f>
@@ -37933,7 +37933,7 @@
       </c>
       <c r="AN40" s="42" t="n">
         <f aca="false">1000*AK40/AK42+100*AJ40+10*AF40/AF42+1*AL40/AL42+AM40</f>
-        <v>475.232688726284</v>
+        <v>1595.83383233333</v>
       </c>
       <c r="AP40" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB40&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB40&amp;"_win")*($U$7:$U$54))</f>
@@ -37945,15 +37945,15 @@
       </c>
       <c r="AR40" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB40)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB40)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS40" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB40)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB40)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT40" s="44" t="n">
         <f aca="false">AR40-AS40</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37988,11 +37988,11 @@
       </c>
       <c r="J41" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA38:AK41,2,0)</f>
-        <v>Suecia</v>
+        <v>República de Corea</v>
       </c>
       <c r="K41" s="76" t="n">
         <f aca="false">L41+M41+N41</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L41" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA38:AK41,3,0)</f>
@@ -38004,11 +38004,11 @@
       </c>
       <c r="N41" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA38:AK41,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O41" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(3,AA38:AK41,7,0)</f>
-        <v>2 - 2</v>
+        <v>3 - 3</v>
       </c>
       <c r="P41" s="77" t="n">
         <f aca="false">L41*3+M41</f>
@@ -38048,7 +38048,7 @@
       </c>
       <c r="AA41" s="40" t="n">
         <f aca="false">COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN41))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB41" s="42" t="str">
         <f aca="false">VLOOKUP("Korea Republic",T,lang,0)</f>
@@ -38056,7 +38056,7 @@
       </c>
       <c r="AC41" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB41 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD41" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB41 &amp; "_draw")</f>
@@ -38068,7 +38068,7 @@
       </c>
       <c r="AF41" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB41,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB41,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG41" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB41,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB41,$F$7:$F$54)</f>
@@ -38076,19 +38076,19 @@
       </c>
       <c r="AH41" s="40" t="n">
         <f aca="false">(AF41-AG41)*100+AK41*10000+AF41</f>
-        <v>-199</v>
+        <v>30003</v>
       </c>
       <c r="AI41" s="40" t="n">
         <f aca="false">AF41-AG41</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AJ41" s="40" t="n">
         <f aca="false">(AI41-AI43)/AI42</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="AK41" s="40" t="n">
         <f aca="false">AC41*3+AD41</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL41" s="40" t="n">
         <f aca="false">AP41/AP42*1000+AQ41/AQ42*100+AT41/AT42*10+AR41/AR42</f>
@@ -38100,7 +38100,7 @@
       </c>
       <c r="AN41" s="42" t="n">
         <f aca="false">1000*AK41/AK42+100*AJ41+10*AF41/AF42+1*AL41/AL42+AM41</f>
-        <v>3.33361833333333</v>
+        <v>790.833618333333</v>
       </c>
       <c r="AP41" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB41&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB41&amp;"_win")*($U$7:$U$54))</f>
@@ -38172,15 +38172,15 @@
       </c>
       <c r="J42" s="87" t="str">
         <f aca="false">VLOOKUP(4,AA38:AK41,2,0)</f>
-        <v>República de Corea</v>
+        <v>Alemania</v>
       </c>
       <c r="K42" s="88" t="n">
         <f aca="false">L42+M42+N42</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L42" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA38:AK41,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA38:AK41,4,0)</f>
@@ -38192,11 +38192,11 @@
       </c>
       <c r="O42" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA38:AK41,6,0) &amp; " - " &amp; VLOOKUP(4,AA38:AK41,7,0)</f>
-        <v>1 - 3</v>
+        <v>2 - 4</v>
       </c>
       <c r="P42" s="89" t="n">
         <f aca="false">L42*3+M42</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R42" s="40" t="n">
         <f aca="false">DATE(2018,6,25)+TIME(7,0,0)+gmt_delta</f>
@@ -38232,7 +38232,7 @@
       </c>
       <c r="AC42" s="40" t="n">
         <f aca="false">MAX(AC38:AC41)-MIN(AC38:AC41)+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD42" s="40" t="n">
         <f aca="false">MAX(AD38:AD41)-MIN(AD38:AD41)+1</f>
@@ -38240,11 +38240,11 @@
       </c>
       <c r="AE42" s="40" t="n">
         <f aca="false">MAX(AE38:AE41)-MIN(AE38:AE41)+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF42" s="40" t="n">
         <f aca="false">MAX(AF38:AF41)-MIN(AF38:AF41)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG42" s="40" t="n">
         <f aca="false">MAX(AG38:AG41)-MIN(AG38:AG41)+1</f>
@@ -38252,23 +38252,23 @@
       </c>
       <c r="AH42" s="40" t="n">
         <f aca="false">MAX(AH38:AH41)-AH43+1</f>
-        <v>60403</v>
+        <v>30504</v>
       </c>
       <c r="AI42" s="40" t="n">
         <f aca="false">MAX(AI38:AI41)-AI43+1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AK42" s="40" t="n">
         <f aca="false">MAX(AK38:AK41)-MIN(AK38:AK41)+1</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AL42" s="40" t="n">
         <f aca="false">MAX(AL38:AL41)-MIN(AL38:AL41)+1</f>
-        <v>508</v>
+        <v>1</v>
       </c>
       <c r="AP42" s="40" t="n">
         <f aca="false">MAX(AP38:AP41)-MIN(AP38:AP41)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ42" s="40" t="n">
         <f aca="false">MAX(AQ38:AQ41)-MIN(AQ38:AQ41)+1</f>
@@ -38276,15 +38276,15 @@
       </c>
       <c r="AR42" s="40" t="n">
         <f aca="false">MAX(AR38:AR41)-MIN(AR38:AR41)+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AS42" s="40" t="n">
         <f aca="false">MAX(AS38:AS41)-MIN(AS38:AS41)+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT42" s="40" t="n">
         <f aca="false">MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BJ42" s="100"/>
       <c r="BK42" s="100"/>
@@ -38362,7 +38362,7 @@
       </c>
       <c r="AH43" s="40" t="n">
         <f aca="false">MIN(AH38:AH41)</f>
-        <v>-199</v>
+        <v>29802</v>
       </c>
       <c r="AI43" s="40" t="n">
         <f aca="false">MIN(AI38:AI41)</f>
@@ -38905,8 +38905,12 @@
         <f aca="false">AB35</f>
         <v>Serbia</v>
       </c>
-      <c r="F47" s="64"/>
-      <c r="G47" s="65"/>
+      <c r="F47" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="65" t="n">
+        <v>2</v>
+      </c>
       <c r="H47" s="66" t="str">
         <f aca="false">AB32</f>
         <v>Brasil</v>
@@ -38945,11 +38949,11 @@
       </c>
       <c r="S47" s="41" t="str">
         <f aca="false">IF(OR(F47="",G47=""),"",IF(F47&gt;G47,E47&amp;"_win",IF(F47&lt;G47,E47&amp;"_lose",E47&amp;"_draw")))</f>
-        <v/>
+        <v>Serbia_lose</v>
       </c>
       <c r="T47" s="41" t="str">
         <f aca="false">IF(S47="","",IF(F47&lt;G47,H47&amp;"_win",IF(F47&gt;G47,H47&amp;"_lose",H47&amp;"_draw")))</f>
-        <v/>
+        <v>Brasil_win</v>
       </c>
       <c r="U47" s="42" t="n">
         <f aca="false">IF(S47="",0,IF(VLOOKUP(E47,$AB$8:$AK$53,7,0)=VLOOKUP(H47,$AB$8:$AK$53,7,0),1,0))</f>
@@ -38967,9 +38971,9 @@
         <f aca="false">IF(OR(E47=my_team,H47=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y47" s="40" t="str">
+      <c r="Y47" s="40" t="n">
         <f aca="false">IF(OR(F47="",G47=""),"",IF(F47&gt;G47,1,IF(F47&lt;G47,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA47" s="40" t="n">
         <f aca="false">COUNTIF(AN44:AN47,CONCATENATE("&gt;=",AN47))</f>
@@ -39072,8 +39076,12 @@
         <f aca="false">AB33</f>
         <v>Suiza</v>
       </c>
-      <c r="F48" s="64"/>
-      <c r="G48" s="65"/>
+      <c r="F48" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="65" t="n">
+        <v>1</v>
+      </c>
       <c r="H48" s="66" t="str">
         <f aca="false">AB34</f>
         <v>Costa Rica</v>
@@ -39112,11 +39120,11 @@
       </c>
       <c r="S48" s="41" t="str">
         <f aca="false">IF(OR(F48="",G48=""),"",IF(F48&gt;G48,E48&amp;"_win",IF(F48&lt;G48,E48&amp;"_lose",E48&amp;"_draw")))</f>
-        <v/>
+        <v>Suiza_draw</v>
       </c>
       <c r="T48" s="41" t="str">
         <f aca="false">IF(S48="","",IF(F48&lt;G48,H48&amp;"_win",IF(F48&gt;G48,H48&amp;"_lose",H48&amp;"_draw")))</f>
-        <v/>
+        <v>Costa Rica_draw</v>
       </c>
       <c r="U48" s="42" t="n">
         <f aca="false">IF(S48="",0,IF(VLOOKUP(E48,$AB$8:$AK$53,7,0)=VLOOKUP(H48,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39134,9 +39142,9 @@
         <f aca="false">IF(OR(E48=my_team,H48=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y48" s="40" t="str">
+      <c r="Y48" s="40" t="n">
         <f aca="false">IF(OR(F48="",G48=""),"",IF(F48&gt;G48,1,IF(F48&lt;G48,-1,0)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AC48" s="40" t="n">
         <f aca="false">MAX(AC44:AC47)-MIN(AC44:AC47)+1</f>
@@ -39219,8 +39227,12 @@
         <f aca="false">AB41</f>
         <v>República de Corea</v>
       </c>
-      <c r="F49" s="64"/>
-      <c r="G49" s="65"/>
+      <c r="F49" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" s="65" t="n">
+        <v>0</v>
+      </c>
       <c r="H49" s="66" t="str">
         <f aca="false">AB38</f>
         <v>Alemania</v>
@@ -39231,11 +39243,11 @@
       </c>
       <c r="S49" s="41" t="str">
         <f aca="false">IF(OR(F49="",G49=""),"",IF(F49&gt;G49,E49&amp;"_win",IF(F49&lt;G49,E49&amp;"_lose",E49&amp;"_draw")))</f>
-        <v/>
+        <v>República de Corea_win</v>
       </c>
       <c r="T49" s="41" t="str">
         <f aca="false">IF(S49="","",IF(F49&lt;G49,H49&amp;"_win",IF(F49&gt;G49,H49&amp;"_lose",H49&amp;"_draw")))</f>
-        <v/>
+        <v>Alemania_lose</v>
       </c>
       <c r="U49" s="42" t="n">
         <f aca="false">IF(S49="",0,IF(VLOOKUP(E49,$AB$8:$AK$53,7,0)=VLOOKUP(H49,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39253,9 +39265,9 @@
         <f aca="false">IF(OR(E49=my_team,H49=my_team),1,0)</f>
         <v>1</v>
       </c>
-      <c r="Y49" s="40" t="str">
+      <c r="Y49" s="40" t="n">
         <f aca="false">IF(OR(F49="",G49=""),"",IF(F49&gt;G49,1,IF(F49&lt;G49,-1,0)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AH49" s="40" t="n">
         <f aca="false">MIN(AH44:AH47)</f>
@@ -39290,8 +39302,12 @@
         <f aca="false">AB39</f>
         <v>México</v>
       </c>
-      <c r="F50" s="64"/>
-      <c r="G50" s="65"/>
+      <c r="F50" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="65" t="n">
+        <v>3</v>
+      </c>
       <c r="H50" s="66" t="str">
         <f aca="false">AB40</f>
         <v>Suecia</v>
@@ -39330,11 +39346,11 @@
       </c>
       <c r="S50" s="41" t="str">
         <f aca="false">IF(OR(F50="",G50=""),"",IF(F50&gt;G50,E50&amp;"_win",IF(F50&lt;G50,E50&amp;"_lose",E50&amp;"_draw")))</f>
-        <v/>
+        <v>México_lose</v>
       </c>
       <c r="T50" s="41" t="str">
         <f aca="false">IF(S50="","",IF(F50&lt;G50,H50&amp;"_win",IF(F50&gt;G50,H50&amp;"_lose",H50&amp;"_draw")))</f>
-        <v/>
+        <v>Suecia_win</v>
       </c>
       <c r="U50" s="42" t="n">
         <f aca="false">IF(S50="",0,IF(VLOOKUP(E50,$AB$8:$AK$53,7,0)=VLOOKUP(H50,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39352,9 +39368,9 @@
         <f aca="false">IF(OR(E50=my_team,H50=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y50" s="40" t="str">
+      <c r="Y50" s="40" t="n">
         <f aca="false">IF(OR(F50="",G50=""),"",IF(F50&gt;G50,1,IF(F50&lt;G50,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA50" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN50))</f>

</xml_diff>

<commit_message>
Resultados actualizados hasta el dia 28 de junio, fin de la fase de grupos
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -14014,9 +14014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486440</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14030,7 +14030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1232280"/>
-          <a:ext cx="224640" cy="147240"/>
+          <a:ext cx="223920" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14051,9 +14051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1486440</xdr:colOff>
+      <xdr:colOff>1485720</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14067,7 +14067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4276080"/>
-          <a:ext cx="224640" cy="147240"/>
+          <a:ext cx="223920" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14088,9 +14088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14104,7 +14104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7324200"/>
-          <a:ext cx="224640" cy="147240"/>
+          <a:ext cx="223920" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14125,9 +14125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14141,7 +14141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="1232280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14162,9 +14162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14178,7 +14178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4470840"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14199,9 +14199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14215,7 +14215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7519320"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14236,9 +14236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14252,7 +14252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1422720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14273,9 +14273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249840</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14289,7 +14289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5461560" y="4280760"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14310,9 +14310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14326,7 +14326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7519320"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14347,9 +14347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14363,7 +14363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1431720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14384,9 +14384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>185040</xdr:rowOff>
+      <xdr:rowOff>184320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14400,7 +14400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4484520"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14421,9 +14421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>176760</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14437,7 +14437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7333560"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14458,9 +14458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14474,7 +14474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1613880"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14495,9 +14495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14511,7 +14511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4661280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14532,9 +14532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14548,7 +14548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7709760"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14569,9 +14569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14585,7 +14585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1613880"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14606,9 +14606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14622,7 +14622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4856400"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14643,9 +14643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14659,7 +14659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="7899840"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14680,9 +14680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14696,7 +14696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="7904520"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14717,9 +14717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14733,7 +14733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4661280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14754,9 +14754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14770,7 +14770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1799640"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,9 +14791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14807,7 +14807,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1804320"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14844,7 +14844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4847040"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14865,9 +14865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14881,7 +14881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7705080"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14902,9 +14902,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14918,7 +14918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1994760"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14939,9 +14939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14955,7 +14955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5042880"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14976,9 +14976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14992,7 +14992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8090280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15013,9 +15013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15029,7 +15029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1994760"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15050,9 +15050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15066,7 +15066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5228640"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15087,9 +15087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15103,7 +15103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8276040"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15124,9 +15124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15140,7 +15140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2184840"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15161,9 +15161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15177,7 +15177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="5042880"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15198,9 +15198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15214,7 +15214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8276040"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15235,9 +15235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15251,7 +15251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="2180160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15272,9 +15272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15288,7 +15288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5228640"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,9 +15309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15325,7 +15325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8085600"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15346,9 +15346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15362,7 +15362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2370600"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15383,9 +15383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15399,7 +15399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5423760"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15420,9 +15420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15436,7 +15436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="8467200"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15457,9 +15457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15473,7 +15473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="2375280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15494,9 +15494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15510,7 +15510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8662320"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15531,9 +15531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15547,7 +15547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5613840"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15568,9 +15568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15584,7 +15584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2565720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15605,9 +15605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15621,7 +15621,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5418360"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15642,9 +15642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15658,7 +15658,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455800" y="8656920"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15679,9 +15679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15695,7 +15695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2564640"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15732,7 +15732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926160" y="5612760"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15753,9 +15753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477440</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15769,7 +15769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8466480"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15806,7 +15806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2757960"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15827,9 +15827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15843,7 +15843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5800680"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15864,9 +15864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15880,7 +15880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="8849160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15901,9 +15901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>196920</xdr:colOff>
+      <xdr:colOff>196200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15917,7 +15917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481720" y="2753280"/>
-          <a:ext cx="148680" cy="148680"/>
+          <a:ext cx="147960" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15938,9 +15938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>192240</xdr:colOff>
+      <xdr:colOff>191520</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15954,7 +15954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5477040" y="5991120"/>
-          <a:ext cx="148680" cy="148680"/>
+          <a:ext cx="147960" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15975,9 +15975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1440000</xdr:colOff>
+      <xdr:colOff>1439280</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15991,7 +15991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956760" y="9039240"/>
-          <a:ext cx="148680" cy="148680"/>
+          <a:ext cx="147960" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16012,9 +16012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16028,7 +16028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2943720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16049,9 +16049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16065,7 +16065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="5800680"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16086,9 +16086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16102,7 +16102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9039240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,9 +16123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16139,7 +16139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="2943720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16160,9 +16160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16176,7 +16176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5991120"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16197,9 +16197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16213,7 +16213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="8849160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16234,9 +16234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16250,7 +16250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3134160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16271,9 +16271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16287,7 +16287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6182280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16308,9 +16308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16324,7 +16324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9229680"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16345,9 +16345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16361,7 +16361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3138840"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16382,9 +16382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16398,7 +16398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6372720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16419,9 +16419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16435,7 +16435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9420120"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16456,9 +16456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16472,7 +16472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3324240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16493,9 +16493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16509,7 +16509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6182280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16530,9 +16530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16546,7 +16546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9420120"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16567,9 +16567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16583,7 +16583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3324240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16604,9 +16604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16620,7 +16620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6372720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16641,9 +16641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16657,7 +16657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9229680"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16678,9 +16678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1462680</xdr:colOff>
+      <xdr:colOff>1461960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16694,7 +16694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="3514680"/>
-          <a:ext cx="176040" cy="148680"/>
+          <a:ext cx="175320" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16715,9 +16715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1462680</xdr:colOff>
+      <xdr:colOff>1461960</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16731,7 +16731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="6563160"/>
-          <a:ext cx="176040" cy="148680"/>
+          <a:ext cx="175320" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16752,9 +16752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>214920</xdr:colOff>
+      <xdr:colOff>214200</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16768,7 +16768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5472360" y="9611280"/>
-          <a:ext cx="176040" cy="148680"/>
+          <a:ext cx="175320" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16789,9 +16789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16805,7 +16805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3514680"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16826,9 +16826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16842,7 +16842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6753240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16863,9 +16863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16879,7 +16879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9801720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16900,9 +16900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16916,7 +16916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3705120"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16937,9 +16937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16953,7 +16953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6563160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16974,9 +16974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16990,7 +16990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9801720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17011,9 +17011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17027,7 +17027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3896280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17048,9 +17048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17064,7 +17064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6943680"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17085,9 +17085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17101,7 +17101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9992160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17122,9 +17122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17138,7 +17138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3900960"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17159,9 +17159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17175,7 +17175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="7134120"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17196,9 +17196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17212,7 +17212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="10182240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17233,9 +17233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17249,7 +17249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="4091400"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17270,9 +17270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>171720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17286,7 +17286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6948360"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17307,9 +17307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17323,7 +17323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="10182240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17344,9 +17344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17360,7 +17360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="4086720"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17381,9 +17381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17397,7 +17397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="7134120"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17418,9 +17418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17434,7 +17434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9992160"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17455,9 +17455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>171720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17471,7 +17471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3709800"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17492,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1483920</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17508,7 +17508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6753240"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17529,9 +17529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479960</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17545,7 +17545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9611280"/>
-          <a:ext cx="221760" cy="148680"/>
+          <a:ext cx="221040" cy="147960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31724,8 +31724,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G49" activeCellId="0" sqref="G49"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34776,7 +34776,7 @@
       </c>
       <c r="AZ22" s="79" t="str">
         <f aca="false">AO44</f>
-        <v>1G</v>
+        <v>Bélgica</v>
       </c>
       <c r="BA22" s="80"/>
       <c r="BB22" s="81"/>
@@ -34971,7 +34971,7 @@
       <c r="AY23" s="78"/>
       <c r="AZ23" s="82" t="str">
         <f aca="false">AO51</f>
-        <v>2H</v>
+        <v>Senegal</v>
       </c>
       <c r="BA23" s="83"/>
       <c r="BB23" s="84"/>
@@ -37580,7 +37580,7 @@
       </c>
       <c r="AZ38" s="79" t="str">
         <f aca="false">AO50</f>
-        <v>1H</v>
+        <v>Colombia</v>
       </c>
       <c r="BA38" s="80"/>
       <c r="BB38" s="81"/>
@@ -37772,7 +37772,7 @@
       <c r="AY39" s="78"/>
       <c r="AZ39" s="82" t="str">
         <f aca="false">AO45</f>
-        <v>2G</v>
+        <v>Inglaterra</v>
       </c>
       <c r="BA39" s="83"/>
       <c r="BB39" s="84"/>
@@ -38470,7 +38470,7 @@
       </c>
       <c r="AC44" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_win")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD44" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_draw")</f>
@@ -38482,7 +38482,7 @@
       </c>
       <c r="AF44" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB44,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB44,$G$7:$G$54)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AG44" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB44,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB44,$F$7:$F$54)</f>
@@ -38490,19 +38490,19 @@
       </c>
       <c r="AH44" s="40" t="n">
         <f aca="false">(AF44-AG44)*100+AK44*10000+AF44</f>
-        <v>60608</v>
+        <v>90709</v>
       </c>
       <c r="AI44" s="40" t="n">
         <f aca="false">AF44-AG44</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AJ44" s="40" t="n">
         <f aca="false">(AI44-AI49)/AI48</f>
-        <v>0.933333333333333</v>
+        <v>0.941176470588235</v>
       </c>
       <c r="AK44" s="40" t="n">
         <f aca="false">AC44*3+AD44</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AL44" s="40" t="n">
         <f aca="false">AP44/AP48*1000+AQ44/AQ48*100+AT44/AT48*10+AR44/AR48</f>
@@ -38514,11 +38514,11 @@
       </c>
       <c r="AN44" s="42" t="n">
         <f aca="false">1000*AK44/AK48+100*AJ44+10*AF44/AF48+1*AL44/AL48+AM44</f>
-        <v>960.476852976191</v>
+        <v>1005.36830955882</v>
       </c>
       <c r="AO44" s="43" t="str">
         <f aca="false">IF(SUM(AC44:AE47)=12,J45,INDEX(T,82,lang))</f>
-        <v>1G</v>
+        <v>Bélgica</v>
       </c>
       <c r="AP44" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB44&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB44&amp;"_win")*($U$7:$U$54))</f>
@@ -38577,11 +38577,11 @@
       </c>
       <c r="K45" s="72" t="n">
         <f aca="false">L45+M45+N45</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L45" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA44:AK47,3,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M45" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA44:AK47,4,0)</f>
@@ -38593,11 +38593,11 @@
       </c>
       <c r="O45" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(1,AA44:AK47,7,0)</f>
-        <v>8 - 2</v>
+        <v>9 - 2</v>
       </c>
       <c r="P45" s="73" t="n">
         <f aca="false">L45*3+M45</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R45" s="40" t="n">
         <f aca="false">DATE(2018,6,26)+TIME(7,0,0)+gmt_delta</f>
@@ -38649,23 +38649,23 @@
       </c>
       <c r="AE45" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB45 &amp; "_lose")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF45" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB45,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB45,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG45" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB45,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB45,$F$7:$F$54)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AH45" s="40" t="n">
         <f aca="false">(AF45-AG45)*100+AK45*10000+AF45</f>
-        <v>-799</v>
+        <v>-898</v>
       </c>
       <c r="AI45" s="40" t="n">
         <f aca="false">AF45-AG45</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="AJ45" s="40" t="n">
         <f aca="false">(AI45-AI49)/AI48</f>
@@ -38685,11 +38685,11 @@
       </c>
       <c r="AN45" s="42" t="n">
         <f aca="false">1000*AK45/AK48+100*AJ45+10*AF45/AF48+1*AL45/AL48+AM45</f>
-        <v>1.2503105</v>
+        <v>2.5003105</v>
       </c>
       <c r="AO45" s="43" t="str">
         <f aca="false">IF(SUM(AC44:AE47)=12,J46,INDEX(T,83,lang))</f>
-        <v>2G</v>
+        <v>Inglaterra</v>
       </c>
       <c r="AP45" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB45&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB45&amp;"_win")*($U$7:$U$54))</f>
@@ -38748,7 +38748,7 @@
       </c>
       <c r="K46" s="76" t="n">
         <f aca="false">L46+M46+N46</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L46" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA44:AK47,3,0)</f>
@@ -38760,11 +38760,11 @@
       </c>
       <c r="N46" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA44:AK47,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O46" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(2,AA44:AK47,7,0)</f>
-        <v>8 - 2</v>
+        <v>8 - 3</v>
       </c>
       <c r="P46" s="77" t="n">
         <f aca="false">L46*3+M46</f>
@@ -38812,7 +38812,7 @@
       </c>
       <c r="AC46" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD46" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_draw")</f>
@@ -38824,27 +38824,27 @@
       </c>
       <c r="AF46" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB46,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB46,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG46" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB46,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB46,$F$7:$F$54)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH46" s="40" t="n">
         <f aca="false">(AF46-AG46)*100+AK46*10000+AF46</f>
-        <v>-397</v>
+        <v>29705</v>
       </c>
       <c r="AI46" s="40" t="n">
         <f aca="false">AF46-AG46</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AJ46" s="40" t="n">
         <f aca="false">(AI46-AI49)/AI48</f>
-        <v>0.266666666666667</v>
+        <v>0.352941176470588</v>
       </c>
       <c r="AK46" s="40" t="n">
         <f aca="false">AC46*3+AD46</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL46" s="40" t="n">
         <f aca="false">AP46/AP48*1000+AQ46/AQ48*100+AT46/AT48*10+AR46/AR48</f>
@@ -38856,7 +38856,7 @@
       </c>
       <c r="AN46" s="42" t="n">
         <f aca="false">1000*AK46/AK48+100*AJ46+10*AF46/AF48+1*AL46/AL48+AM46</f>
-        <v>30.4170856666667</v>
+        <v>341.544536647059</v>
       </c>
       <c r="AP46" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB46&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB46&amp;"_win")*($U$7:$U$54))</f>
@@ -38921,11 +38921,11 @@
       </c>
       <c r="K47" s="76" t="n">
         <f aca="false">L47+M47+N47</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L47" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA44:AK47,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA44:AK47,4,0)</f>
@@ -38937,11 +38937,11 @@
       </c>
       <c r="O47" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(3,AA44:AK47,7,0)</f>
-        <v>3 - 7</v>
+        <v>5 - 8</v>
       </c>
       <c r="P47" s="77" t="n">
         <f aca="false">L47*3+M47</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R47" s="40" t="n">
         <f aca="false">DATE(2018,6,27)+TIME(7,0,0)+gmt_delta</f>
@@ -38993,7 +38993,7 @@
       </c>
       <c r="AE47" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB47 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF47" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB47,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB47,$G$7:$G$54)</f>
@@ -39001,19 +39001,19 @@
       </c>
       <c r="AG47" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB47,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB47,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH47" s="40" t="n">
         <f aca="false">(AF47-AG47)*100+AK47*10000+AF47</f>
-        <v>60608</v>
+        <v>60508</v>
       </c>
       <c r="AI47" s="40" t="n">
         <f aca="false">AF47-AG47</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AJ47" s="40" t="n">
         <f aca="false">(AI47-AI49)/AI48</f>
-        <v>0.933333333333333</v>
+        <v>0.823529411764706</v>
       </c>
       <c r="AK47" s="40" t="n">
         <f aca="false">AC47*3+AD47</f>
@@ -39029,7 +39029,7 @@
       </c>
       <c r="AN47" s="42" t="n">
         <f aca="false">1000*AK47/AK48+100*AJ47+10*AF47/AF48+1*AL47/AL48+AM47</f>
-        <v>960.47671397619</v>
+        <v>692.353464676471</v>
       </c>
       <c r="AP47" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB47&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB47&amp;"_win")*($U$7:$U$54))</f>
@@ -39092,7 +39092,7 @@
       </c>
       <c r="K48" s="88" t="n">
         <f aca="false">L48+M48+N48</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L48" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA44:AK47,3,0)</f>
@@ -39104,11 +39104,11 @@
       </c>
       <c r="N48" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA44:AK47,5,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O48" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA44:AK47,6,0) &amp; " - " &amp; VLOOKUP(4,AA44:AK47,7,0)</f>
-        <v>1 - 9</v>
+        <v>2 - 11</v>
       </c>
       <c r="P48" s="89" t="n">
         <f aca="false">L48*3+M48</f>
@@ -39148,7 +39148,7 @@
       </c>
       <c r="AC48" s="40" t="n">
         <f aca="false">MAX(AC44:AC47)-MIN(AC44:AC47)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD48" s="40" t="n">
         <f aca="false">MAX(AD44:AD47)-MIN(AD44:AD47)+1</f>
@@ -39156,7 +39156,7 @@
       </c>
       <c r="AE48" s="40" t="n">
         <f aca="false">MAX(AE44:AE47)-MIN(AE44:AE47)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF48" s="40" t="n">
         <f aca="false">MAX(AF44:AF47)-MIN(AF44:AF47)+1</f>
@@ -39164,19 +39164,19 @@
       </c>
       <c r="AG48" s="40" t="n">
         <f aca="false">MAX(AG44:AG47)-MIN(AG44:AG47)+1</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AH48" s="40" t="n">
         <f aca="false">MAX(AH44:AH47)-AH49+1</f>
-        <v>61408</v>
+        <v>91608</v>
       </c>
       <c r="AI48" s="40" t="n">
         <f aca="false">MAX(AI44:AI47)-AI49+1</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AK48" s="40" t="n">
         <f aca="false">MAX(AK44:AK47)-MIN(AK44:AK47)+1</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AL48" s="40" t="n">
         <f aca="false">MAX(AL44:AL47)-MIN(AL44:AL47)+1</f>
@@ -39271,11 +39271,11 @@
       </c>
       <c r="AH49" s="40" t="n">
         <f aca="false">MIN(AH44:AH47)</f>
-        <v>-799</v>
+        <v>-898</v>
       </c>
       <c r="AI49" s="40" t="n">
         <f aca="false">MIN(AI44:AI47)</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="AY49" s="103"/>
       <c r="AZ49" s="103"/>
@@ -39382,7 +39382,7 @@
       </c>
       <c r="AC50" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD50" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_draw")</f>
@@ -39394,7 +39394,7 @@
       </c>
       <c r="AF50" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB50,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB50,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG50" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB50,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB50,$F$7:$F$54)</f>
@@ -39402,11 +39402,11 @@
       </c>
       <c r="AH50" s="40" t="n">
         <f aca="false">(AF50-AG50)*100+AK50*10000+AF50</f>
-        <v>-399</v>
+        <v>29702</v>
       </c>
       <c r="AI50" s="40" t="n">
         <f aca="false">AF50-AG50</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AJ50" s="40" t="n">
         <f aca="false">(AI50-AI55)/AI54</f>
@@ -39414,7 +39414,7 @@
       </c>
       <c r="AK50" s="40" t="n">
         <f aca="false">AC50*3+AD50</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL50" s="40" t="n">
         <f aca="false">AP50/AP54*1000+AQ50/AQ54*100+AT50/AT54*10+AR50/AR54</f>
@@ -39426,11 +39426,11 @@
       </c>
       <c r="AN50" s="42" t="n">
         <f aca="false">1000*AK50/AK54+100*AJ50+10*AF50/AF54+1*AL50/AL54+AM50</f>
-        <v>2.5006045</v>
+        <v>755.0006045</v>
       </c>
       <c r="AO50" s="43" t="str">
         <f aca="false">IF(SUM(AC50:AE53)=12,J51,INDEX(T,84,lang))</f>
-        <v>1H</v>
+        <v>Colombia</v>
       </c>
       <c r="AP50" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB50&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB50&amp;"_win")*($U$7:$U$54))</f>
@@ -39477,39 +39477,43 @@
         <f aca="false">AB47</f>
         <v>Inglaterra</v>
       </c>
-      <c r="F51" s="64"/>
-      <c r="G51" s="65"/>
+      <c r="F51" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="65" t="n">
+        <v>1</v>
+      </c>
       <c r="H51" s="66" t="str">
         <f aca="false">AB44</f>
         <v>Bélgica</v>
       </c>
       <c r="J51" s="71" t="str">
         <f aca="false">VLOOKUP(1,AA50:AK53,2,0)</f>
-        <v>Senegal</v>
+        <v>Colombia</v>
       </c>
       <c r="K51" s="72" t="n">
         <f aca="false">L51+M51+N51</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L51" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA50:AK53,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M51" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA50:AK53,4,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="72" t="n">
         <f aca="false">VLOOKUP(1,AA50:AK53,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51" s="72" t="str">
         <f aca="false">VLOOKUP(1,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(1,AA50:AK53,7,0)</f>
-        <v>4 - 3</v>
+        <v>5 - 2</v>
       </c>
       <c r="P51" s="73" t="n">
         <f aca="false">L51*3+M51</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R51" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(7,0,0)+gmt_delta</f>
@@ -39517,11 +39521,11 @@
       </c>
       <c r="S51" s="41" t="str">
         <f aca="false">IF(OR(F51="",G51=""),"",IF(F51&gt;G51,E51&amp;"_win",IF(F51&lt;G51,E51&amp;"_lose",E51&amp;"_draw")))</f>
-        <v/>
+        <v>Inglaterra_lose</v>
       </c>
       <c r="T51" s="41" t="str">
         <f aca="false">IF(S51="","",IF(F51&lt;G51,H51&amp;"_win",IF(F51&gt;G51,H51&amp;"_lose",H51&amp;"_draw")))</f>
-        <v/>
+        <v>Bélgica_win</v>
       </c>
       <c r="U51" s="42" t="n">
         <f aca="false">IF(S51="",0,IF(VLOOKUP(E51,$AB$8:$AK$53,7,0)=VLOOKUP(H51,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39539,13 +39543,13 @@
         <f aca="false">IF(OR(E51=my_team,H51=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y51" s="40" t="str">
+      <c r="Y51" s="40" t="n">
         <f aca="false">IF(OR(F51="",G51=""),"",IF(F51&gt;G51,1,IF(F51&lt;G51,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA51" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN51))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB51" s="42" t="str">
         <f aca="false">VLOOKUP("Senegal",T,lang,0)</f>
@@ -39561,7 +39565,7 @@
       </c>
       <c r="AE51" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB51 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF51" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB51,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB51,$G$7:$G$54)</f>
@@ -39569,19 +39573,19 @@
       </c>
       <c r="AG51" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB51,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB51,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH51" s="40" t="n">
         <f aca="false">(AF51-AG51)*100+AK51*10000+AF51</f>
-        <v>40104</v>
+        <v>40004</v>
       </c>
       <c r="AI51" s="40" t="n">
         <f aca="false">AF51-AG51</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ51" s="40" t="n">
         <f aca="false">(AI51-AI55)/AI54</f>
-        <v>0.714285714285714</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="AK51" s="40" t="n">
         <f aca="false">AC51*3+AD51</f>
@@ -39597,11 +39601,11 @@
       </c>
       <c r="AN51" s="42" t="n">
         <f aca="false">1000*AK51/AK54+100*AJ51+10*AF51/AF54+1*AL51/AL54+AM51</f>
-        <v>882.409658589862</v>
+        <v>1053.83823001843</v>
       </c>
       <c r="AO51" s="43" t="str">
         <f aca="false">IF(SUM(AC50:AE53)=12,J52,INDEX(T,85,lang))</f>
-        <v>2H</v>
+        <v>Senegal</v>
       </c>
       <c r="AP51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB51&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB51&amp;"_win")*($U$7:$U$54))</f>
@@ -39648,19 +39652,23 @@
         <f aca="false">AB45</f>
         <v>Panamá</v>
       </c>
-      <c r="F52" s="64"/>
-      <c r="G52" s="65"/>
+      <c r="F52" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="65" t="n">
+        <v>2</v>
+      </c>
       <c r="H52" s="66" t="str">
         <f aca="false">AB46</f>
         <v>Túnez</v>
       </c>
       <c r="J52" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA50:AK53,2,0)</f>
-        <v>Japón</v>
+        <v>Senegal</v>
       </c>
       <c r="K52" s="76" t="n">
         <f aca="false">L52+M52+N52</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,3,0)</f>
@@ -39672,11 +39680,11 @@
       </c>
       <c r="N52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(2,AA50:AK53,7,0)</f>
-        <v>4 - 3</v>
+        <v>4 - 4</v>
       </c>
       <c r="P52" s="77" t="n">
         <f aca="false">L52*3+M52</f>
@@ -39688,11 +39696,11 @@
       </c>
       <c r="S52" s="41" t="str">
         <f aca="false">IF(OR(F52="",G52=""),"",IF(F52&gt;G52,E52&amp;"_win",IF(F52&lt;G52,E52&amp;"_lose",E52&amp;"_draw")))</f>
-        <v/>
+        <v>Panamá_lose</v>
       </c>
       <c r="T52" s="41" t="str">
         <f aca="false">IF(S52="","",IF(F52&lt;G52,H52&amp;"_win",IF(F52&gt;G52,H52&amp;"_lose",H52&amp;"_draw")))</f>
-        <v/>
+        <v>Túnez_win</v>
       </c>
       <c r="U52" s="42" t="n">
         <f aca="false">IF(S52="",0,IF(VLOOKUP(E52,$AB$8:$AK$53,7,0)=VLOOKUP(H52,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39710,13 +39718,13 @@
         <f aca="false">IF(OR(E52=my_team,H52=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y52" s="40" t="str">
+      <c r="Y52" s="40" t="n">
         <f aca="false">IF(OR(F52="",G52=""),"",IF(F52&gt;G52,1,IF(F52&lt;G52,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA52" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN52))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB52" s="42" t="str">
         <f aca="false">VLOOKUP("Colombia",T,lang,0)</f>
@@ -39724,7 +39732,7 @@
       </c>
       <c r="AC52" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD52" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_draw")</f>
@@ -39736,7 +39744,7 @@
       </c>
       <c r="AF52" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB52,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB52,$G$7:$G$54)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG52" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB52,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB52,$F$7:$F$54)</f>
@@ -39744,11 +39752,11 @@
       </c>
       <c r="AH52" s="40" t="n">
         <f aca="false">(AF52-AG52)*100+AK52*10000+AF52</f>
-        <v>30204</v>
+        <v>60305</v>
       </c>
       <c r="AI52" s="40" t="n">
         <f aca="false">AF52-AG52</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ52" s="40" t="n">
         <f aca="false">(AI52-AI55)/AI54</f>
@@ -39756,7 +39764,7 @@
       </c>
       <c r="AK52" s="40" t="n">
         <f aca="false">AC52*3+AD52</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL52" s="40" t="n">
         <f aca="false">AP52/AP54*1000+AQ52/AQ54*100+AT52/AT54*10+AR52/AR54</f>
@@ -39768,7 +39776,7 @@
       </c>
       <c r="AN52" s="42" t="n">
         <f aca="false">1000*AK52/AK54+100*AJ52+10*AF52/AF54+1*AL52/AL54+AM52</f>
-        <v>695.714824714286</v>
+        <v>1598.21482471429</v>
       </c>
       <c r="AP52" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB52&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB52&amp;"_win")*($U$7:$U$54))</f>
@@ -39815,19 +39823,23 @@
         <f aca="false">AB53</f>
         <v>Japón</v>
       </c>
-      <c r="F53" s="64"/>
-      <c r="G53" s="65"/>
+      <c r="F53" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="65" t="n">
+        <v>1</v>
+      </c>
       <c r="H53" s="66" t="str">
         <f aca="false">AB50</f>
         <v>Polonia</v>
       </c>
       <c r="J53" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA50:AK53,2,0)</f>
-        <v>Colombia</v>
+        <v>Japón</v>
       </c>
       <c r="K53" s="76" t="n">
         <f aca="false">L53+M53+N53</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L53" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA50:AK53,3,0)</f>
@@ -39835,7 +39847,7 @@
       </c>
       <c r="M53" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA50:AK53,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N53" s="76" t="n">
         <f aca="false">VLOOKUP(3,AA50:AK53,5,0)</f>
@@ -39843,11 +39855,11 @@
       </c>
       <c r="O53" s="76" t="str">
         <f aca="false">VLOOKUP(3,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(3,AA50:AK53,7,0)</f>
-        <v>4 - 2</v>
+        <v>4 - 4</v>
       </c>
       <c r="P53" s="77" t="n">
         <f aca="false">L53*3+M53</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R53" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -39855,11 +39867,11 @@
       </c>
       <c r="S53" s="41" t="str">
         <f aca="false">IF(OR(F53="",G53=""),"",IF(F53&gt;G53,E53&amp;"_win",IF(F53&lt;G53,E53&amp;"_lose",E53&amp;"_draw")))</f>
-        <v/>
+        <v>Japón_lose</v>
       </c>
       <c r="T53" s="41" t="str">
         <f aca="false">IF(S53="","",IF(F53&lt;G53,H53&amp;"_win",IF(F53&gt;G53,H53&amp;"_lose",H53&amp;"_draw")))</f>
-        <v/>
+        <v>Polonia_win</v>
       </c>
       <c r="U53" s="42" t="n">
         <f aca="false">IF(S53="",0,IF(VLOOKUP(E53,$AB$8:$AK$53,7,0)=VLOOKUP(H53,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39877,13 +39889,13 @@
         <f aca="false">IF(OR(E53=my_team,H53=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y53" s="40" t="str">
+      <c r="Y53" s="40" t="n">
         <f aca="false">IF(OR(F53="",G53=""),"",IF(F53&gt;G53,1,IF(F53&lt;G53,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA53" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN53))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB53" s="42" t="str">
         <f aca="false">VLOOKUP("Japan",T,lang,0)</f>
@@ -39899,7 +39911,7 @@
       </c>
       <c r="AE53" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB53 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF53" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB53,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB53,$G$7:$G$54)</f>
@@ -39907,19 +39919,19 @@
       </c>
       <c r="AG53" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB53,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB53,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH53" s="40" t="n">
         <f aca="false">(AF53-AG53)*100+AK53*10000+AF53</f>
-        <v>40104</v>
+        <v>40004</v>
       </c>
       <c r="AI53" s="40" t="n">
         <f aca="false">AF53-AG53</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ53" s="40" t="n">
         <f aca="false">(AI53-AI55)/AI54</f>
-        <v>0.714285714285714</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="AK53" s="40" t="n">
         <f aca="false">AC53*3+AD53</f>
@@ -39935,7 +39947,7 @@
       </c>
       <c r="AN53" s="42" t="n">
         <f aca="false">1000*AK53/AK54+100*AJ53+10*AF53/AF54+1*AL53/AL54+AM53</f>
-        <v>882.409516589862</v>
+        <v>1053.83808801843</v>
       </c>
       <c r="AP53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB53&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_win")*($U$7:$U$54))</f>
@@ -39978,8 +39990,12 @@
         <f aca="false">AB51</f>
         <v>Senegal</v>
       </c>
-      <c r="F54" s="83"/>
-      <c r="G54" s="84"/>
+      <c r="F54" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="84" t="n">
+        <v>1</v>
+      </c>
       <c r="H54" s="109" t="str">
         <f aca="false">AB52</f>
         <v>Colombia</v>
@@ -39990,11 +40006,11 @@
       </c>
       <c r="K54" s="88" t="n">
         <f aca="false">L54+M54+N54</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,4,0)</f>
@@ -40006,11 +40022,11 @@
       </c>
       <c r="O54" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(4,AA50:AK53,7,0)</f>
-        <v>1 - 5</v>
+        <v>2 - 5</v>
       </c>
       <c r="P54" s="89" t="n">
         <f aca="false">L54*3+M54</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R54" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -40018,11 +40034,11 @@
       </c>
       <c r="S54" s="41" t="str">
         <f aca="false">IF(OR(F54="",G54=""),"",IF(F54&gt;G54,E54&amp;"_win",IF(F54&lt;G54,E54&amp;"_lose",E54&amp;"_draw")))</f>
-        <v/>
+        <v>Senegal_lose</v>
       </c>
       <c r="T54" s="41" t="str">
         <f aca="false">IF(S54="","",IF(F54&lt;G54,H54&amp;"_win",IF(F54&gt;G54,H54&amp;"_lose",H54&amp;"_draw")))</f>
-        <v/>
+        <v>Colombia_win</v>
       </c>
       <c r="U54" s="42" t="n">
         <f aca="false">IF(S54="",0,IF(VLOOKUP(E54,$AB$8:$AK$53,7,0)=VLOOKUP(H54,$AB$8:$AK$53,7,0),1,0))</f>
@@ -40040,9 +40056,9 @@
         <f aca="false">IF(OR(E54=my_team,H54=my_team),1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y54" s="40" t="str">
+      <c r="Y54" s="40" t="n">
         <f aca="false">IF(OR(F54="",G54=""),"",IF(F54&gt;G54,1,IF(F54&lt;G54,-1,0)))</f>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AC54" s="40" t="n">
         <f aca="false">MAX(AC50:AC53)-MIN(AC50:AC53)+1</f>
@@ -40054,7 +40070,7 @@
       </c>
       <c r="AE54" s="40" t="n">
         <f aca="false">MAX(AE50:AE53)-MIN(AE50:AE53)+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF54" s="40" t="n">
         <f aca="false">MAX(AF50:AF53)-MIN(AF50:AF53)+1</f>
@@ -40066,7 +40082,7 @@
       </c>
       <c r="AH54" s="40" t="n">
         <f aca="false">MAX(AH50:AH53)-AH55+1</f>
-        <v>40504</v>
+        <v>30604</v>
       </c>
       <c r="AI54" s="40" t="n">
         <f aca="false">MAX(AI50:AI53)-AI55+1</f>
@@ -40074,7 +40090,7 @@
       </c>
       <c r="AK54" s="40" t="n">
         <f aca="false">MAX(AK50:AK53)-MIN(AK50:AK53)+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL54" s="40" t="n">
         <f aca="false">MAX(AL50:AL53)-MIN(AL50:AL53)+1</f>
@@ -40119,11 +40135,11 @@
       <c r="P55" s="92"/>
       <c r="AH55" s="40" t="n">
         <f aca="false">MIN(AH50:AH53)</f>
-        <v>-399</v>
+        <v>29702</v>
       </c>
       <c r="AI55" s="40" t="n">
         <f aca="false">MIN(AI50:AI53)</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Se actualizan resultados de los dias 30 de junio y 1 de julio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -14014,9 +14014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1485360</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14030,7 +14030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1232280"/>
-          <a:ext cx="223920" cy="146520"/>
+          <a:ext cx="223560" cy="146160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14051,9 +14051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485720</xdr:colOff>
+      <xdr:colOff>1485360</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14067,7 +14067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4276080"/>
-          <a:ext cx="223920" cy="146520"/>
+          <a:ext cx="223560" cy="146160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14088,9 +14088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14104,7 +14104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7324200"/>
-          <a:ext cx="223920" cy="146520"/>
+          <a:ext cx="223560" cy="146160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14125,9 +14125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14141,7 +14141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="1232280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14162,9 +14162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14178,7 +14178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4470840"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14199,9 +14199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14215,7 +14215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7519320"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14236,9 +14236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14252,7 +14252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1422720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14273,9 +14273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>248760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14289,7 +14289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5461560" y="4280760"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14310,9 +14310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14326,7 +14326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7519320"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14347,9 +14347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
+      <xdr:rowOff>179280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14363,7 +14363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1431720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14384,9 +14384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>184320</xdr:rowOff>
+      <xdr:rowOff>183960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14400,7 +14400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4484520"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14421,9 +14421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>175680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14437,7 +14437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7333560"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14458,9 +14458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14474,7 +14474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1613880"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14495,9 +14495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14511,7 +14511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4661280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14532,9 +14532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14548,7 +14548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7709760"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14569,9 +14569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14585,7 +14585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1613880"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14606,9 +14606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14622,7 +14622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4856400"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14643,9 +14643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14659,7 +14659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="7899840"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14680,9 +14680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14696,7 +14696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="7904520"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14717,9 +14717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14733,7 +14733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4661280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14754,9 +14754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14770,7 +14770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1799640"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,9 +14791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14807,7 +14807,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1804320"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14844,7 +14844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4847040"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14865,9 +14865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14881,7 +14881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7705080"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14902,9 +14902,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14918,7 +14918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1994760"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14939,9 +14939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14955,7 +14955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5042880"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14976,9 +14976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14992,7 +14992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8090280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15013,9 +15013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15029,7 +15029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1994760"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15050,9 +15050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15066,7 +15066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5228640"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15087,9 +15087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15103,7 +15103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8276040"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15124,9 +15124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15140,7 +15140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2184840"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15161,9 +15161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15177,7 +15177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="5042880"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15198,9 +15198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15214,7 +15214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8276040"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15235,9 +15235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15251,7 +15251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="2180160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15272,9 +15272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15288,7 +15288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5228640"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,9 +15309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15325,7 +15325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8085600"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15346,9 +15346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15362,7 +15362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2370600"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15383,9 +15383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15399,7 +15399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5423760"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15420,9 +15420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15436,7 +15436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="8467200"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15457,9 +15457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15473,7 +15473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="2375280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15494,9 +15494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15510,7 +15510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8662320"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15531,9 +15531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15547,7 +15547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5613840"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15568,9 +15568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15584,7 +15584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2565720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15605,9 +15605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239040</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15621,7 +15621,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5418360"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15642,9 +15642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15658,7 +15658,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455800" y="8656920"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15679,9 +15679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239040</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15695,7 +15695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2564640"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15732,7 +15732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926160" y="5612760"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15753,9 +15753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477440</xdr:colOff>
+      <xdr:colOff>1477080</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15769,7 +15769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8466480"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15806,7 +15806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2757960"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15827,9 +15827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15843,7 +15843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5800680"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15864,9 +15864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15880,7 +15880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="8849160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15901,9 +15901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>196200</xdr:colOff>
+      <xdr:colOff>195840</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15917,7 +15917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481720" y="2753280"/>
-          <a:ext cx="147960" cy="147960"/>
+          <a:ext cx="147600" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15938,9 +15938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>191520</xdr:colOff>
+      <xdr:colOff>191160</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15954,7 +15954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5477040" y="5991120"/>
-          <a:ext cx="147960" cy="147960"/>
+          <a:ext cx="147600" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15975,9 +15975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1439280</xdr:colOff>
+      <xdr:colOff>1438920</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15991,7 +15991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956760" y="9039240"/>
-          <a:ext cx="147960" cy="147960"/>
+          <a:ext cx="147600" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16012,9 +16012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16028,7 +16028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2943720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16049,9 +16049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16065,7 +16065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="5800680"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16086,9 +16086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16102,7 +16102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9039240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,9 +16123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16139,7 +16139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="2943720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16160,9 +16160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16176,7 +16176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5991120"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16197,9 +16197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16213,7 +16213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="8849160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16234,9 +16234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16250,7 +16250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3134160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16271,9 +16271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16287,7 +16287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6182280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16308,9 +16308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16324,7 +16324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9229680"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16345,9 +16345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16361,7 +16361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3138840"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16382,9 +16382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16398,7 +16398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6372720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16419,9 +16419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16435,7 +16435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9420120"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16456,9 +16456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16472,7 +16472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3324240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16493,9 +16493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16509,7 +16509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6182280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16530,9 +16530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16546,7 +16546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9420120"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16567,9 +16567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16583,7 +16583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3324240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16604,9 +16604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16620,7 +16620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6372720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16641,9 +16641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16657,7 +16657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9229680"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16678,9 +16678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1461960</xdr:colOff>
+      <xdr:colOff>1461600</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16694,7 +16694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="3514680"/>
-          <a:ext cx="175320" cy="147960"/>
+          <a:ext cx="174960" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16715,9 +16715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1461960</xdr:colOff>
+      <xdr:colOff>1461600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16731,7 +16731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="6563160"/>
-          <a:ext cx="175320" cy="147960"/>
+          <a:ext cx="174960" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16752,9 +16752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>214200</xdr:colOff>
+      <xdr:colOff>213840</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16768,7 +16768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5472360" y="9611280"/>
-          <a:ext cx="175320" cy="147960"/>
+          <a:ext cx="174960" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16789,9 +16789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16805,7 +16805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3514680"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16826,9 +16826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16842,7 +16842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6753240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16863,9 +16863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16879,7 +16879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9801720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16900,9 +16900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16916,7 +16916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3705120"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16937,9 +16937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16953,7 +16953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6563160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16974,9 +16974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16990,7 +16990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9801720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17011,9 +17011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17027,7 +17027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3896280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17048,9 +17048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17064,7 +17064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6943680"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17085,9 +17085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17101,7 +17101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9992160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17122,9 +17122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17138,7 +17138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3900960"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17159,9 +17159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17175,7 +17175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="7134120"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17196,9 +17196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17212,7 +17212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="10182240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17233,9 +17233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17249,7 +17249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="4091400"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17270,9 +17270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17286,7 +17286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6948360"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17307,9 +17307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17323,7 +17323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="10182240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17344,9 +17344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17360,7 +17360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="4086720"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17381,9 +17381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17397,7 +17397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="7134120"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17418,9 +17418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17434,7 +17434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9992160"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17455,9 +17455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>245160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17471,7 +17471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3709800"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17492,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483920</xdr:colOff>
+      <xdr:colOff>1483560</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17508,7 +17508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6753240"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17529,9 +17529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1479240</xdr:colOff>
+      <xdr:colOff>1478880</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17545,7 +17545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9611280"/>
-          <a:ext cx="221040" cy="147960"/>
+          <a:ext cx="220680" cy="147600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31724,8 +31724,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AZ30" activeCellId="0" sqref="AZ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32646,7 +32646,9 @@
         <f aca="false">AO8</f>
         <v>Uruguay</v>
       </c>
-      <c r="BA10" s="80"/>
+      <c r="BA10" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="BB10" s="81"/>
       <c r="BC10" s="70"/>
       <c r="BD10" s="70"/>
@@ -32838,7 +32840,9 @@
         <f aca="false">AO15</f>
         <v>Portugal</v>
       </c>
-      <c r="BA11" s="83"/>
+      <c r="BA11" s="83" t="n">
+        <v>1</v>
+      </c>
       <c r="BB11" s="84"/>
       <c r="BC11" s="85"/>
       <c r="BD11" s="70"/>
@@ -33019,7 +33023,7 @@
       </c>
       <c r="BF12" s="79" t="str">
         <f aca="false">T58</f>
-        <v>W49</v>
+        <v>Uruguay</v>
       </c>
       <c r="BG12" s="80"/>
       <c r="BH12" s="81"/>
@@ -33125,7 +33129,7 @@
       <c r="BE13" s="78"/>
       <c r="BF13" s="82" t="str">
         <f aca="false">T59</f>
-        <v>W50</v>
+        <v>Francia</v>
       </c>
       <c r="BG13" s="83"/>
       <c r="BH13" s="84"/>
@@ -33319,7 +33323,9 @@
         <f aca="false">AO20</f>
         <v>Francia</v>
       </c>
-      <c r="BA14" s="80"/>
+      <c r="BA14" s="80" t="n">
+        <v>4</v>
+      </c>
       <c r="BB14" s="81"/>
       <c r="BC14" s="94"/>
       <c r="BD14" s="70"/>
@@ -33515,7 +33521,9 @@
         <f aca="false">AO27</f>
         <v>Argentina</v>
       </c>
-      <c r="BA15" s="83"/>
+      <c r="BA15" s="83" t="n">
+        <v>3</v>
+      </c>
       <c r="BB15" s="84"/>
       <c r="BC15" s="70"/>
       <c r="BD15" s="70"/>
@@ -34971,7 +34979,7 @@
       <c r="AY23" s="78"/>
       <c r="AZ23" s="82" t="str">
         <f aca="false">AO51</f>
-        <v>Senegal</v>
+        <v>Japón</v>
       </c>
       <c r="BA23" s="83"/>
       <c r="BB23" s="84"/>
@@ -35450,8 +35458,12 @@
         <f aca="false">AO14</f>
         <v>España</v>
       </c>
-      <c r="BA26" s="80"/>
-      <c r="BB26" s="81"/>
+      <c r="BA26" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB26" s="81" t="n">
+        <v>3</v>
+      </c>
       <c r="BC26" s="70"/>
       <c r="BD26" s="70"/>
       <c r="BE26" s="70"/>
@@ -35646,8 +35658,12 @@
         <f aca="false">AO9</f>
         <v>Rusia</v>
       </c>
-      <c r="BA27" s="83"/>
-      <c r="BB27" s="84"/>
+      <c r="BA27" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB27" s="84" t="n">
+        <v>4</v>
+      </c>
       <c r="BC27" s="85"/>
       <c r="BD27" s="70"/>
       <c r="BE27" s="70" t="str">
@@ -35847,7 +35863,7 @@
       </c>
       <c r="BF28" s="79" t="str">
         <f aca="false">T60</f>
-        <v>W51</v>
+        <v>Rusia</v>
       </c>
       <c r="BG28" s="80"/>
       <c r="BH28" s="81"/>
@@ -37477,15 +37493,15 @@
       </c>
       <c r="U38" s="42" t="n">
         <f aca="false">IF(S38="",0,IF(VLOOKUP(E38,$AB$8:$AK$53,7,0)=VLOOKUP(H38,$AB$8:$AK$53,7,0),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V38" s="40" t="n">
         <f aca="false">U38*F38</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W38" s="40" t="n">
         <f aca="false">U38*G38</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X38" s="40" t="n">
         <f aca="false">IF(OR(E38=my_team,H38=my_team),1,0)</f>
@@ -39382,11 +39398,11 @@
       </c>
       <c r="AC50" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_win")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD50" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE50" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_lose")</f>
@@ -39398,15 +39414,15 @@
       </c>
       <c r="AG50" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB50,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB50,$F$7:$F$54)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH50" s="40" t="n">
         <f aca="false">(AF50-AG50)*100+AK50*10000+AF50</f>
-        <v>29702</v>
+        <v>9602</v>
       </c>
       <c r="AI50" s="40" t="n">
         <f aca="false">AF50-AG50</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AJ50" s="40" t="n">
         <f aca="false">(AI50-AI55)/AI54</f>
@@ -39414,7 +39430,7 @@
       </c>
       <c r="AK50" s="40" t="n">
         <f aca="false">AC50*3+AD50</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL50" s="40" t="n">
         <f aca="false">AP50/AP54*1000+AQ50/AQ54*100+AT50/AT54*10+AR50/AR54</f>
@@ -39426,7 +39442,7 @@
       </c>
       <c r="AN50" s="42" t="n">
         <f aca="false">1000*AK50/AK54+100*AJ50+10*AF50/AF54+1*AL50/AL54+AM50</f>
-        <v>755.0006045</v>
+        <v>171.667271166667</v>
       </c>
       <c r="AO50" s="43" t="str">
         <f aca="false">IF(SUM(AC50:AE53)=12,J51,INDEX(T,84,lang))</f>
@@ -39549,7 +39565,7 @@
       </c>
       <c r="AA51" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN51))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB51" s="42" t="str">
         <f aca="false">VLOOKUP("Senegal",T,lang,0)</f>
@@ -39585,7 +39601,7 @@
       </c>
       <c r="AJ51" s="40" t="n">
         <f aca="false">(AI51-AI55)/AI54</f>
-        <v>0.428571428571429</v>
+        <v>0.5</v>
       </c>
       <c r="AK51" s="40" t="n">
         <f aca="false">AC51*3+AD51</f>
@@ -39593,7 +39609,7 @@
       </c>
       <c r="AL51" s="40" t="n">
         <f aca="false">AP51/AP54*1000+AQ51/AQ54*100+AT51/AT54*10+AR51/AR54</f>
-        <v>50.6666666666667</v>
+        <v>0</v>
       </c>
       <c r="AM51" s="40" t="n">
         <f aca="false">VLOOKUP(AB51,db_fifarank,2,0)/2000000</f>
@@ -39601,11 +39617,11 @@
       </c>
       <c r="AN51" s="42" t="n">
         <f aca="false">1000*AK51/AK54+100*AJ51+10*AF51/AF54+1*AL51/AL54+AM51</f>
-        <v>1053.83823001843</v>
+        <v>726.667108666667</v>
       </c>
       <c r="AO51" s="43" t="str">
         <f aca="false">IF(SUM(AC50:AE53)=12,J52,INDEX(T,85,lang))</f>
-        <v>Senegal</v>
+        <v>Japón</v>
       </c>
       <c r="AP51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB51&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB51&amp;"_win")*($U$7:$U$54))</f>
@@ -39613,15 +39629,15 @@
       </c>
       <c r="AQ51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB51&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB51&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB51)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB51)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS51" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB51)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB51)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT51" s="44" t="n">
         <f aca="false">AR51-AS51</f>
@@ -39664,7 +39680,7 @@
       </c>
       <c r="J52" s="75" t="str">
         <f aca="false">VLOOKUP(2,AA50:AK53,2,0)</f>
-        <v>Senegal</v>
+        <v>Japón</v>
       </c>
       <c r="K52" s="76" t="n">
         <f aca="false">L52+M52+N52</f>
@@ -39676,19 +39692,19 @@
       </c>
       <c r="M52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N52" s="76" t="n">
         <f aca="false">VLOOKUP(2,AA50:AK53,5,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O52" s="76" t="str">
         <f aca="false">VLOOKUP(2,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(2,AA50:AK53,7,0)</f>
-        <v>4 - 4</v>
+        <v>5 - 4</v>
       </c>
       <c r="P52" s="77" t="n">
         <f aca="false">L52*3+M52</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R52" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(7,0,0)+gmt_delta</f>
@@ -39760,7 +39776,7 @@
       </c>
       <c r="AJ52" s="40" t="n">
         <f aca="false">(AI52-AI55)/AI54</f>
-        <v>0.857142857142857</v>
+        <v>0.875</v>
       </c>
       <c r="AK52" s="40" t="n">
         <f aca="false">AC52*3+AD52</f>
@@ -39776,7 +39792,7 @@
       </c>
       <c r="AN52" s="42" t="n">
         <f aca="false">1000*AK52/AK54+100*AJ52+10*AF52/AF54+1*AL52/AL54+AM52</f>
-        <v>1598.21482471429</v>
+        <v>1100.000539</v>
       </c>
       <c r="AP52" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB52&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB52&amp;"_win")*($U$7:$U$54))</f>
@@ -39824,7 +39840,7 @@
         <v>Japón</v>
       </c>
       <c r="F53" s="64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="65" t="n">
         <v>1</v>
@@ -39835,7 +39851,7 @@
       </c>
       <c r="J53" s="75" t="str">
         <f aca="false">VLOOKUP(3,AA50:AK53,2,0)</f>
-        <v>Japón</v>
+        <v>Senegal</v>
       </c>
       <c r="K53" s="76" t="n">
         <f aca="false">L53+M53+N53</f>
@@ -39867,11 +39883,11 @@
       </c>
       <c r="S53" s="41" t="str">
         <f aca="false">IF(OR(F53="",G53=""),"",IF(F53&gt;G53,E53&amp;"_win",IF(F53&lt;G53,E53&amp;"_lose",E53&amp;"_draw")))</f>
-        <v>Japón_lose</v>
+        <v>Japón_draw</v>
       </c>
       <c r="T53" s="41" t="str">
         <f aca="false">IF(S53="","",IF(F53&lt;G53,H53&amp;"_win",IF(F53&gt;G53,H53&amp;"_lose",H53&amp;"_draw")))</f>
-        <v>Polonia_win</v>
+        <v>Polonia_draw</v>
       </c>
       <c r="U53" s="42" t="n">
         <f aca="false">IF(S53="",0,IF(VLOOKUP(E53,$AB$8:$AK$53,7,0)=VLOOKUP(H53,$AB$8:$AK$53,7,0),1,0))</f>
@@ -39891,11 +39907,11 @@
       </c>
       <c r="Y53" s="40" t="n">
         <f aca="false">IF(OR(F53="",G53=""),"",IF(F53&gt;G53,1,IF(F53&lt;G53,-1,0)))</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA53" s="40" t="n">
         <f aca="false">COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN53))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB53" s="42" t="str">
         <f aca="false">VLOOKUP("Japan",T,lang,0)</f>
@@ -39907,15 +39923,15 @@
       </c>
       <c r="AD53" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB53 &amp; "_draw")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE53" s="40" t="n">
         <f aca="false">COUNTIF($S$7:$T$54,"=" &amp; AB53 &amp; "_lose")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF53" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB53,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB53,$G$7:$G$54)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG53" s="40" t="n">
         <f aca="false">SUMIF($E$7:$E$54,$AB53,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB53,$F$7:$F$54)</f>
@@ -39923,23 +39939,23 @@
       </c>
       <c r="AH53" s="40" t="n">
         <f aca="false">(AF53-AG53)*100+AK53*10000+AF53</f>
-        <v>40004</v>
+        <v>50105</v>
       </c>
       <c r="AI53" s="40" t="n">
         <f aca="false">AF53-AG53</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ53" s="40" t="n">
         <f aca="false">(AI53-AI55)/AI54</f>
-        <v>0.428571428571429</v>
+        <v>0.625</v>
       </c>
       <c r="AK53" s="40" t="n">
         <f aca="false">AC53*3+AD53</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL53" s="40" t="n">
         <f aca="false">AP53/AP54*1000+AQ53/AQ54*100+AT53/AT54*10+AR53/AR54</f>
-        <v>50.6666666666667</v>
+        <v>0</v>
       </c>
       <c r="AM53" s="40" t="n">
         <f aca="false">VLOOKUP(AB53,db_fifarank,2,0)/2000000</f>
@@ -39947,7 +39963,7 @@
       </c>
       <c r="AN53" s="42" t="n">
         <f aca="false">1000*AK53/AK54+100*AJ53+10*AF53/AF54+1*AL53/AL54+AM53</f>
-        <v>1053.83808801843</v>
+        <v>908.333633333333</v>
       </c>
       <c r="AP53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB53&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_win")*($U$7:$U$54))</f>
@@ -39955,15 +39971,15 @@
       </c>
       <c r="AQ53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($S$7:$S$54=AB53&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB53)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB53)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS53" s="44" t="n">
         <f aca="false">SUMPRODUCT(($E$7:$E$54=AB53)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB53)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT53" s="44" t="n">
         <f aca="false">AR53-AS53</f>
@@ -40010,11 +40026,11 @@
       </c>
       <c r="L54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,3,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N54" s="88" t="n">
         <f aca="false">VLOOKUP(4,AA50:AK53,5,0)</f>
@@ -40022,11 +40038,11 @@
       </c>
       <c r="O54" s="88" t="str">
         <f aca="false">VLOOKUP(4,AA50:AK53,6,0) &amp; " - " &amp; VLOOKUP(4,AA50:AK53,7,0)</f>
-        <v>2 - 5</v>
+        <v>2 - 6</v>
       </c>
       <c r="P54" s="89" t="n">
         <f aca="false">L54*3+M54</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R54" s="40" t="n">
         <f aca="false">DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -40062,15 +40078,15 @@
       </c>
       <c r="AC54" s="40" t="n">
         <f aca="false">MAX(AC50:AC53)-MIN(AC50:AC53)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD54" s="40" t="n">
         <f aca="false">MAX(AD50:AD53)-MIN(AD50:AD53)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE54" s="40" t="n">
         <f aca="false">MAX(AE50:AE53)-MIN(AE50:AE53)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF54" s="40" t="n">
         <f aca="false">MAX(AF50:AF53)-MIN(AF50:AF53)+1</f>
@@ -40078,23 +40094,23 @@
       </c>
       <c r="AG54" s="40" t="n">
         <f aca="false">MAX(AG50:AG53)-MIN(AG50:AG53)+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH54" s="40" t="n">
         <f aca="false">MAX(AH50:AH53)-AH55+1</f>
-        <v>30604</v>
+        <v>50704</v>
       </c>
       <c r="AI54" s="40" t="n">
         <f aca="false">MAX(AI50:AI53)-AI55+1</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AK54" s="40" t="n">
         <f aca="false">MAX(AK50:AK53)-MIN(AK50:AK53)+1</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AL54" s="40" t="n">
         <f aca="false">MAX(AL50:AL53)-MIN(AL50:AL53)+1</f>
-        <v>51.6666666666667</v>
+        <v>1</v>
       </c>
       <c r="AP54" s="40" t="n">
         <f aca="false">MAX(AP50:AP53)-MIN(AP50:AP53)+1</f>
@@ -40102,15 +40118,15 @@
       </c>
       <c r="AQ54" s="40" t="n">
         <f aca="false">MAX(AQ50:AQ53)-MIN(AQ50:AQ53)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR54" s="40" t="n">
         <f aca="false">MAX(AR50:AR53)-MIN(AR50:AR53)+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AS54" s="40" t="n">
         <f aca="false">MAX(AS50:AS53)-MIN(AS50:AS53)+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT54" s="40" t="n">
         <f aca="false">MAX(AT50:AT53)-MIN(AT50:AT53)+1</f>
@@ -40135,11 +40151,11 @@
       <c r="P55" s="92"/>
       <c r="AH55" s="40" t="n">
         <f aca="false">MIN(AH50:AH53)</f>
-        <v>29702</v>
+        <v>9602</v>
       </c>
       <c r="AI55" s="40" t="n">
         <f aca="false">MIN(AI50:AI53)</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -40151,11 +40167,11 @@
       </c>
       <c r="S58" s="41" t="str">
         <f aca="false">IF(OR(BA10="",BA11=""),"",IF(BA10&gt;BA11,AZ10,IF(BA10&lt;BA11,AZ11,IF(OR(BB10="",BB11=""),"draw",IF(BB10&gt;BB11,AZ10,IF(BB10&lt;BB11,AZ11,"draw"))))))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="T58" s="41" t="str">
         <f aca="false">IF(OR(S58="",S58="draw"),INDEX(T,86,lang),S58)</f>
-        <v>W49</v>
+        <v>Uruguay</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40165,11 +40181,11 @@
       </c>
       <c r="S59" s="41" t="str">
         <f aca="false">IF(OR(BA14="",BA15=""),"",IF(BA14&gt;BA15,AZ14,IF(BA14&lt;BA15,AZ15,IF(OR(BB14="",BB15=""),"draw",IF(BB14&gt;BB15,AZ14,IF(BB14&lt;BB15,AZ15,"draw"))))))</f>
-        <v/>
+        <v>Francia</v>
       </c>
       <c r="T59" s="41" t="str">
         <f aca="false">IF(OR(S59="",S59="draw"),INDEX(T,87,lang),S59)</f>
-        <v>W50</v>
+        <v>Francia</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40179,11 +40195,11 @@
       </c>
       <c r="S60" s="41" t="str">
         <f aca="false">IF(OR(BA26="",BA27=""),"",IF(BA26&gt;BA27,AZ26,IF(BA26&lt;BA27,AZ27,IF(OR(BB26="",BB27=""),"draw",IF(BB26&gt;BB27,AZ26,IF(BB26&lt;BB27,AZ27,"draw"))))))</f>
-        <v/>
+        <v>Rusia</v>
       </c>
       <c r="T60" s="41" t="str">
         <f aca="false">IF(OR(S60="",S60="draw"),INDEX(T,88,lang),S60)</f>
-        <v>W51</v>
+        <v>Rusia</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Resultados actualizados al dia 2 de julio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -14014,9 +14014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14030,7 +14030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1232280"/>
-          <a:ext cx="223560" cy="146160"/>
+          <a:ext cx="222840" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14051,9 +14051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1485360</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14067,7 +14067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4276080"/>
-          <a:ext cx="223560" cy="146160"/>
+          <a:ext cx="222840" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14088,9 +14088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246960</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14104,7 +14104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7324200"/>
-          <a:ext cx="223560" cy="146160"/>
+          <a:ext cx="222840" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14125,9 +14125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14141,7 +14141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="1232280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14162,9 +14162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14178,7 +14178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4470840"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14199,9 +14199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14215,7 +14215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7519320"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14236,9 +14236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14252,7 +14252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1422720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14273,9 +14273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14289,7 +14289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5461560" y="4280760"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14310,9 +14310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14326,7 +14326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7519320"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14347,9 +14347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:rowOff>178560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14363,7 +14363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1431720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14384,9 +14384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>183960</xdr:rowOff>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14400,7 +14400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4484520"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14421,9 +14421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>175680</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14437,7 +14437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7333560"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14458,9 +14458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14474,7 +14474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1613880"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14495,9 +14495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14511,7 +14511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4661280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14532,9 +14532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14548,7 +14548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7709760"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14569,9 +14569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14585,7 +14585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1613880"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14606,9 +14606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14622,7 +14622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4856400"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14643,9 +14643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1477080</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14659,7 +14659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="7899840"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14680,9 +14680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14696,7 +14696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="7904520"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14717,9 +14717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14733,7 +14733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4661280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14754,9 +14754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14770,7 +14770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1799640"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,9 +14791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14807,7 +14807,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1804320"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14844,7 +14844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4847040"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14865,9 +14865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14881,7 +14881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7705080"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14902,9 +14902,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14918,7 +14918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1994760"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14939,9 +14939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14955,7 +14955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5042880"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14976,9 +14976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14992,7 +14992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8090280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15013,9 +15013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15029,7 +15029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1994760"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15050,9 +15050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15066,7 +15066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5228640"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15087,9 +15087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1477080</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15103,7 +15103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8276040"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15124,9 +15124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15140,7 +15140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2184840"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15161,9 +15161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15177,7 +15177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="5042880"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15198,9 +15198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15214,7 +15214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8276040"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15235,9 +15235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15251,7 +15251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="2180160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15272,9 +15272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15288,7 +15288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5228640"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,9 +15309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1477080</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15325,7 +15325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8085600"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15346,9 +15346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15362,7 +15362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2370600"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15383,9 +15383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15399,7 +15399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5423760"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15420,9 +15420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15436,7 +15436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="8467200"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15457,9 +15457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15473,7 +15473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="2375280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15494,9 +15494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1477080</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15510,7 +15510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8662320"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15531,9 +15531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15547,7 +15547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5613840"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15568,9 +15568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481760</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15584,7 +15584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2565720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15605,9 +15605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>237960</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15621,7 +15621,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5418360"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15642,9 +15642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>242280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15658,7 +15658,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455800" y="8656920"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15679,9 +15679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>237960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15695,7 +15695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2564640"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15732,7 +15732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926160" y="5612760"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15753,9 +15753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477080</xdr:colOff>
+      <xdr:colOff>1476360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15769,7 +15769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8466480"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15806,7 +15806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2757960"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15827,9 +15827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15843,7 +15843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5800680"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15864,9 +15864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15880,7 +15880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="8849160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15901,9 +15901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>195840</xdr:colOff>
+      <xdr:colOff>195120</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15917,7 +15917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481720" y="2753280"/>
-          <a:ext cx="147600" cy="147600"/>
+          <a:ext cx="146880" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15938,9 +15938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>191160</xdr:colOff>
+      <xdr:colOff>190440</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15954,7 +15954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5477040" y="5991120"/>
-          <a:ext cx="147600" cy="147600"/>
+          <a:ext cx="146880" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15975,9 +15975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1438920</xdr:colOff>
+      <xdr:colOff>1438200</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15991,7 +15991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956760" y="9039240"/>
-          <a:ext cx="147600" cy="147600"/>
+          <a:ext cx="146880" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16012,9 +16012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16028,7 +16028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2943720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16049,9 +16049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16065,7 +16065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="5800680"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16086,9 +16086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16102,7 +16102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9039240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,9 +16123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16139,7 +16139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="2943720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16160,9 +16160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16176,7 +16176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5991120"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16197,9 +16197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16213,7 +16213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="8849160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16234,9 +16234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16250,7 +16250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3134160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16271,9 +16271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16287,7 +16287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6182280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16308,9 +16308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16324,7 +16324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9229680"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16345,9 +16345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16361,7 +16361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3138840"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16382,9 +16382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16398,7 +16398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6372720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16419,9 +16419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16435,7 +16435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9420120"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16456,9 +16456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16472,7 +16472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3324240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16493,9 +16493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16509,7 +16509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6182280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16530,9 +16530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16546,7 +16546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9420120"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16567,9 +16567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16583,7 +16583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3324240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16604,9 +16604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16620,7 +16620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6372720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16641,9 +16641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16657,7 +16657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9229680"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16678,9 +16678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1461600</xdr:colOff>
+      <xdr:colOff>1460880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16694,7 +16694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="3514680"/>
-          <a:ext cx="174960" cy="147600"/>
+          <a:ext cx="174240" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16715,9 +16715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1461600</xdr:colOff>
+      <xdr:colOff>1460880</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16731,7 +16731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="6563160"/>
-          <a:ext cx="174960" cy="147600"/>
+          <a:ext cx="174240" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16752,9 +16752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>213840</xdr:colOff>
+      <xdr:colOff>213120</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16768,7 +16768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5472360" y="9611280"/>
-          <a:ext cx="174960" cy="147600"/>
+          <a:ext cx="174240" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16789,9 +16789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16805,7 +16805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3514680"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16826,9 +16826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16842,7 +16842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6753240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16863,9 +16863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16879,7 +16879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9801720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16900,9 +16900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16916,7 +16916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3705120"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16937,9 +16937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16953,7 +16953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6563160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16974,9 +16974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16990,7 +16990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9801720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17011,9 +17011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17027,7 +17027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3896280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17048,9 +17048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17064,7 +17064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6943680"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17085,9 +17085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17101,7 +17101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9992160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17122,9 +17122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17138,7 +17138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3900960"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17159,9 +17159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17175,7 +17175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="7134120"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17196,9 +17196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17212,7 +17212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="10182240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17233,9 +17233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17249,7 +17249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="4091400"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17270,9 +17270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17286,7 +17286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6948360"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17307,9 +17307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17323,7 +17323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="10182240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17344,9 +17344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17360,7 +17360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="4086720"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17381,9 +17381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17397,7 +17397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="7134120"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17418,9 +17418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17434,7 +17434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9992160"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17455,9 +17455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244440</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17471,7 +17471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3709800"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17492,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483560</xdr:colOff>
+      <xdr:colOff>1482840</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17508,7 +17508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6753240"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17529,9 +17529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478880</xdr:colOff>
+      <xdr:colOff>1478160</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17545,7 +17545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9611280"/>
-          <a:ext cx="220680" cy="147600"/>
+          <a:ext cx="219960" cy="146880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31724,8 +31724,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ30" activeCellId="0" sqref="AZ30"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AZ24" activeCellId="0" sqref="AZ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34089,7 +34089,9 @@
         <f aca="false">AO32</f>
         <v>Brasil</v>
       </c>
-      <c r="BA18" s="80"/>
+      <c r="BA18" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="BB18" s="81"/>
       <c r="BC18" s="70"/>
       <c r="BD18" s="70"/>
@@ -34192,7 +34194,9 @@
         <f aca="false">AO39</f>
         <v>México</v>
       </c>
-      <c r="BA19" s="83"/>
+      <c r="BA19" s="83" t="n">
+        <v>0</v>
+      </c>
       <c r="BB19" s="84"/>
       <c r="BC19" s="85"/>
       <c r="BD19" s="70"/>
@@ -34397,7 +34401,7 @@
       </c>
       <c r="BF20" s="79" t="str">
         <f aca="false">T62</f>
-        <v>W53</v>
+        <v>Brasil</v>
       </c>
       <c r="BG20" s="80"/>
       <c r="BH20" s="81"/>
@@ -34596,7 +34600,7 @@
       <c r="BE21" s="78"/>
       <c r="BF21" s="82" t="str">
         <f aca="false">T63</f>
-        <v>W54</v>
+        <v>Bélgica</v>
       </c>
       <c r="BG21" s="83"/>
       <c r="BH21" s="84"/>
@@ -34786,7 +34790,9 @@
         <f aca="false">AO44</f>
         <v>Bélgica</v>
       </c>
-      <c r="BA22" s="80"/>
+      <c r="BA22" s="80" t="n">
+        <v>3</v>
+      </c>
       <c r="BB22" s="81"/>
       <c r="BC22" s="94"/>
       <c r="BD22" s="70"/>
@@ -34981,7 +34987,9 @@
         <f aca="false">AO51</f>
         <v>Japón</v>
       </c>
-      <c r="BA23" s="83"/>
+      <c r="BA23" s="83" t="n">
+        <v>2</v>
+      </c>
       <c r="BB23" s="84"/>
       <c r="BC23" s="70"/>
       <c r="BD23" s="70"/>
@@ -36058,7 +36066,7 @@
       <c r="BE29" s="78"/>
       <c r="BF29" s="82" t="str">
         <f aca="false">T61</f>
-        <v>W52</v>
+        <v>Croacia</v>
       </c>
       <c r="BG29" s="83"/>
       <c r="BH29" s="84"/>
@@ -36228,8 +36236,12 @@
         <f aca="false">AO26</f>
         <v>Croacia</v>
       </c>
-      <c r="BA30" s="80"/>
-      <c r="BB30" s="81"/>
+      <c r="BA30" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB30" s="81" t="n">
+        <v>4</v>
+      </c>
       <c r="BC30" s="94"/>
       <c r="BD30" s="70"/>
       <c r="BE30" s="70"/>
@@ -36324,8 +36336,12 @@
         <f aca="false">AO21</f>
         <v>Dinamarca</v>
       </c>
-      <c r="BA31" s="83"/>
-      <c r="BB31" s="84"/>
+      <c r="BA31" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB31" s="84" t="n">
+        <v>3</v>
+      </c>
       <c r="BC31" s="70"/>
       <c r="BD31" s="70"/>
       <c r="BE31" s="70"/>
@@ -40209,11 +40225,11 @@
       </c>
       <c r="S61" s="41" t="str">
         <f aca="false">IF(OR(BA30="",BA31=""),"",IF(BA30&gt;BA31,AZ30,IF(BA30&lt;BA31,AZ31,IF(OR(BB30="",BB31=""),"draw",IF(BB30&gt;BB31,AZ30,IF(BB30&lt;BB31,AZ31,"draw"))))))</f>
-        <v/>
+        <v>Croacia</v>
       </c>
       <c r="T61" s="41" t="str">
         <f aca="false">IF(OR(S61="",S61="draw"),INDEX(T,89,lang),S61)</f>
-        <v>W52</v>
+        <v>Croacia</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40223,11 +40239,11 @@
       </c>
       <c r="S62" s="41" t="str">
         <f aca="false">IF(OR(BA18="",BA19=""),"",IF(BA18&gt;BA19,AZ18,IF(BA18&lt;BA19,AZ19,IF(OR(BB18="",BB19=""),"draw",IF(BB18&gt;BB19,AZ18,IF(BB18&lt;BB19,AZ19,"draw"))))))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="T62" s="41" t="str">
         <f aca="false">IF(OR(S62="",S62="draw"),INDEX(T,90,lang),S62)</f>
-        <v>W53</v>
+        <v>Brasil</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40237,11 +40253,11 @@
       </c>
       <c r="S63" s="41" t="str">
         <f aca="false">IF(OR(BA22="",BA23=""),"",IF(BA22&gt;BA23,AZ22,IF(BA22&lt;BA23,AZ23,IF(OR(BB22="",BB23=""),"draw",IF(BB22&gt;BB23,AZ22,IF(BB22&lt;BB23,AZ23,"draw"))))))</f>
-        <v/>
+        <v>Bélgica</v>
       </c>
       <c r="T63" s="41" t="str">
         <f aca="false">IF(OR(S63="",S63="draw"),INDEX(T,91,lang),S63)</f>
-        <v>W54</v>
+        <v>Bélgica</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Resultados actualizados al dia 3 de julio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -14014,9 +14014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1484280</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14030,7 +14030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1232280"/>
-          <a:ext cx="222840" cy="145440"/>
+          <a:ext cx="222480" cy="145080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14051,9 +14051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484640</xdr:colOff>
+      <xdr:colOff>1484280</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14067,7 +14067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4276080"/>
-          <a:ext cx="222840" cy="145440"/>
+          <a:ext cx="222480" cy="145080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14088,9 +14088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245880</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14104,7 +14104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7324200"/>
-          <a:ext cx="222840" cy="145440"/>
+          <a:ext cx="222480" cy="145080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14125,9 +14125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14141,7 +14141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="1232280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14162,9 +14162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14178,7 +14178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4470840"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14199,9 +14199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14215,7 +14215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7519320"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14236,9 +14236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14252,7 +14252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1422720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14273,9 +14273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14289,7 +14289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5461560" y="4280760"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14310,9 +14310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14326,7 +14326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7519320"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14347,9 +14347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>178560</xdr:rowOff>
+      <xdr:rowOff>178200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14363,7 +14363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1431720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14384,9 +14384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14400,7 +14400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4484520"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14421,9 +14421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14437,7 +14437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7333560"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14458,9 +14458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14474,7 +14474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1613880"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14495,9 +14495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14511,7 +14511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4661280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14532,9 +14532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14548,7 +14548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7709760"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14569,9 +14569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14585,7 +14585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1613880"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14606,9 +14606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14622,7 +14622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4856400"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14643,9 +14643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477080</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14659,7 +14659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="7899840"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14680,9 +14680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14696,7 +14696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="7904520"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14717,9 +14717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14733,7 +14733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4661280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14754,9 +14754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14770,7 +14770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1799640"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,9 +14791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14807,7 +14807,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1804320"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14844,7 +14844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4847040"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14865,9 +14865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14881,7 +14881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7705080"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14902,9 +14902,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14918,7 +14918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1994760"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14939,9 +14939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14955,7 +14955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5042880"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14976,9 +14976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14992,7 +14992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8090280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15013,9 +15013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15029,7 +15029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1994760"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15050,9 +15050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15066,7 +15066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5228640"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15087,9 +15087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477080</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15103,7 +15103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8276040"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15124,9 +15124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15140,7 +15140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2184840"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15161,9 +15161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15177,7 +15177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="5042880"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15198,9 +15198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15214,7 +15214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8276040"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15235,9 +15235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15251,7 +15251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="2180160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15272,9 +15272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15288,7 +15288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5228640"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,9 +15309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477080</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15325,7 +15325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8085600"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15346,9 +15346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15362,7 +15362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2370600"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15383,9 +15383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15399,7 +15399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5423760"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15420,9 +15420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15436,7 +15436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="8467200"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15457,9 +15457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15473,7 +15473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="2375280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15494,9 +15494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477080</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15510,7 +15510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8662320"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15531,9 +15531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15547,7 +15547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5613840"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15568,9 +15568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481760</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15584,7 +15584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2565720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15605,9 +15605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>237960</xdr:colOff>
+      <xdr:colOff>237600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15621,7 +15621,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5418360"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15642,9 +15642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15658,7 +15658,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455800" y="8656920"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15679,9 +15679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>237960</xdr:colOff>
+      <xdr:colOff>237600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15695,7 +15695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2564640"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480680</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15732,7 +15732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926160" y="5612760"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15753,9 +15753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1476360</xdr:colOff>
+      <xdr:colOff>1476000</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15769,7 +15769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8466480"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15806,7 +15806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2757960"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15827,9 +15827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15843,7 +15843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5800680"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15864,9 +15864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15880,7 +15880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="8849160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15901,9 +15901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>195120</xdr:colOff>
+      <xdr:colOff>194760</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15917,7 +15917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481720" y="2753280"/>
-          <a:ext cx="146880" cy="146880"/>
+          <a:ext cx="146520" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15938,9 +15938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>190440</xdr:colOff>
+      <xdr:colOff>190080</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15954,7 +15954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5477040" y="5991120"/>
-          <a:ext cx="146880" cy="146880"/>
+          <a:ext cx="146520" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15975,9 +15975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1438200</xdr:colOff>
+      <xdr:colOff>1437840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15991,7 +15991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956760" y="9039240"/>
-          <a:ext cx="146880" cy="146880"/>
+          <a:ext cx="146520" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16012,9 +16012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16028,7 +16028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2943720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16049,9 +16049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16065,7 +16065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="5800680"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16086,9 +16086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16102,7 +16102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9039240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,9 +16123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16139,7 +16139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="2943720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16160,9 +16160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16176,7 +16176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5991120"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16197,9 +16197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16213,7 +16213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="8849160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16234,9 +16234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16250,7 +16250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3134160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16271,9 +16271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16287,7 +16287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6182280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16308,9 +16308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16324,7 +16324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9229680"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16345,9 +16345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16361,7 +16361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3138840"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16382,9 +16382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16398,7 +16398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6372720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16419,9 +16419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16435,7 +16435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9420120"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16456,9 +16456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16472,7 +16472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3324240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16493,9 +16493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16509,7 +16509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6182280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16530,9 +16530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16546,7 +16546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9420120"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16567,9 +16567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16583,7 +16583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3324240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16604,9 +16604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16620,7 +16620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6372720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16641,9 +16641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16657,7 +16657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9229680"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16678,9 +16678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1460880</xdr:colOff>
+      <xdr:colOff>1460520</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16694,7 +16694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="3514680"/>
-          <a:ext cx="174240" cy="146880"/>
+          <a:ext cx="173880" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16715,9 +16715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1460880</xdr:colOff>
+      <xdr:colOff>1460520</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16731,7 +16731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="6563160"/>
-          <a:ext cx="174240" cy="146880"/>
+          <a:ext cx="173880" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16752,9 +16752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>213120</xdr:colOff>
+      <xdr:colOff>212760</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16768,7 +16768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5472360" y="9611280"/>
-          <a:ext cx="174240" cy="146880"/>
+          <a:ext cx="173880" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16789,9 +16789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16805,7 +16805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3514680"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16826,9 +16826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16842,7 +16842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6753240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16863,9 +16863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16879,7 +16879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9801720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16900,9 +16900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16916,7 +16916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3705120"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16937,9 +16937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16953,7 +16953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6563160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16974,9 +16974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16990,7 +16990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9801720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17011,9 +17011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17027,7 +17027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3896280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17048,9 +17048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17064,7 +17064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6943680"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17085,9 +17085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17101,7 +17101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9992160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17122,9 +17122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17138,7 +17138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3900960"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17159,9 +17159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17175,7 +17175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="7134120"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17196,9 +17196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17212,7 +17212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="10182240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17233,9 +17233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17249,7 +17249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="4091400"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17270,9 +17270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17286,7 +17286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6948360"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17307,9 +17307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17323,7 +17323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="10182240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17344,9 +17344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17360,7 +17360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="4086720"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17381,9 +17381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17397,7 +17397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="7134120"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17418,9 +17418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17434,7 +17434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9992160"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17455,9 +17455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17471,7 +17471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3709800"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17492,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482840</xdr:colOff>
+      <xdr:colOff>1482480</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17508,7 +17508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6753240"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17529,9 +17529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1478160</xdr:colOff>
+      <xdr:colOff>1477800</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17545,7 +17545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9611280"/>
-          <a:ext cx="219960" cy="146880"/>
+          <a:ext cx="219600" cy="146520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31724,8 +31724,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ24" activeCellId="0" sqref="AZ24"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AY28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BG42" activeCellId="0" sqref="BG42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36937,7 +36937,9 @@
         <f aca="false">AO38</f>
         <v>Suecia</v>
       </c>
-      <c r="BA34" s="80"/>
+      <c r="BA34" s="80" t="n">
+        <v>1</v>
+      </c>
       <c r="BB34" s="81"/>
       <c r="BC34" s="70"/>
       <c r="BD34" s="70"/>
@@ -37132,7 +37134,9 @@
         <f aca="false">AO33</f>
         <v>Suiza</v>
       </c>
-      <c r="BA35" s="83"/>
+      <c r="BA35" s="83" t="n">
+        <v>0</v>
+      </c>
       <c r="BB35" s="84"/>
       <c r="BC35" s="85"/>
       <c r="BD35" s="70"/>
@@ -37318,7 +37322,7 @@
       </c>
       <c r="BF36" s="79" t="str">
         <f aca="false">T64</f>
-        <v>W55</v>
+        <v>Suecia</v>
       </c>
       <c r="BG36" s="80"/>
       <c r="BH36" s="81"/>
@@ -37420,7 +37424,7 @@
       <c r="BE37" s="78"/>
       <c r="BF37" s="82" t="str">
         <f aca="false">T65</f>
-        <v>W56</v>
+        <v>Inglaterra</v>
       </c>
       <c r="BG37" s="83"/>
       <c r="BH37" s="84"/>
@@ -37614,8 +37618,12 @@
         <f aca="false">AO50</f>
         <v>Colombia</v>
       </c>
-      <c r="BA38" s="80"/>
-      <c r="BB38" s="81"/>
+      <c r="BA38" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB38" s="81" t="n">
+        <v>3</v>
+      </c>
       <c r="BC38" s="94"/>
       <c r="BD38" s="70"/>
       <c r="BI38" s="70"/>
@@ -37806,8 +37814,12 @@
         <f aca="false">AO45</f>
         <v>Inglaterra</v>
       </c>
-      <c r="BA39" s="83"/>
-      <c r="BB39" s="84"/>
+      <c r="BA39" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB39" s="84" t="n">
+        <v>4</v>
+      </c>
       <c r="BC39" s="70"/>
       <c r="BD39" s="70"/>
       <c r="BK39" s="70"/>
@@ -40267,11 +40279,11 @@
       </c>
       <c r="S64" s="41" t="str">
         <f aca="false">IF(OR(BA34="",BA35=""),"",IF(BA34&gt;BA35,AZ34,IF(BA34&lt;BA35,AZ35,IF(OR(BB34="",BB35=""),"draw",IF(BB34&gt;BB35,AZ34,IF(BB34&lt;BB35,AZ35,"draw"))))))</f>
-        <v/>
+        <v>Suecia</v>
       </c>
       <c r="T64" s="41" t="str">
         <f aca="false">IF(OR(S64="",S64="draw"),INDEX(T,92,lang),S64)</f>
-        <v>W55</v>
+        <v>Suecia</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40281,11 +40293,11 @@
       </c>
       <c r="S65" s="41" t="str">
         <f aca="false">IF(OR(BA38="",BA39=""),"",IF(BA38&gt;BA39,AZ38,IF(BA38&lt;BA39,AZ39,IF(OR(BB38="",BB39=""),"draw",IF(BB38&gt;BB39,AZ38,IF(BB38&lt;BB39,AZ39,"draw"))))))</f>
-        <v/>
+        <v>Inglaterra</v>
       </c>
       <c r="T65" s="41" t="str">
         <f aca="false">IF(OR(S65="",S65="draw"),INDEX(T,93,lang),S65)</f>
-        <v>W56</v>
+        <v>Inglaterra</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Resultados actualizados al dis 10 de julio
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -14014,9 +14014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483200</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14030,7 +14030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1232280"/>
-          <a:ext cx="222480" cy="145080"/>
+          <a:ext cx="221400" cy="144000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14051,9 +14051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1484280</xdr:colOff>
+      <xdr:colOff>1483200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14067,7 +14067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4276080"/>
-          <a:ext cx="222480" cy="145080"/>
+          <a:ext cx="221400" cy="144000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14088,9 +14088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>244800</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14104,7 +14104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7324200"/>
-          <a:ext cx="222480" cy="145080"/>
+          <a:ext cx="221400" cy="144000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14125,9 +14125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14141,7 +14141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="1232280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14162,9 +14162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14178,7 +14178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4470840"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14199,9 +14199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14215,7 +14215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7519320"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14236,9 +14236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14252,7 +14252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1422720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14273,9 +14273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247680</xdr:colOff>
+      <xdr:colOff>246600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14289,7 +14289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5461560" y="4280760"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14310,9 +14310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14326,7 +14326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7519320"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14347,9 +14347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14363,7 +14363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1431720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14384,9 +14384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>181800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14400,7 +14400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4484520"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14421,9 +14421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>173520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14437,7 +14437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7333560"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14458,9 +14458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14474,7 +14474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1613880"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14495,9 +14495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14511,7 +14511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4661280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14532,9 +14532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14548,7 +14548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="7709760"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14569,9 +14569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14585,7 +14585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1613880"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14606,9 +14606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14622,7 +14622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4856400"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14643,9 +14643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1476720</xdr:colOff>
+      <xdr:colOff>1475640</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14659,7 +14659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="7899840"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14680,9 +14680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14696,7 +14696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="7904520"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14717,9 +14717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14733,7 +14733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="4661280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14754,9 +14754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14770,7 +14770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1799640"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,9 +14791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14807,7 +14807,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1804320"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14844,7 +14844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="4847040"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14865,9 +14865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14881,7 +14881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="7705080"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14902,9 +14902,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14918,7 +14918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="1994760"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14939,9 +14939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14955,7 +14955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5042880"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14976,9 +14976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14992,7 +14992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8090280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15013,9 +15013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15029,7 +15029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="1994760"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15050,9 +15050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15066,7 +15066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5228640"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15087,9 +15087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1476720</xdr:colOff>
+      <xdr:colOff>1475640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15103,7 +15103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8276040"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15124,9 +15124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15140,7 +15140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2184840"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15161,9 +15161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15177,7 +15177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="5042880"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15198,9 +15198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15214,7 +15214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="8276040"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15235,9 +15235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15251,7 +15251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="2180160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15272,9 +15272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15288,7 +15288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5228640"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,9 +15309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1476720</xdr:colOff>
+      <xdr:colOff>1475640</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15325,7 +15325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8085600"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15346,9 +15346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15362,7 +15362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2370600"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15383,9 +15383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15399,7 +15399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="5423760"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15420,9 +15420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15436,7 +15436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="8467200"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15457,9 +15457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15473,7 +15473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5456880" y="2375280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15494,9 +15494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1476720</xdr:colOff>
+      <xdr:colOff>1475640</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15510,7 +15510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3922560" y="8662320"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15531,9 +15531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15547,7 +15547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5452200" y="5613840"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15568,9 +15568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1481400</xdr:colOff>
+      <xdr:colOff>1480320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15584,7 +15584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3927240" y="2565720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15605,9 +15605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>237600</xdr:colOff>
+      <xdr:colOff>236520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15621,7 +15621,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="5418360"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15642,9 +15642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241920</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15658,7 +15658,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5455800" y="8656920"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15679,9 +15679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>237600</xdr:colOff>
+      <xdr:colOff>236520</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15695,7 +15695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5451480" y="2564640"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1480320</xdr:colOff>
+      <xdr:colOff>1479240</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15732,7 +15732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3926160" y="5612760"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15753,9 +15753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1476000</xdr:colOff>
+      <xdr:colOff>1474920</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15769,7 +15769,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3921840" y="8466480"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15806,7 +15806,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2757960"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15827,9 +15827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15843,7 +15843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5800680"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15864,9 +15864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15880,7 +15880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="8849160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15901,9 +15901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>194760</xdr:colOff>
+      <xdr:colOff>193680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15917,7 +15917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5481720" y="2753280"/>
-          <a:ext cx="146520" cy="146520"/>
+          <a:ext cx="145440" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15938,9 +15938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>190080</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15954,7 +15954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5477040" y="5991120"/>
-          <a:ext cx="146520" cy="146520"/>
+          <a:ext cx="145440" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15975,9 +15975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1437840</xdr:colOff>
+      <xdr:colOff>1436760</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15991,7 +15991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3956760" y="9039240"/>
-          <a:ext cx="146520" cy="146520"/>
+          <a:ext cx="145440" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16012,9 +16012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16028,7 +16028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="2943720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16049,9 +16049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16065,7 +16065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="5800680"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16086,9 +16086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16102,7 +16102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9039240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,9 +16123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16139,7 +16139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="2943720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16160,9 +16160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16176,7 +16176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="5991120"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16197,9 +16197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16213,7 +16213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="8849160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16234,9 +16234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16250,7 +16250,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3134160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16271,9 +16271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16287,7 +16287,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6182280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16308,9 +16308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16324,7 +16324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9229680"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16345,9 +16345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16361,7 +16361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3138840"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16382,9 +16382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16398,7 +16398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6372720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16419,9 +16419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16435,7 +16435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9420120"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16456,9 +16456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16472,7 +16472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3324240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16493,9 +16493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16509,7 +16509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6182280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16530,9 +16530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16546,7 +16546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9420120"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16567,9 +16567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16583,7 +16583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3324240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16604,9 +16604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16620,7 +16620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="6372720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16641,9 +16641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16657,7 +16657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9229680"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16678,9 +16678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1460520</xdr:colOff>
+      <xdr:colOff>1459440</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16694,7 +16694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="3514680"/>
-          <a:ext cx="173880" cy="146520"/>
+          <a:ext cx="172800" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16715,9 +16715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1460520</xdr:colOff>
+      <xdr:colOff>1459440</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16731,7 +16731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952080" y="6563160"/>
-          <a:ext cx="173880" cy="146520"/>
+          <a:ext cx="172800" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16752,9 +16752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>212760</xdr:colOff>
+      <xdr:colOff>211680</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16768,7 +16768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5472360" y="9611280"/>
-          <a:ext cx="173880" cy="146520"/>
+          <a:ext cx="172800" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16789,9 +16789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16805,7 +16805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="3514680"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16826,9 +16826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16842,7 +16842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6753240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16863,9 +16863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16879,7 +16879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9801720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16900,9 +16900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16916,7 +16916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3705120"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16937,9 +16937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16953,7 +16953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="6563160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16974,9 +16974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16990,7 +16990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9801720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17011,9 +17011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17027,7 +17027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="3896280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17048,9 +17048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17064,7 +17064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6943680"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17085,9 +17085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17101,7 +17101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="9992160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17122,9 +17122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17138,7 +17138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3900960"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17159,9 +17159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17175,7 +17175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="7134120"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17196,9 +17196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17212,7 +17212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="10182240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17233,9 +17233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17249,7 +17249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="4091400"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17270,9 +17270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17286,7 +17286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="6948360"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17307,9 +17307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17323,7 +17323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="10182240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17344,9 +17344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17360,7 +17360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5453280" y="4086720"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17381,9 +17381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17397,7 +17397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="7134120"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17418,9 +17418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17434,7 +17434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="9992160"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17455,9 +17455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17471,7 +17471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5457960" y="3709800"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17492,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1482480</xdr:colOff>
+      <xdr:colOff>1481400</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17508,7 +17508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3928320" y="6753240"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17529,9 +17529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1477800</xdr:colOff>
+      <xdr:colOff>1476720</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17545,7 +17545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3923640" y="9611280"/>
-          <a:ext cx="219600" cy="146520"/>
+          <a:ext cx="218520" cy="145440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -31724,8 +31724,8 @@
   </sheetPr>
   <dimension ref="A1:BT96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AY28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BG42" activeCellId="0" sqref="BG42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AY4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM18" activeCellId="0" sqref="BM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33025,7 +33025,9 @@
         <f aca="false">T58</f>
         <v>Uruguay</v>
       </c>
-      <c r="BG12" s="80"/>
+      <c r="BG12" s="80" t="n">
+        <v>0</v>
+      </c>
       <c r="BH12" s="81"/>
       <c r="BI12" s="70"/>
       <c r="BJ12" s="70"/>
@@ -33131,7 +33133,9 @@
         <f aca="false">T59</f>
         <v>Francia</v>
       </c>
-      <c r="BG13" s="83"/>
+      <c r="BG13" s="83" t="n">
+        <v>2</v>
+      </c>
       <c r="BH13" s="84"/>
       <c r="BI13" s="85"/>
       <c r="BJ13" s="70"/>
@@ -33730,9 +33734,11 @@
       </c>
       <c r="BL16" s="79" t="str">
         <f aca="false">T69</f>
-        <v>W57</v>
-      </c>
-      <c r="BM16" s="80"/>
+        <v>Francia</v>
+      </c>
+      <c r="BM16" s="80" t="n">
+        <v>1</v>
+      </c>
       <c r="BN16" s="81"/>
       <c r="BO16" s="70"/>
       <c r="BP16" s="95"/>
@@ -33925,9 +33931,11 @@
       <c r="BK17" s="78"/>
       <c r="BL17" s="82" t="str">
         <f aca="false">T70</f>
-        <v>W58</v>
-      </c>
-      <c r="BM17" s="83"/>
+        <v>Bélgica</v>
+      </c>
+      <c r="BM17" s="83" t="n">
+        <v>0</v>
+      </c>
       <c r="BN17" s="84"/>
       <c r="BO17" s="85"/>
       <c r="BP17" s="96"/>
@@ -34403,7 +34411,9 @@
         <f aca="false">T62</f>
         <v>Brasil</v>
       </c>
-      <c r="BG20" s="80"/>
+      <c r="BG20" s="80" t="n">
+        <v>1</v>
+      </c>
       <c r="BH20" s="81"/>
       <c r="BI20" s="94"/>
       <c r="BJ20" s="70"/>
@@ -34602,7 +34612,9 @@
         <f aca="false">T63</f>
         <v>Bélgica</v>
       </c>
-      <c r="BG21" s="83"/>
+      <c r="BG21" s="83" t="n">
+        <v>2</v>
+      </c>
       <c r="BH21" s="84"/>
       <c r="BI21" s="70"/>
       <c r="BJ21" s="70"/>
@@ -35010,7 +35022,7 @@
       </c>
       <c r="BR23" s="79" t="str">
         <f aca="false">T76</f>
-        <v>W61</v>
+        <v>Francia</v>
       </c>
       <c r="BS23" s="80"/>
       <c r="BT23" s="81"/>
@@ -35873,8 +35885,12 @@
         <f aca="false">T60</f>
         <v>Rusia</v>
       </c>
-      <c r="BG28" s="80"/>
-      <c r="BH28" s="81"/>
+      <c r="BG28" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH28" s="81" t="n">
+        <v>3</v>
+      </c>
       <c r="BI28" s="70"/>
       <c r="BJ28" s="70"/>
       <c r="BK28" s="70"/>
@@ -36068,8 +36084,12 @@
         <f aca="false">T61</f>
         <v>Croacia</v>
       </c>
-      <c r="BG29" s="83"/>
-      <c r="BH29" s="84"/>
+      <c r="BG29" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH29" s="84" t="n">
+        <v>4</v>
+      </c>
       <c r="BI29" s="85"/>
       <c r="BJ29" s="70"/>
       <c r="BK29" s="70"/>
@@ -36554,7 +36574,7 @@
       </c>
       <c r="BL32" s="79" t="str">
         <f aca="false">T71</f>
-        <v>W59</v>
+        <v>Croacia</v>
       </c>
       <c r="BM32" s="80"/>
       <c r="BN32" s="81"/>
@@ -36753,7 +36773,7 @@
       <c r="BK33" s="78"/>
       <c r="BL33" s="82" t="str">
         <f aca="false">T72</f>
-        <v>W60</v>
+        <v>Inglaterra</v>
       </c>
       <c r="BM33" s="83"/>
       <c r="BN33" s="84"/>
@@ -37160,7 +37180,7 @@
       </c>
       <c r="BR35" s="79" t="str">
         <f aca="false">Z76</f>
-        <v>L61</v>
+        <v>Bélgica</v>
       </c>
       <c r="BS35" s="80"/>
       <c r="BT35" s="81"/>
@@ -37324,7 +37344,9 @@
         <f aca="false">T64</f>
         <v>Suecia</v>
       </c>
-      <c r="BG36" s="80"/>
+      <c r="BG36" s="80" t="n">
+        <v>0</v>
+      </c>
       <c r="BH36" s="81"/>
       <c r="BI36" s="94"/>
       <c r="BJ36" s="70"/>
@@ -37426,7 +37448,9 @@
         <f aca="false">T65</f>
         <v>Inglaterra</v>
       </c>
-      <c r="BG37" s="83"/>
+      <c r="BG37" s="83" t="n">
+        <v>2</v>
+      </c>
       <c r="BH37" s="84"/>
       <c r="BI37" s="70"/>
       <c r="BJ37" s="70"/>
@@ -40310,11 +40334,11 @@
       </c>
       <c r="S69" s="41" t="str">
         <f aca="false">IF(OR(BG12="",BG13=""),"",IF(BG12&gt;BG13,BF12,IF(BG12&lt;BG13,BF13,IF(OR(BH12="",BH13=""),"draw",IF(BH12&gt;BH13,BF12,IF(BH12&lt;BH13,BF13,"draw"))))))</f>
-        <v/>
+        <v>Francia</v>
       </c>
       <c r="T69" s="41" t="str">
         <f aca="false">IF(OR(S69="",S69="draw"),INDEX(T,94,lang),S69)</f>
-        <v>W57</v>
+        <v>Francia</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40324,11 +40348,11 @@
       </c>
       <c r="S70" s="41" t="str">
         <f aca="false">IF(OR(BG20="",BG21=""),"",IF(BG20&gt;BG21,BF20,IF(BG20&lt;BG21,BF21,IF(OR(BH20="",BH21=""),"draw",IF(BH20&gt;BH21,BF20,IF(BH20&lt;BH21,BF21,"draw"))))))</f>
-        <v/>
+        <v>Bélgica</v>
       </c>
       <c r="T70" s="41" t="str">
         <f aca="false">IF(OR(S70="",S70="draw"),INDEX(T,95,lang),S70)</f>
-        <v>W58</v>
+        <v>Bélgica</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40338,11 +40362,11 @@
       </c>
       <c r="S71" s="41" t="str">
         <f aca="false">IF(OR(BG28="",BG29=""),"",IF(BG28&gt;BG29,BF28,IF(BG28&lt;BG29,BF29,IF(OR(BH28="",BH29=""),"draw",IF(BH28&gt;BH29,BF28,IF(BH28&lt;BH29,BF29,"draw"))))))</f>
-        <v/>
+        <v>Croacia</v>
       </c>
       <c r="T71" s="41" t="str">
         <f aca="false">IF(OR(S71="",S71="draw"),INDEX(T,96,lang),S71)</f>
-        <v>W59</v>
+        <v>Croacia</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40352,11 +40376,11 @@
       </c>
       <c r="S72" s="41" t="str">
         <f aca="false">IF(OR(BG36="",BG37=""),"",IF(BG36&gt;BG37,BF36,IF(BG36&lt;BG37,BF37,IF(OR(BH36="",BH37=""),"draw",IF(BH36&gt;BH37,BF36,IF(BH36&lt;BH37,BF37,"draw"))))))</f>
-        <v/>
+        <v>Inglaterra</v>
       </c>
       <c r="T72" s="41" t="str">
         <f aca="false">IF(OR(S72="",S72="draw"),INDEX(T,97,lang),S72)</f>
-        <v>W60</v>
+        <v>Inglaterra</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -40369,19 +40393,19 @@
       </c>
       <c r="S76" s="41" t="str">
         <f aca="false">IF(OR(BM16="",BM17=""),"",IF(BM16&gt;BM17,BL16,IF(BM16&lt;BM17,BL17,IF(OR(BN16="",BN17=""),"draw",IF(BN16&gt;BN17,BL16,IF(BN16&lt;BN17,BL17,"draw"))))))</f>
-        <v/>
+        <v>Francia</v>
       </c>
       <c r="T76" s="41" t="str">
         <f aca="false">IF(OR(S76="",S76="draw"),INDEX(T,98,lang),S76)</f>
-        <v>W61</v>
+        <v>Francia</v>
       </c>
       <c r="U76" s="41" t="str">
         <f aca="false">IF(OR(BM16="",BM17=""),"",IF(BM16&lt;BM17,BL16,IF(BM16&gt;BM17,BL17,IF(OR(BN16="",BN17=""),"draw",IF(BN16&lt;BN17,BL16,IF(BN16&gt;BN17,BL17,"draw"))))))</f>
-        <v/>
+        <v>Bélgica</v>
       </c>
       <c r="Z76" s="41" t="str">
         <f aca="false">IF(OR(U76="",U76="draw"),INDEX(T,100,lang),U76)</f>
-        <v>L61</v>
+        <v>Bélgica</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Resultados actualizados hasta el dia 15 de julio, con campeon del mundo decidido
</commit_message>
<xml_diff>
--- a/world_cup_2018.xlsx
+++ b/world_cup_2018.xlsx
@@ -13176,7 +13176,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483199</xdr:colOff>
+      <xdr:colOff>1483197</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>166679</xdr:rowOff>
     </xdr:to>
@@ -13209,11 +13209,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1261799</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1483199</xdr:colOff>
+      <xdr:colOff>1483197</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>162719</xdr:rowOff>
     </xdr:to>
@@ -13246,7 +13246,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>23399</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
@@ -13287,7 +13287,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>168119</xdr:rowOff>
     </xdr:to>
@@ -13324,7 +13324,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>168119</xdr:rowOff>
     </xdr:to>
@@ -13472,7 +13472,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>168839</xdr:rowOff>
     </xdr:to>
@@ -13503,7 +13503,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>31679</xdr:rowOff>
     </xdr:from>
@@ -13694,7 +13694,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>168839</xdr:rowOff>
     </xdr:to>
@@ -13725,7 +13725,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>23399</xdr:rowOff>
     </xdr:from>
@@ -13768,7 +13768,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>172799</xdr:rowOff>
     </xdr:to>
@@ -13799,7 +13799,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1257119</xdr:colOff>
+      <xdr:colOff>1257118</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>22679</xdr:rowOff>
     </xdr:from>
@@ -13836,7 +13836,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>27359</xdr:rowOff>
     </xdr:from>
@@ -13879,7 +13879,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>168119</xdr:rowOff>
     </xdr:to>
@@ -13912,7 +13912,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1261799</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -13947,7 +13947,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>23399</xdr:rowOff>
     </xdr:from>
@@ -14023,7 +14023,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1261799</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -14132,7 +14132,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>22679</xdr:rowOff>
     </xdr:from>
@@ -14169,7 +14169,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>23399</xdr:rowOff>
     </xdr:from>
@@ -14206,9 +14206,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
@@ -14243,7 +14243,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1257119</xdr:colOff>
+      <xdr:colOff>1257118</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>17999</xdr:rowOff>
     </xdr:from>
@@ -14323,7 +14323,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>168839</xdr:rowOff>
     </xdr:to>
@@ -14354,7 +14354,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>17999</xdr:rowOff>
     </xdr:from>
@@ -14391,7 +14391,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>17999</xdr:rowOff>
     </xdr:from>
@@ -14430,7 +14430,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1261799</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -14465,7 +14465,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1257119</xdr:colOff>
+      <xdr:colOff>1257118</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>17999</xdr:rowOff>
     </xdr:from>
@@ -14578,11 +14578,11 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>23399</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>18719</xdr:rowOff>
+      <xdr:rowOff>18717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>164159</xdr:rowOff>
     </xdr:to>
@@ -14619,7 +14619,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>241919</xdr:colOff>
+      <xdr:colOff>241915</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>168119</xdr:rowOff>
     </xdr:to>
@@ -14650,7 +14650,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1257119</xdr:colOff>
+      <xdr:colOff>1257118</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>23399</xdr:rowOff>
     </xdr:from>
@@ -14687,7 +14687,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>18719</xdr:colOff>
+      <xdr:colOff>18717</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>22679</xdr:rowOff>
     </xdr:from>
@@ -14798,7 +14798,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>22319</xdr:colOff>
+      <xdr:colOff>22318</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>17999</xdr:rowOff>
     </xdr:from>
@@ -14856,7 +14856,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5104349" y="2545724"/>
+          <a:off x="5104349" y="2545723"/>
           <a:ext cx="218519" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15115,7 +15115,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5129909" y="5972204"/>
+          <a:off x="5129909" y="5972203"/>
           <a:ext cx="145439" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15137,7 +15137,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1436759</xdr:colOff>
+      <xdr:colOff>1436758</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>164519</xdr:rowOff>
     </xdr:to>
@@ -15337,7 +15337,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3263129" y="5972204"/>
+          <a:off x="3263129" y="5972203"/>
           <a:ext cx="218520" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15448,7 +15448,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3258449" y="6163424"/>
+          <a:off x="3258449" y="6163423"/>
           <a:ext cx="218520" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15670,7 +15670,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5106149" y="6163424"/>
+          <a:off x="5106149" y="6163423"/>
           <a:ext cx="218520" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15834,7 +15834,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1286639</xdr:colOff>
+      <xdr:colOff>1286638</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>19079</xdr:rowOff>
     </xdr:from>
@@ -15871,7 +15871,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1286639</xdr:colOff>
+      <xdr:colOff>1286638</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>19799</xdr:rowOff>
     </xdr:from>
@@ -16336,7 +16336,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5110829" y="7115204"/>
+          <a:off x="5110829" y="7115203"/>
           <a:ext cx="218520" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16558,7 +16558,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3263129" y="7115204"/>
+          <a:off x="3263129" y="7115203"/>
           <a:ext cx="218520" cy="145439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -17063,8 +17063,12 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill/>
-        <a:solidFill/>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525">
@@ -17119,7 +17123,9 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill/>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
         <a:solidFill/>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -31366,20 +31372,6 @@
       <c r="AT2" s="41"/>
     </row>
     <row ht="12.75" customHeight="1" r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
       <c r="O3" s="44" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v xml:space="preserve">Language: Spanish</v>
@@ -34546,7 +34538,9 @@
         <f>T76</f>
         <v>Francia</v>
       </c>
-      <c r="BS23" s="77"/>
+      <c r="BS23" s="77">
+        <v>4</v>
+      </c>
       <c r="BT23" s="78"/>
     </row>
     <row ht="15" customHeight="1" r="24">
@@ -34717,7 +34711,9 @@
         <f>T77</f>
         <v>Croacia</v>
       </c>
-      <c r="BS24" s="80"/>
+      <c r="BS24" s="80">
+        <v>2</v>
+      </c>
       <c r="BT24" s="81"/>
     </row>
     <row ht="15" customHeight="1" r="25">
@@ -37730,7 +37726,7 @@
       <c r="BN41" s="94"/>
       <c r="BO41" s="95" t="str">
         <f>S85</f>
-        <v/>
+        <v>Francia</v>
       </c>
       <c r="BP41" s="95"/>
       <c r="BQ41" s="95"/>
@@ -39981,11 +39977,11 @@
       </c>
       <c r="S85" s="40" t="str">
         <f>IF(OR(BS23="",BS24=""),"",IF(BS23&gt;BS24,BR23,IF(BS23&lt;BS24,BR24,IF(OR(BT23="",BT24=""),"",IF(BT23&gt;BT24,BR23,IF(BT23&lt;BT24,BR24,""))))))</f>
-        <v/>
+        <v>Francia</v>
       </c>
       <c r="T85" s="40" t="str">
         <f>S85</f>
-        <v/>
+        <v>Francia</v>
       </c>
     </row>
     <row ht="12.75" customHeight="1" r="87"/>

</xml_diff>